<commit_message>
version 3.4 Update Post And Customer
</commit_message>
<xml_diff>
--- a/rau.xlsx
+++ b/rau.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yui\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\FoodRau\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6765" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6765" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="LoaiSP" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Slider" sheetId="4" r:id="rId4"/>
     <sheet name="Post" sheetId="5" r:id="rId5"/>
     <sheet name="Relative_food" sheetId="6" r:id="rId6"/>
+    <sheet name="Customer" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="176">
   <si>
     <t>type_id</t>
   </si>
@@ -443,6 +444,120 @@
   </si>
   <si>
     <t>ID</t>
+  </si>
+  <si>
+    <t>SELECT [username] ,[password] ,[name] ,[phone] ,[email] ,[address] ,[num_order] ,[num_successful_order] ,[sum] ,[status] ,[created] FROM [dbo].[customer]</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>num_order</t>
+  </si>
+  <si>
+    <t>num_successful_order</t>
+  </si>
+  <si>
+    <t>sum</t>
+  </si>
+  <si>
+    <t>0356241963</t>
+  </si>
+  <si>
+    <t>0356241964</t>
+  </si>
+  <si>
+    <t>0356241965</t>
+  </si>
+  <si>
+    <t>0356241966</t>
+  </si>
+  <si>
+    <t>0356241967</t>
+  </si>
+  <si>
+    <t>0356241968</t>
+  </si>
+  <si>
+    <t>0356241969</t>
+  </si>
+  <si>
+    <t>0356241970</t>
+  </si>
+  <si>
+    <t>0356241971</t>
+  </si>
+  <si>
+    <t>0356241972</t>
+  </si>
+  <si>
+    <t>0356241973</t>
+  </si>
+  <si>
+    <t>0356241974</t>
+  </si>
+  <si>
+    <t>0356241975</t>
+  </si>
+  <si>
+    <t>0356241976</t>
+  </si>
+  <si>
+    <t>0356241977</t>
+  </si>
+  <si>
+    <t>0356241978</t>
+  </si>
+  <si>
+    <t>a123</t>
+  </si>
+  <si>
+    <t>a124</t>
+  </si>
+  <si>
+    <t>a125</t>
+  </si>
+  <si>
+    <t>a126</t>
+  </si>
+  <si>
+    <t>a127</t>
+  </si>
+  <si>
+    <t>a128</t>
+  </si>
+  <si>
+    <t>a129</t>
+  </si>
+  <si>
+    <t>a130</t>
+  </si>
+  <si>
+    <t>a131</t>
+  </si>
+  <si>
+    <t>a132</t>
+  </si>
+  <si>
+    <t>a133</t>
+  </si>
+  <si>
+    <t>a134</t>
+  </si>
+  <si>
+    <t>a135</t>
+  </si>
+  <si>
+    <t>a136</t>
+  </si>
+  <si>
+    <t>a137</t>
+  </si>
+  <si>
+    <t>a138</t>
   </si>
 </sst>
 </file>
@@ -493,7 +608,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -501,6 +616,12 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -840,7 +961,7 @@
       </c>
       <c r="F2" s="3" t="str">
         <f ca="1">TEXT(NOW(),"MM/dd/yyyy")</f>
-        <v>12/18/2019</v>
+        <v>12/26/2019</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -863,7 +984,7 @@
       </c>
       <c r="F3" s="3" t="str">
         <f t="shared" ref="F3:F5" ca="1" si="0">TEXT(NOW(),"MM/dd/yyyy")</f>
-        <v>12/18/2019</v>
+        <v>12/26/2019</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -886,7 +1007,7 @@
       </c>
       <c r="F4" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>12/18/2019</v>
+        <v>12/26/2019</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -909,7 +1030,7 @@
       </c>
       <c r="F5" s="3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>12/18/2019</v>
+        <v>12/26/2019</v>
       </c>
     </row>
     <row r="25" spans="2:2" x14ac:dyDescent="0.25">
@@ -928,7 +1049,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
@@ -1101,7 +1222,7 @@
         <v>1</v>
       </c>
       <c r="J7" t="str">
-        <f t="shared" ref="J6:J16" si="4">"INSERT INTO [dbo].[member] ([username] ,[pass] ,[name] ,[email] ,[phone] ,[role] ,[status]) VALUES ('"&amp;B7&amp;"' ,'"&amp;C7&amp;"' ,'"&amp;D7&amp;"' ,'"&amp;E7&amp;"' ,'"&amp;F7&amp;"' ,"&amp;G7&amp;","&amp;H7&amp;")"</f>
+        <f t="shared" ref="J7:J16" si="4">"INSERT INTO [dbo].[member] ([username] ,[pass] ,[name] ,[email] ,[phone] ,[role] ,[status]) VALUES ('"&amp;B7&amp;"' ,'"&amp;C7&amp;"' ,'"&amp;D7&amp;"' ,'"&amp;E7&amp;"' ,'"&amp;F7&amp;"' ,"&amp;G7&amp;","&amp;H7&amp;")"</f>
         <v>INSERT INTO [dbo].[member] ([username] ,[pass] ,[name] ,[email] ,[phone] ,[role] ,[status]) VALUES ('khuong4' ,'125' ,'JYui' ,'Jyui@gmail.com' ,'0356241964' ,1,1)</v>
       </c>
     </row>
@@ -1494,19 +1615,19 @@
 IF(RANDBETWEEN(1,4)=2,"Stawberry",
 IF(RANDBETWEEN(1,4)=3,"Green Beans","Tomatoe"
 )))</f>
-        <v>Tomatoe</v>
+        <v>Stawberry</v>
       </c>
       <c r="C2" t="str">
         <f t="shared" ref="C2:C18" ca="1" si="1">"Description "&amp;B2</f>
-        <v>Description Tomatoe</v>
+        <v>Description Stawberry</v>
       </c>
       <c r="D2" t="str">
         <f ca="1">TEXT(RANDBETWEEN(1,1000),"0")</f>
-        <v>922</v>
+        <v>957</v>
       </c>
       <c r="E2" s="2" t="str">
         <f ca="1">TEXT(D2-D2*RAND()*0.1,"0")</f>
-        <v>875</v>
+        <v>953</v>
       </c>
       <c r="F2" t="str">
         <f t="shared" ref="F2:F18" si="2">"product-"&amp;A2&amp;".jpg"</f>
@@ -1521,23 +1642,23 @@
       </c>
       <c r="I2" s="2" t="str">
         <f ca="1">TEXT(RAND()+0.1-0.2,"0.0")</f>
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
       <c r="J2">
         <f t="shared" ref="J2:K18" ca="1" si="4">RANDBETWEEN(1,10)</f>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="K2">
         <f t="shared" ca="1" si="4"/>
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="L2" s="2">
         <f ca="1">ABS(TEXT(RAND()+0.1-0.2,"0.0"))</f>
-        <v>0.2</v>
+        <v>0.7</v>
       </c>
       <c r="M2">
         <f t="shared" ref="M2:M18" ca="1" si="5">RANDBETWEEN(1,4)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N2">
         <v>1</v>
@@ -1548,11 +1669,11 @@
       </c>
       <c r="P2" s="4" t="str">
         <f ca="1">TEXT(NOW(),"MM/dd/yyyy")</f>
-        <v>12/18/2019</v>
+        <v>12/26/2019</v>
       </c>
       <c r="R2" t="str">
         <f ca="1">"INSERT INTO [dbo].[food] ([name] ,[description] ,[price] ,[price_promo] ,[thumb] ,[img] ,[unit] ,[percent_promo] ,[rating] ,[sold] ,[point] ,[type] ,[status] ,[username] ,[modified]) VALUES ('"&amp;B2&amp;"' ,'"&amp;C2&amp;"' ,"&amp;D2&amp;" ,"&amp;E2&amp;",' "&amp;F2&amp;"','"&amp;G2&amp;"' ,'"&amp;H2&amp;"' ,"&amp;I2&amp;" ,"&amp;J2&amp;","&amp;K2&amp;","&amp;L2&amp;" ,"&amp;M2&amp;","&amp;N2&amp;",'"&amp;O2&amp;"','"&amp;P2&amp;"')"</f>
-        <v>INSERT INTO [dbo].[food] ([name] ,[description] ,[price] ,[price_promo] ,[thumb] ,[img] ,[unit] ,[percent_promo] ,[rating] ,[sold] ,[point] ,[type] ,[status] ,[username] ,[modified]) VALUES ('Tomatoe' ,'Description Tomatoe' ,922 ,875,' product-1.jpg','product-1.jpg' ,'gam' ,0.6 ,1,7,0.2 ,2,1,'khuong','12/18/2019')</v>
+        <v>INSERT INTO [dbo].[food] ([name] ,[description] ,[price] ,[price_promo] ,[thumb] ,[img] ,[unit] ,[percent_promo] ,[rating] ,[sold] ,[point] ,[type] ,[status] ,[username] ,[modified]) VALUES ('Stawberry' ,'Description Stawberry' ,957 ,953,' product-1.jpg','product-1.jpg' ,'gam' ,0.5 ,8,10,0.7 ,1,1,'khuong','12/26/2019')</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
@@ -1561,19 +1682,19 @@
       </c>
       <c r="B3" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Stawberry</v>
+        <v>Tomatoe</v>
       </c>
       <c r="C3" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Description Stawberry</v>
+        <v>Description Tomatoe</v>
       </c>
       <c r="D3" t="str">
         <f t="shared" ref="D3:D18" ca="1" si="7">TEXT(RANDBETWEEN(1,1000),"0")</f>
-        <v>511</v>
+        <v>376</v>
       </c>
       <c r="E3" s="2" t="str">
         <f t="shared" ref="E3:E18" ca="1" si="8">TEXT(D3-D3*RAND()*0.1,"0")</f>
-        <v>483</v>
+        <v>348</v>
       </c>
       <c r="F3" t="str">
         <f t="shared" si="2"/>
@@ -1588,23 +1709,23 @@
       </c>
       <c r="I3" s="2" t="str">
         <f t="shared" ref="I3:I18" ca="1" si="9">TEXT(RAND()+0.1-0.2,"0.0")</f>
-        <v>-0.1</v>
+        <v>0.7</v>
       </c>
       <c r="J3">
         <f t="shared" ca="1" si="4"/>
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="K3">
         <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L3" s="2">
         <f t="shared" ref="L3:L18" ca="1" si="10">ABS(TEXT(RAND()+0.1-0.2,"0.0"))</f>
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="M3">
         <f t="shared" ca="1" si="5"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="N3">
         <v>1</v>
@@ -1615,11 +1736,11 @@
       </c>
       <c r="P3" s="4" t="str">
         <f t="shared" ref="P3:P18" ca="1" si="11">TEXT(NOW(),"MM/dd/yyyy")</f>
-        <v>12/18/2019</v>
+        <v>12/26/2019</v>
       </c>
       <c r="R3" t="str">
         <f t="shared" ref="R3:R18" ca="1" si="12">"INSERT INTO [dbo].[food] ([name] ,[description] ,[price] ,[price_promo] ,[thumb] ,[img] ,[unit] ,[percent_promo] ,[rating] ,[sold] ,[point] ,[type] ,[status] ,[username] ,[modified]) VALUES ('"&amp;B3&amp;"' ,'"&amp;C3&amp;"' ,"&amp;D3&amp;" ,"&amp;E3&amp;",' "&amp;F3&amp;"','"&amp;G3&amp;"' ,'"&amp;H3&amp;"' ,"&amp;I3&amp;" ,"&amp;J3&amp;","&amp;K3&amp;","&amp;L3&amp;" ,"&amp;M3&amp;","&amp;N3&amp;",'"&amp;O3&amp;"','"&amp;P3&amp;"')"</f>
-        <v>INSERT INTO [dbo].[food] ([name] ,[description] ,[price] ,[price_promo] ,[thumb] ,[img] ,[unit] ,[percent_promo] ,[rating] ,[sold] ,[point] ,[type] ,[status] ,[username] ,[modified]) VALUES ('Stawberry' ,'Description Stawberry' ,511 ,483,' product-2.jpg','product-2.jpg' ,'gam' ,-0.1 ,3,2,0.2 ,4,1,'khuong','12/18/2019')</v>
+        <v>INSERT INTO [dbo].[food] ([name] ,[description] ,[price] ,[price_promo] ,[thumb] ,[img] ,[unit] ,[percent_promo] ,[rating] ,[sold] ,[point] ,[type] ,[status] ,[username] ,[modified]) VALUES ('Tomatoe' ,'Description Tomatoe' ,376 ,348,' product-2.jpg','product-2.jpg' ,'gam' ,0.7 ,10,3,0.5 ,2,1,'khuong','12/26/2019')</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
@@ -1636,11 +1757,11 @@
       </c>
       <c r="D4" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>270</v>
+        <v>104</v>
       </c>
       <c r="E4" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>266</v>
+        <v>95</v>
       </c>
       <c r="F4" t="str">
         <f t="shared" si="2"/>
@@ -1655,19 +1776,19 @@
       </c>
       <c r="I4" s="2" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
       <c r="J4">
         <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K4">
         <f t="shared" ca="1" si="4"/>
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="L4" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="M4">
         <f t="shared" ca="1" si="5"/>
@@ -1682,11 +1803,11 @@
       </c>
       <c r="P4" s="4" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>12/18/2019</v>
+        <v>12/26/2019</v>
       </c>
       <c r="R4" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>INSERT INTO [dbo].[food] ([name] ,[description] ,[price] ,[price_promo] ,[thumb] ,[img] ,[unit] ,[percent_promo] ,[rating] ,[sold] ,[point] ,[type] ,[status] ,[username] ,[modified]) VALUES ('Tomatoe' ,'Description Tomatoe' ,270 ,266,' product-3.jpg','product-3.jpg' ,'gam' ,0.4 ,1,10,0.2 ,2,1,'khuong','12/18/2019')</v>
+        <v>INSERT INTO [dbo].[food] ([name] ,[description] ,[price] ,[price_promo] ,[thumb] ,[img] ,[unit] ,[percent_promo] ,[rating] ,[sold] ,[point] ,[type] ,[status] ,[username] ,[modified]) VALUES ('Tomatoe' ,'Description Tomatoe' ,104 ,95,' product-3.jpg','product-3.jpg' ,'gam' ,0.3 ,2,4,0.4 ,2,1,'khuong','12/26/2019')</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
@@ -1695,19 +1816,19 @@
       </c>
       <c r="B5" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Green Beans</v>
+        <v>Stawberry</v>
       </c>
       <c r="C5" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Description Green Beans</v>
+        <v>Description Stawberry</v>
       </c>
       <c r="D5" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>878</v>
+        <v>918</v>
       </c>
       <c r="E5" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>840</v>
+        <v>843</v>
       </c>
       <c r="F5" t="str">
         <f t="shared" si="2"/>
@@ -1726,15 +1847,15 @@
       </c>
       <c r="J5">
         <f t="shared" ca="1" si="4"/>
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="K5">
         <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L5" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>0.1</v>
+        <v>0.4</v>
       </c>
       <c r="M5">
         <f t="shared" ca="1" si="5"/>
@@ -1749,11 +1870,11 @@
       </c>
       <c r="P5" s="4" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>12/18/2019</v>
+        <v>12/26/2019</v>
       </c>
       <c r="R5" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>INSERT INTO [dbo].[food] ([name] ,[description] ,[price] ,[price_promo] ,[thumb] ,[img] ,[unit] ,[percent_promo] ,[rating] ,[sold] ,[point] ,[type] ,[status] ,[username] ,[modified]) VALUES ('Green Beans' ,'Description Green Beans' ,878 ,840,' product-4.jpg','product-4.jpg' ,'gam' ,0.6 ,4,2,0.1 ,2,1,'khuong','12/18/2019')</v>
+        <v>INSERT INTO [dbo].[food] ([name] ,[description] ,[price] ,[price_promo] ,[thumb] ,[img] ,[unit] ,[percent_promo] ,[rating] ,[sold] ,[point] ,[type] ,[status] ,[username] ,[modified]) VALUES ('Stawberry' ,'Description Stawberry' ,918 ,843,' product-4.jpg','product-4.jpg' ,'gam' ,0.6 ,9,3,0.4 ,2,1,'khuong','12/26/2019')</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
@@ -1762,19 +1883,19 @@
       </c>
       <c r="B6" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Stawberry</v>
+        <v>Bell Perpper</v>
       </c>
       <c r="C6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Description Stawberry</v>
+        <v>Description Bell Perpper</v>
       </c>
       <c r="D6" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="E6" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="F6" t="str">
         <f t="shared" si="2"/>
@@ -1789,23 +1910,23 @@
       </c>
       <c r="I6" s="2" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>0.9</v>
+        <v>0.2</v>
       </c>
       <c r="J6">
         <f t="shared" ca="1" si="4"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="K6">
         <f t="shared" ca="1" si="4"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="L6" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="M6">
         <f t="shared" ca="1" si="5"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N6">
         <v>1</v>
@@ -1816,11 +1937,11 @@
       </c>
       <c r="P6" s="4" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>12/18/2019</v>
+        <v>12/26/2019</v>
       </c>
       <c r="R6" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>INSERT INTO [dbo].[food] ([name] ,[description] ,[price] ,[price_promo] ,[thumb] ,[img] ,[unit] ,[percent_promo] ,[rating] ,[sold] ,[point] ,[type] ,[status] ,[username] ,[modified]) VALUES ('Stawberry' ,'Description Stawberry' ,114 ,106,' product-5.jpg','product-5.jpg' ,'gam' ,0.9 ,4,7,0.5 ,3,1,'khuong','12/18/2019')</v>
+        <v>INSERT INTO [dbo].[food] ([name] ,[description] ,[price] ,[price_promo] ,[thumb] ,[img] ,[unit] ,[percent_promo] ,[rating] ,[sold] ,[point] ,[type] ,[status] ,[username] ,[modified]) VALUES ('Bell Perpper' ,'Description Bell Perpper' ,106 ,101,' product-5.jpg','product-5.jpg' ,'gam' ,0.2 ,8,2,0.1 ,2,1,'khuong','12/26/2019')</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
@@ -1829,19 +1950,19 @@
       </c>
       <c r="B7" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Green Beans</v>
+        <v>Tomatoe</v>
       </c>
       <c r="C7" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Description Green Beans</v>
+        <v>Description Tomatoe</v>
       </c>
       <c r="D7" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>964</v>
+        <v>847</v>
       </c>
       <c r="E7" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>950</v>
+        <v>830</v>
       </c>
       <c r="F7" t="str">
         <f t="shared" si="2"/>
@@ -1856,7 +1977,7 @@
       </c>
       <c r="I7" s="2" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="J7">
         <f t="shared" ca="1" si="4"/>
@@ -1864,15 +1985,15 @@
       </c>
       <c r="K7">
         <f t="shared" ca="1" si="4"/>
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="L7" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>0.6</v>
+        <v>0.3</v>
       </c>
       <c r="M7">
         <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N7">
         <v>1</v>
@@ -1883,11 +2004,11 @@
       </c>
       <c r="P7" s="4" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>12/18/2019</v>
+        <v>12/26/2019</v>
       </c>
       <c r="R7" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>INSERT INTO [dbo].[food] ([name] ,[description] ,[price] ,[price_promo] ,[thumb] ,[img] ,[unit] ,[percent_promo] ,[rating] ,[sold] ,[point] ,[type] ,[status] ,[username] ,[modified]) VALUES ('Green Beans' ,'Description Green Beans' ,964 ,950,' product-6.jpg','product-6.jpg' ,'gam' ,0.6 ,6,7,0.6 ,2,1,'khuong','12/18/2019')</v>
+        <v>INSERT INTO [dbo].[food] ([name] ,[description] ,[price] ,[price_promo] ,[thumb] ,[img] ,[unit] ,[percent_promo] ,[rating] ,[sold] ,[point] ,[type] ,[status] ,[username] ,[modified]) VALUES ('Tomatoe' ,'Description Tomatoe' ,847 ,830,' product-6.jpg','product-6.jpg' ,'gam' ,0.4 ,6,10,0.3 ,4,1,'khuong','12/26/2019')</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
@@ -1896,19 +2017,19 @@
       </c>
       <c r="B8" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Green Beans</v>
+        <v>Bell Perpper</v>
       </c>
       <c r="C8" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Description Green Beans</v>
+        <v>Description Bell Perpper</v>
       </c>
       <c r="D8" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>204</v>
+        <v>899</v>
       </c>
       <c r="E8" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>200</v>
+        <v>816</v>
       </c>
       <c r="F8" t="str">
         <f t="shared" si="2"/>
@@ -1923,15 +2044,15 @@
       </c>
       <c r="I8" s="2" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>0.9</v>
+        <v>0.7</v>
       </c>
       <c r="J8">
         <f t="shared" ca="1" si="4"/>
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="K8">
         <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="L8" s="2">
         <f t="shared" ca="1" si="10"/>
@@ -1939,7 +2060,7 @@
       </c>
       <c r="M8">
         <f t="shared" ca="1" si="5"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N8">
         <v>1</v>
@@ -1950,11 +2071,11 @@
       </c>
       <c r="P8" s="4" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>12/18/2019</v>
+        <v>12/26/2019</v>
       </c>
       <c r="R8" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>INSERT INTO [dbo].[food] ([name] ,[description] ,[price] ,[price_promo] ,[thumb] ,[img] ,[unit] ,[percent_promo] ,[rating] ,[sold] ,[point] ,[type] ,[status] ,[username] ,[modified]) VALUES ('Green Beans' ,'Description Green Beans' ,204 ,200,' product-7.jpg','product-7.jpg' ,'gam' ,0.9 ,7,1,0.5 ,1,1,'khuong','12/18/2019')</v>
+        <v>INSERT INTO [dbo].[food] ([name] ,[description] ,[price] ,[price_promo] ,[thumb] ,[img] ,[unit] ,[percent_promo] ,[rating] ,[sold] ,[point] ,[type] ,[status] ,[username] ,[modified]) VALUES ('Bell Perpper' ,'Description Bell Perpper' ,899 ,816,' product-7.jpg','product-7.jpg' ,'gam' ,0.7 ,3,10,0.5 ,2,1,'khuong','12/26/2019')</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
@@ -1971,11 +2092,11 @@
       </c>
       <c r="D9" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>402</v>
+        <v>906</v>
       </c>
       <c r="E9" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>386</v>
+        <v>847</v>
       </c>
       <c r="F9" t="str">
         <f t="shared" si="2"/>
@@ -1990,23 +2111,23 @@
       </c>
       <c r="I9" s="2" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>0.8</v>
+        <v>0.2</v>
       </c>
       <c r="J9">
         <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="K9">
         <f t="shared" ca="1" si="4"/>
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="L9" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>0.1</v>
+        <v>0.8</v>
       </c>
       <c r="M9">
         <f t="shared" ca="1" si="5"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N9">
         <v>1</v>
@@ -2017,11 +2138,11 @@
       </c>
       <c r="P9" s="4" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>12/18/2019</v>
+        <v>12/26/2019</v>
       </c>
       <c r="R9" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>INSERT INTO [dbo].[food] ([name] ,[description] ,[price] ,[price_promo] ,[thumb] ,[img] ,[unit] ,[percent_promo] ,[rating] ,[sold] ,[point] ,[type] ,[status] ,[username] ,[modified]) VALUES ('Tomatoe' ,'Description Tomatoe' ,402 ,386,' product-8.jpg','product-8.jpg' ,'gam' ,0.8 ,1,7,0.1 ,1,1,'khuong','12/18/2019')</v>
+        <v>INSERT INTO [dbo].[food] ([name] ,[description] ,[price] ,[price_promo] ,[thumb] ,[img] ,[unit] ,[percent_promo] ,[rating] ,[sold] ,[point] ,[type] ,[status] ,[username] ,[modified]) VALUES ('Tomatoe' ,'Description Tomatoe' ,906 ,847,' product-8.jpg','product-8.jpg' ,'gam' ,0.2 ,10,3,0.8 ,3,1,'khuong','12/26/2019')</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
@@ -2030,19 +2151,19 @@
       </c>
       <c r="B10" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Tomatoe</v>
+        <v>Bell Perpper</v>
       </c>
       <c r="C10" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Description Tomatoe</v>
+        <v>Description Bell Perpper</v>
       </c>
       <c r="D10" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>196</v>
+        <v>85</v>
       </c>
       <c r="E10" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>180</v>
+        <v>81</v>
       </c>
       <c r="F10" t="str">
         <f t="shared" si="2"/>
@@ -2057,23 +2178,23 @@
       </c>
       <c r="I10" s="2" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="J10">
         <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="K10">
         <f t="shared" ca="1" si="4"/>
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="L10" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>0.8</v>
+        <v>0.3</v>
       </c>
       <c r="M10">
         <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N10">
         <v>1</v>
@@ -2084,11 +2205,11 @@
       </c>
       <c r="P10" s="4" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>12/18/2019</v>
+        <v>12/26/2019</v>
       </c>
       <c r="R10" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>INSERT INTO [dbo].[food] ([name] ,[description] ,[price] ,[price_promo] ,[thumb] ,[img] ,[unit] ,[percent_promo] ,[rating] ,[sold] ,[point] ,[type] ,[status] ,[username] ,[modified]) VALUES ('Tomatoe' ,'Description Tomatoe' ,196 ,180,' product-9.jpg','product-9.jpg' ,'gam' ,0.5 ,2,3,0.8 ,2,1,'khuong','12/18/2019')</v>
+        <v>INSERT INTO [dbo].[food] ([name] ,[description] ,[price] ,[price_promo] ,[thumb] ,[img] ,[unit] ,[percent_promo] ,[rating] ,[sold] ,[point] ,[type] ,[status] ,[username] ,[modified]) VALUES ('Bell Perpper' ,'Description Bell Perpper' ,85 ,81,' product-9.jpg','product-9.jpg' ,'gam' ,0.3 ,6,10,0.3 ,3,1,'khuong','12/26/2019')</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
@@ -2097,19 +2218,19 @@
       </c>
       <c r="B11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Bell Perpper</v>
+        <v>Stawberry</v>
       </c>
       <c r="C11" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Description Bell Perpper</v>
+        <v>Description Stawberry</v>
       </c>
       <c r="D11" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>702</v>
+        <v>768</v>
       </c>
       <c r="E11" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>679</v>
+        <v>751</v>
       </c>
       <c r="F11" t="str">
         <f t="shared" si="2"/>
@@ -2124,23 +2245,23 @@
       </c>
       <c r="I11" s="2" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>0.6</v>
+        <v>0.0</v>
       </c>
       <c r="J11">
         <f t="shared" ca="1" si="4"/>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="K11">
         <f t="shared" ca="1" si="4"/>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="L11" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
       <c r="M11">
         <f t="shared" ca="1" si="5"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="N11">
         <v>1</v>
@@ -2151,11 +2272,11 @@
       </c>
       <c r="P11" s="4" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>12/18/2019</v>
+        <v>12/26/2019</v>
       </c>
       <c r="R11" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>INSERT INTO [dbo].[food] ([name] ,[description] ,[price] ,[price_promo] ,[thumb] ,[img] ,[unit] ,[percent_promo] ,[rating] ,[sold] ,[point] ,[type] ,[status] ,[username] ,[modified]) VALUES ('Bell Perpper' ,'Description Bell Perpper' ,702 ,679,' product-10.jpg','product-10.jpg' ,'gam' ,0.6 ,8,10,0.3 ,4,1,'khuong','12/18/2019')</v>
+        <v>INSERT INTO [dbo].[food] ([name] ,[description] ,[price] ,[price_promo] ,[thumb] ,[img] ,[unit] ,[percent_promo] ,[rating] ,[sold] ,[point] ,[type] ,[status] ,[username] ,[modified]) VALUES ('Stawberry' ,'Description Stawberry' ,768 ,751,' product-10.jpg','product-10.jpg' ,'gam' ,0.0 ,5,8,0.1 ,2,1,'khuong','12/26/2019')</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
@@ -2164,19 +2285,19 @@
       </c>
       <c r="B12" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Tomatoe</v>
+        <v>Green Beans</v>
       </c>
       <c r="C12" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Description Tomatoe</v>
+        <v>Description Green Beans</v>
       </c>
       <c r="D12" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>951</v>
+        <v>39</v>
       </c>
       <c r="E12" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>877</v>
+        <v>39</v>
       </c>
       <c r="F12" t="str">
         <f t="shared" si="2"/>
@@ -2191,19 +2312,19 @@
       </c>
       <c r="I12" s="2" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
       <c r="J12">
         <f t="shared" ca="1" si="4"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="K12">
         <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="L12" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>0.3</v>
+        <v>0.9</v>
       </c>
       <c r="M12">
         <f t="shared" ca="1" si="5"/>
@@ -2218,11 +2339,11 @@
       </c>
       <c r="P12" s="4" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>12/18/2019</v>
+        <v>12/26/2019</v>
       </c>
       <c r="R12" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>INSERT INTO [dbo].[food] ([name] ,[description] ,[price] ,[price_promo] ,[thumb] ,[img] ,[unit] ,[percent_promo] ,[rating] ,[sold] ,[point] ,[type] ,[status] ,[username] ,[modified]) VALUES ('Tomatoe' ,'Description Tomatoe' ,951 ,877,' product-11.jpg','product-11.jpg' ,'gam' ,0.4 ,6,2,0.3 ,4,1,'khuong','12/18/2019')</v>
+        <v>INSERT INTO [dbo].[food] ([name] ,[description] ,[price] ,[price_promo] ,[thumb] ,[img] ,[unit] ,[percent_promo] ,[rating] ,[sold] ,[point] ,[type] ,[status] ,[username] ,[modified]) VALUES ('Green Beans' ,'Description Green Beans' ,39 ,39,' product-11.jpg','product-11.jpg' ,'gam' ,0.6 ,3,5,0.9 ,4,1,'khuong','12/26/2019')</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
@@ -2239,11 +2360,11 @@
       </c>
       <c r="D13" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>674</v>
+        <v>171</v>
       </c>
       <c r="E13" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>670</v>
+        <v>166</v>
       </c>
       <c r="F13" t="str">
         <f t="shared" si="2"/>
@@ -2258,23 +2379,23 @@
       </c>
       <c r="I13" s="2" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
       <c r="J13">
         <f t="shared" ca="1" si="4"/>
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="K13">
         <f t="shared" ca="1" si="4"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="L13" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="M13">
         <f t="shared" ca="1" si="5"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="N13">
         <v>1</v>
@@ -2285,11 +2406,11 @@
       </c>
       <c r="P13" s="4" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>12/18/2019</v>
+        <v>12/26/2019</v>
       </c>
       <c r="R13" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>INSERT INTO [dbo].[food] ([name] ,[description] ,[price] ,[price_promo] ,[thumb] ,[img] ,[unit] ,[percent_promo] ,[rating] ,[sold] ,[point] ,[type] ,[status] ,[username] ,[modified]) VALUES ('Tomatoe' ,'Description Tomatoe' ,674 ,670,' product-12.jpg','product-12.jpg' ,'gam' ,0.6 ,4,4,0.8 ,3,1,'khuong','12/18/2019')</v>
+        <v>INSERT INTO [dbo].[food] ([name] ,[description] ,[price] ,[price_promo] ,[thumb] ,[img] ,[unit] ,[percent_promo] ,[rating] ,[sold] ,[point] ,[type] ,[status] ,[username] ,[modified]) VALUES ('Tomatoe' ,'Description Tomatoe' ,171 ,166,' product-12.jpg','product-12.jpg' ,'gam' ,0.8 ,9,1,0.9 ,1,1,'khuong','12/26/2019')</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
@@ -2298,19 +2419,19 @@
       </c>
       <c r="B14" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Stawberry</v>
+        <v>Bell Perpper</v>
       </c>
       <c r="C14" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Description Stawberry</v>
+        <v>Description Bell Perpper</v>
       </c>
       <c r="D14" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>946</v>
+        <v>599</v>
       </c>
       <c r="E14" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>925</v>
+        <v>554</v>
       </c>
       <c r="F14" t="str">
         <f t="shared" si="2"/>
@@ -2325,19 +2446,19 @@
       </c>
       <c r="I14" s="2" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>0.6</v>
+        <v>0.0</v>
       </c>
       <c r="J14">
         <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="K14">
         <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="L14" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="M14">
         <f t="shared" ca="1" si="5"/>
@@ -2352,11 +2473,11 @@
       </c>
       <c r="P14" s="4" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>12/18/2019</v>
+        <v>12/26/2019</v>
       </c>
       <c r="R14" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>INSERT INTO [dbo].[food] ([name] ,[description] ,[price] ,[price_promo] ,[thumb] ,[img] ,[unit] ,[percent_promo] ,[rating] ,[sold] ,[point] ,[type] ,[status] ,[username] ,[modified]) VALUES ('Stawberry' ,'Description Stawberry' ,946 ,925,' product-13.jpg','product-13.jpg' ,'gam' ,0.6 ,2,2,0.4 ,2,1,'khuong','12/18/2019')</v>
+        <v>INSERT INTO [dbo].[food] ([name] ,[description] ,[price] ,[price_promo] ,[thumb] ,[img] ,[unit] ,[percent_promo] ,[rating] ,[sold] ,[point] ,[type] ,[status] ,[username] ,[modified]) VALUES ('Bell Perpper' ,'Description Bell Perpper' ,599 ,554,' product-13.jpg','product-13.jpg' ,'gam' ,0.0 ,9,6,0.2 ,2,1,'khuong','12/26/2019')</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
@@ -2373,11 +2494,11 @@
       </c>
       <c r="D15" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>348</v>
+        <v>819</v>
       </c>
       <c r="E15" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>327</v>
+        <v>768</v>
       </c>
       <c r="F15" t="str">
         <f t="shared" si="2"/>
@@ -2392,23 +2513,23 @@
       </c>
       <c r="I15" s="2" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>0.9</v>
+        <v>0.7</v>
       </c>
       <c r="J15">
         <f t="shared" ca="1" si="4"/>
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="K15">
         <f t="shared" ca="1" si="4"/>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="L15" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>0.8</v>
+        <v>0.4</v>
       </c>
       <c r="M15">
         <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N15">
         <v>1</v>
@@ -2419,11 +2540,11 @@
       </c>
       <c r="P15" s="4" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>12/18/2019</v>
+        <v>12/26/2019</v>
       </c>
       <c r="R15" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>INSERT INTO [dbo].[food] ([name] ,[description] ,[price] ,[price_promo] ,[thumb] ,[img] ,[unit] ,[percent_promo] ,[rating] ,[sold] ,[point] ,[type] ,[status] ,[username] ,[modified]) VALUES ('Tomatoe' ,'Description Tomatoe' ,348 ,327,' product-14.jpg','product-14.jpg' ,'gam' ,0.9 ,4,7,0.8 ,2,1,'khuong','12/18/2019')</v>
+        <v>INSERT INTO [dbo].[food] ([name] ,[description] ,[price] ,[price_promo] ,[thumb] ,[img] ,[unit] ,[percent_promo] ,[rating] ,[sold] ,[point] ,[type] ,[status] ,[username] ,[modified]) VALUES ('Tomatoe' ,'Description Tomatoe' ,819 ,768,' product-14.jpg','product-14.jpg' ,'gam' ,0.7 ,10,4,0.4 ,3,1,'khuong','12/26/2019')</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
@@ -2440,11 +2561,11 @@
       </c>
       <c r="D16" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>410</v>
+        <v>829</v>
       </c>
       <c r="E16" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>396</v>
+        <v>817</v>
       </c>
       <c r="F16" t="str">
         <f t="shared" si="2"/>
@@ -2459,15 +2580,15 @@
       </c>
       <c r="I16" s="2" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="J16">
         <f t="shared" ca="1" si="4"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="K16">
         <f t="shared" ca="1" si="4"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="L16" s="2">
         <f t="shared" ca="1" si="10"/>
@@ -2475,7 +2596,7 @@
       </c>
       <c r="M16">
         <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N16">
         <v>1</v>
@@ -2486,11 +2607,11 @@
       </c>
       <c r="P16" s="4" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>12/18/2019</v>
+        <v>12/26/2019</v>
       </c>
       <c r="R16" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>INSERT INTO [dbo].[food] ([name] ,[description] ,[price] ,[price_promo] ,[thumb] ,[img] ,[unit] ,[percent_promo] ,[rating] ,[sold] ,[point] ,[type] ,[status] ,[username] ,[modified]) VALUES ('Tomatoe' ,'Description Tomatoe' ,410 ,396,' product-15.jpg','product-15.jpg' ,'gam' ,0.5 ,7,7,0.1 ,2,1,'khuong','12/18/2019')</v>
+        <v>INSERT INTO [dbo].[food] ([name] ,[description] ,[price] ,[price_promo] ,[thumb] ,[img] ,[unit] ,[percent_promo] ,[rating] ,[sold] ,[point] ,[type] ,[status] ,[username] ,[modified]) VALUES ('Tomatoe' ,'Description Tomatoe' ,829 ,817,' product-15.jpg','product-15.jpg' ,'gam' ,0.1 ,8,2,0.1 ,1,1,'khuong','12/26/2019')</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
@@ -2499,19 +2620,19 @@
       </c>
       <c r="B17" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Bell Perpper</v>
+        <v>Tomatoe</v>
       </c>
       <c r="C17" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Description Bell Perpper</v>
+        <v>Description Tomatoe</v>
       </c>
       <c r="D17" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>965</v>
+        <v>305</v>
       </c>
       <c r="E17" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>944</v>
+        <v>291</v>
       </c>
       <c r="F17" t="str">
         <f t="shared" si="2"/>
@@ -2526,23 +2647,23 @@
       </c>
       <c r="I17" s="2" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
       <c r="J17">
         <f t="shared" ca="1" si="4"/>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="K17">
         <f t="shared" ca="1" si="4"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L17" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="M17">
         <f t="shared" ca="1" si="5"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N17">
         <v>1</v>
@@ -2553,11 +2674,11 @@
       </c>
       <c r="P17" s="4" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>12/18/2019</v>
+        <v>12/26/2019</v>
       </c>
       <c r="R17" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>INSERT INTO [dbo].[food] ([name] ,[description] ,[price] ,[price_promo] ,[thumb] ,[img] ,[unit] ,[percent_promo] ,[rating] ,[sold] ,[point] ,[type] ,[status] ,[username] ,[modified]) VALUES ('Bell Perpper' ,'Description Bell Perpper' ,965 ,944,' product-16.jpg','product-16.jpg' ,'gam' ,0.5 ,5,9,0.5 ,4,1,'khuong','12/18/2019')</v>
+        <v>INSERT INTO [dbo].[food] ([name] ,[description] ,[price] ,[price_promo] ,[thumb] ,[img] ,[unit] ,[percent_promo] ,[rating] ,[sold] ,[point] ,[type] ,[status] ,[username] ,[modified]) VALUES ('Tomatoe' ,'Description Tomatoe' ,305 ,291,' product-16.jpg','product-16.jpg' ,'gam' ,0.7 ,9,10,0.1 ,3,1,'khuong','12/26/2019')</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
@@ -2566,19 +2687,19 @@
       </c>
       <c r="B18" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Stawberry</v>
+        <v>Green Beans</v>
       </c>
       <c r="C18" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Description Stawberry</v>
+        <v>Description Green Beans</v>
       </c>
       <c r="D18" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>76</v>
+        <v>194</v>
       </c>
       <c r="E18" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>73</v>
+        <v>186</v>
       </c>
       <c r="F18" t="str">
         <f t="shared" si="2"/>
@@ -2593,7 +2714,7 @@
       </c>
       <c r="I18" s="2" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>-0.1</v>
+        <v>0.0</v>
       </c>
       <c r="J18">
         <f t="shared" ca="1" si="4"/>
@@ -2601,15 +2722,15 @@
       </c>
       <c r="K18">
         <f t="shared" ca="1" si="4"/>
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="L18" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>0.7</v>
+        <v>0.1</v>
       </c>
       <c r="M18">
         <f t="shared" ca="1" si="5"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="N18">
         <v>1</v>
@@ -2620,11 +2741,11 @@
       </c>
       <c r="P18" s="4" t="str">
         <f t="shared" ca="1" si="11"/>
-        <v>12/18/2019</v>
+        <v>12/26/2019</v>
       </c>
       <c r="R18" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>INSERT INTO [dbo].[food] ([name] ,[description] ,[price] ,[price_promo] ,[thumb] ,[img] ,[unit] ,[percent_promo] ,[rating] ,[sold] ,[point] ,[type] ,[status] ,[username] ,[modified]) VALUES ('Stawberry' ,'Description Stawberry' ,76 ,73,' product-17.jpg','product-17.jpg' ,'gam' ,-0.1 ,4,9,0.7 ,4,1,'khuong','12/18/2019')</v>
+        <v>INSERT INTO [dbo].[food] ([name] ,[description] ,[price] ,[price_promo] ,[thumb] ,[img] ,[unit] ,[percent_promo] ,[rating] ,[sold] ,[point] ,[type] ,[status] ,[username] ,[modified]) VALUES ('Green Beans' ,'Description Green Beans' ,194 ,186,' product-17.jpg','product-17.jpg' ,'gam' ,0.0 ,4,6,0.1 ,2,1,'khuong','12/26/2019')</v>
       </c>
     </row>
   </sheetData>
@@ -2703,7 +2824,7 @@
       </c>
       <c r="I2" s="3">
         <f ca="1">NOW()</f>
-        <v>43817.962288310184</v>
+        <v>43825.10472210648</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -2734,7 +2855,7 @@
       </c>
       <c r="I3" s="3">
         <f t="shared" ref="I3:I5" ca="1" si="1">NOW()</f>
-        <v>43817.962288310184</v>
+        <v>43825.10472210648</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -2765,7 +2886,7 @@
       </c>
       <c r="I4" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>43817.962288310184</v>
+        <v>43825.10472210648</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -2796,7 +2917,7 @@
       </c>
       <c r="I5" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>43817.962288310184</v>
+        <v>43825.10472210648</v>
       </c>
     </row>
   </sheetData>
@@ -2869,7 +2990,7 @@
       </c>
       <c r="E2">
         <f ca="1">RANDBETWEEN(1,4)</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F2" t="str">
         <f t="shared" ref="F2:F31" si="0">"image_1 ("&amp;A2&amp;").jpg"</f>
@@ -2883,15 +3004,15 @@
       </c>
       <c r="I2" s="3">
         <f ca="1">NOW()</f>
-        <v>43817.962288310184</v>
+        <v>43825.10472210648</v>
       </c>
       <c r="J2" s="3">
         <f ca="1">NOW()</f>
-        <v>43817.962288310184</v>
+        <v>43825.10472210648</v>
       </c>
       <c r="L2" t="str">
         <f ca="1">"UPDATE [dbo].[post] SET [type] = '"&amp;E2&amp;"' WHERE post_id="&amp;A2</f>
-        <v>UPDATE [dbo].[post] SET [type] = '4' WHERE post_id=1</v>
+        <v>UPDATE [dbo].[post] SET [type] = '1' WHERE post_id=1</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -2909,7 +3030,7 @@
       </c>
       <c r="E3">
         <f t="shared" ref="E3:E31" ca="1" si="1">RANDBETWEEN(1,4)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F3" t="str">
         <f t="shared" si="0"/>
@@ -2923,15 +3044,15 @@
       </c>
       <c r="I3" s="3">
         <f t="shared" ref="I3:J31" ca="1" si="2">NOW()</f>
-        <v>43817.962288310184</v>
+        <v>43825.10472210648</v>
       </c>
       <c r="J3" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43817.962288310184</v>
+        <v>43825.10472210648</v>
       </c>
       <c r="L3" t="str">
         <f t="shared" ref="L3:L31" ca="1" si="3">"UPDATE [dbo].[post] SET [type] = '"&amp;E3&amp;"' WHERE post_id="&amp;A3</f>
-        <v>UPDATE [dbo].[post] SET [type] = '4' WHERE post_id=2</v>
+        <v>UPDATE [dbo].[post] SET [type] = '3' WHERE post_id=2</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -2963,11 +3084,11 @@
       </c>
       <c r="I4" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43817.962288310184</v>
+        <v>43825.10472210648</v>
       </c>
       <c r="J4" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43817.962288310184</v>
+        <v>43825.10472210648</v>
       </c>
       <c r="L4" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -3003,11 +3124,11 @@
       </c>
       <c r="I5" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43817.962288310184</v>
+        <v>43825.10472210648</v>
       </c>
       <c r="J5" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43817.962288310184</v>
+        <v>43825.10472210648</v>
       </c>
       <c r="L5" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -3043,11 +3164,11 @@
       </c>
       <c r="I6" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43817.962288310184</v>
+        <v>43825.10472210648</v>
       </c>
       <c r="J6" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43817.962288310184</v>
+        <v>43825.10472210648</v>
       </c>
       <c r="L6" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -3069,7 +3190,7 @@
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F7" t="str">
         <f t="shared" si="0"/>
@@ -3083,15 +3204,15 @@
       </c>
       <c r="I7" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43817.962288310184</v>
+        <v>43825.10472210648</v>
       </c>
       <c r="J7" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43817.962288310184</v>
+        <v>43825.10472210648</v>
       </c>
       <c r="L7" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>UPDATE [dbo].[post] SET [type] = '4' WHERE post_id=6</v>
+        <v>UPDATE [dbo].[post] SET [type] = '2' WHERE post_id=6</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -3123,11 +3244,11 @@
       </c>
       <c r="I8" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43817.962288310184</v>
+        <v>43825.10472210648</v>
       </c>
       <c r="J8" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43817.962288310184</v>
+        <v>43825.10472210648</v>
       </c>
       <c r="L8" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -3163,11 +3284,11 @@
       </c>
       <c r="I9" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43817.962288310184</v>
+        <v>43825.10472210648</v>
       </c>
       <c r="J9" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43817.962288310184</v>
+        <v>43825.10472210648</v>
       </c>
       <c r="L9" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -3189,7 +3310,7 @@
       </c>
       <c r="E10">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F10" t="str">
         <f t="shared" si="0"/>
@@ -3203,15 +3324,15 @@
       </c>
       <c r="I10" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43817.962288310184</v>
+        <v>43825.10472210648</v>
       </c>
       <c r="J10" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43817.962288310184</v>
+        <v>43825.10472210648</v>
       </c>
       <c r="L10" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>UPDATE [dbo].[post] SET [type] = '4' WHERE post_id=9</v>
+        <v>UPDATE [dbo].[post] SET [type] = '2' WHERE post_id=9</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -3229,7 +3350,7 @@
       </c>
       <c r="E11">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F11" t="str">
         <f t="shared" si="0"/>
@@ -3243,15 +3364,15 @@
       </c>
       <c r="I11" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43817.962288310184</v>
+        <v>43825.10472210648</v>
       </c>
       <c r="J11" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43817.962288310184</v>
+        <v>43825.10472210648</v>
       </c>
       <c r="L11" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>UPDATE [dbo].[post] SET [type] = '4' WHERE post_id=10</v>
+        <v>UPDATE [dbo].[post] SET [type] = '3' WHERE post_id=10</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -3269,7 +3390,7 @@
       </c>
       <c r="E12">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F12" t="str">
         <f t="shared" si="0"/>
@@ -3283,15 +3404,15 @@
       </c>
       <c r="I12" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43817.962288310184</v>
+        <v>43825.10472210648</v>
       </c>
       <c r="J12" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43817.962288310184</v>
+        <v>43825.10472210648</v>
       </c>
       <c r="L12" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>UPDATE [dbo].[post] SET [type] = '4' WHERE post_id=11</v>
+        <v>UPDATE [dbo].[post] SET [type] = '1' WHERE post_id=11</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -3309,7 +3430,7 @@
       </c>
       <c r="E13">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F13" t="str">
         <f t="shared" si="0"/>
@@ -3323,15 +3444,15 @@
       </c>
       <c r="I13" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43817.962288310184</v>
+        <v>43825.10472210648</v>
       </c>
       <c r="J13" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43817.962288310184</v>
+        <v>43825.10472210648</v>
       </c>
       <c r="L13" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>UPDATE [dbo].[post] SET [type] = '1' WHERE post_id=12</v>
+        <v>UPDATE [dbo].[post] SET [type] = '2' WHERE post_id=12</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -3363,11 +3484,11 @@
       </c>
       <c r="I14" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43817.962288310184</v>
+        <v>43825.10472210648</v>
       </c>
       <c r="J14" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43817.962288310184</v>
+        <v>43825.10472210648</v>
       </c>
       <c r="L14" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -3389,7 +3510,7 @@
       </c>
       <c r="E15">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F15" t="str">
         <f t="shared" si="0"/>
@@ -3403,15 +3524,15 @@
       </c>
       <c r="I15" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43817.962288310184</v>
+        <v>43825.10472210648</v>
       </c>
       <c r="J15" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43817.962288310184</v>
+        <v>43825.10472210648</v>
       </c>
       <c r="L15" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>UPDATE [dbo].[post] SET [type] = '4' WHERE post_id=14</v>
+        <v>UPDATE [dbo].[post] SET [type] = '3' WHERE post_id=14</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -3429,7 +3550,7 @@
       </c>
       <c r="E16">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F16" t="str">
         <f t="shared" si="0"/>
@@ -3443,15 +3564,15 @@
       </c>
       <c r="I16" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43817.962288310184</v>
+        <v>43825.10472210648</v>
       </c>
       <c r="J16" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43817.962288310184</v>
+        <v>43825.10472210648</v>
       </c>
       <c r="L16" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>UPDATE [dbo].[post] SET [type] = '3' WHERE post_id=15</v>
+        <v>UPDATE [dbo].[post] SET [type] = '2' WHERE post_id=15</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -3469,7 +3590,7 @@
       </c>
       <c r="E17">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F17" t="str">
         <f t="shared" si="0"/>
@@ -3483,15 +3604,15 @@
       </c>
       <c r="I17" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43817.962288310184</v>
+        <v>43825.10472210648</v>
       </c>
       <c r="J17" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43817.962288310184</v>
+        <v>43825.10472210648</v>
       </c>
       <c r="L17" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>UPDATE [dbo].[post] SET [type] = '2' WHERE post_id=16</v>
+        <v>UPDATE [dbo].[post] SET [type] = '4' WHERE post_id=16</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -3509,7 +3630,7 @@
       </c>
       <c r="E18">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F18" t="str">
         <f t="shared" si="0"/>
@@ -3523,15 +3644,15 @@
       </c>
       <c r="I18" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43817.962288310184</v>
+        <v>43825.10472210648</v>
       </c>
       <c r="J18" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43817.962288310184</v>
+        <v>43825.10472210648</v>
       </c>
       <c r="L18" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>UPDATE [dbo].[post] SET [type] = '2' WHERE post_id=17</v>
+        <v>UPDATE [dbo].[post] SET [type] = '1' WHERE post_id=17</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
@@ -3549,7 +3670,7 @@
       </c>
       <c r="E19">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F19" t="str">
         <f t="shared" si="0"/>
@@ -3563,15 +3684,15 @@
       </c>
       <c r="I19" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43817.962288310184</v>
+        <v>43825.10472210648</v>
       </c>
       <c r="J19" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43817.962288310184</v>
+        <v>43825.10472210648</v>
       </c>
       <c r="L19" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>UPDATE [dbo].[post] SET [type] = '3' WHERE post_id=18</v>
+        <v>UPDATE [dbo].[post] SET [type] = '4' WHERE post_id=18</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -3589,7 +3710,7 @@
       </c>
       <c r="E20">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F20" t="str">
         <f t="shared" si="0"/>
@@ -3603,15 +3724,15 @@
       </c>
       <c r="I20" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43817.962288310184</v>
+        <v>43825.10472210648</v>
       </c>
       <c r="J20" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43817.962288310184</v>
+        <v>43825.10472210648</v>
       </c>
       <c r="L20" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>UPDATE [dbo].[post] SET [type] = '1' WHERE post_id=19</v>
+        <v>UPDATE [dbo].[post] SET [type] = '2' WHERE post_id=19</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -3629,7 +3750,7 @@
       </c>
       <c r="E21">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F21" t="str">
         <f t="shared" si="0"/>
@@ -3643,15 +3764,15 @@
       </c>
       <c r="I21" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43817.962288310184</v>
+        <v>43825.10472210648</v>
       </c>
       <c r="J21" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43817.962288310184</v>
+        <v>43825.10472210648</v>
       </c>
       <c r="L21" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>UPDATE [dbo].[post] SET [type] = '4' WHERE post_id=20</v>
+        <v>UPDATE [dbo].[post] SET [type] = '1' WHERE post_id=20</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
@@ -3669,7 +3790,7 @@
       </c>
       <c r="E22">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F22" t="str">
         <f t="shared" si="0"/>
@@ -3683,15 +3804,15 @@
       </c>
       <c r="I22" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43817.962288310184</v>
+        <v>43825.10472210648</v>
       </c>
       <c r="J22" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43817.962288310184</v>
+        <v>43825.10472210648</v>
       </c>
       <c r="L22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>UPDATE [dbo].[post] SET [type] = '4' WHERE post_id=21</v>
+        <v>UPDATE [dbo].[post] SET [type] = '1' WHERE post_id=21</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
@@ -3709,7 +3830,7 @@
       </c>
       <c r="E23">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F23" t="str">
         <f t="shared" si="0"/>
@@ -3723,15 +3844,15 @@
       </c>
       <c r="I23" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43817.962288310184</v>
+        <v>43825.10472210648</v>
       </c>
       <c r="J23" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43817.962288310184</v>
+        <v>43825.10472210648</v>
       </c>
       <c r="L23" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>UPDATE [dbo].[post] SET [type] = '2' WHERE post_id=22</v>
+        <v>UPDATE [dbo].[post] SET [type] = '3' WHERE post_id=22</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
@@ -3763,11 +3884,11 @@
       </c>
       <c r="I24" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43817.962288310184</v>
+        <v>43825.10472210648</v>
       </c>
       <c r="J24" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43817.962288310184</v>
+        <v>43825.10472210648</v>
       </c>
       <c r="L24" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -3789,7 +3910,7 @@
       </c>
       <c r="E25">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F25" t="str">
         <f t="shared" si="0"/>
@@ -3803,15 +3924,15 @@
       </c>
       <c r="I25" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43817.962288310184</v>
+        <v>43825.10472210648</v>
       </c>
       <c r="J25" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43817.962288310184</v>
+        <v>43825.10472210648</v>
       </c>
       <c r="L25" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>UPDATE [dbo].[post] SET [type] = '1' WHERE post_id=24</v>
+        <v>UPDATE [dbo].[post] SET [type] = '4' WHERE post_id=24</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
@@ -3829,7 +3950,7 @@
       </c>
       <c r="E26">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F26" t="str">
         <f t="shared" si="0"/>
@@ -3843,15 +3964,15 @@
       </c>
       <c r="I26" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43817.962288310184</v>
+        <v>43825.10472210648</v>
       </c>
       <c r="J26" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43817.962288310184</v>
+        <v>43825.10472210648</v>
       </c>
       <c r="L26" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>UPDATE [dbo].[post] SET [type] = '3' WHERE post_id=25</v>
+        <v>UPDATE [dbo].[post] SET [type] = '2' WHERE post_id=25</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
@@ -3869,7 +3990,7 @@
       </c>
       <c r="E27">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F27" t="str">
         <f t="shared" si="0"/>
@@ -3883,15 +4004,15 @@
       </c>
       <c r="I27" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43817.962288310184</v>
+        <v>43825.10472210648</v>
       </c>
       <c r="J27" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43817.962288310184</v>
+        <v>43825.10472210648</v>
       </c>
       <c r="L27" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>UPDATE [dbo].[post] SET [type] = '2' WHERE post_id=26</v>
+        <v>UPDATE [dbo].[post] SET [type] = '3' WHERE post_id=26</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
@@ -3909,7 +4030,7 @@
       </c>
       <c r="E28">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F28" t="str">
         <f t="shared" si="0"/>
@@ -3923,15 +4044,15 @@
       </c>
       <c r="I28" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43817.962288310184</v>
+        <v>43825.10472210648</v>
       </c>
       <c r="J28" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43817.962288310184</v>
+        <v>43825.10472210648</v>
       </c>
       <c r="L28" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>UPDATE [dbo].[post] SET [type] = '2' WHERE post_id=27</v>
+        <v>UPDATE [dbo].[post] SET [type] = '3' WHERE post_id=27</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
@@ -3963,11 +4084,11 @@
       </c>
       <c r="I29" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43817.962288310184</v>
+        <v>43825.10472210648</v>
       </c>
       <c r="J29" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43817.962288310184</v>
+        <v>43825.10472210648</v>
       </c>
       <c r="L29" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -4003,11 +4124,11 @@
       </c>
       <c r="I30" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43817.962288310184</v>
+        <v>43825.10472210648</v>
       </c>
       <c r="J30" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43817.962288310184</v>
+        <v>43825.10472210648</v>
       </c>
       <c r="L30" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -4029,7 +4150,7 @@
       </c>
       <c r="E31">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F31" t="str">
         <f t="shared" si="0"/>
@@ -4043,15 +4164,15 @@
       </c>
       <c r="I31" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43817.962288310184</v>
+        <v>43825.10472210648</v>
       </c>
       <c r="J31" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43817.962288310184</v>
+        <v>43825.10472210648</v>
       </c>
       <c r="L31" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>UPDATE [dbo].[post] SET [type] = '4' WHERE post_id=30</v>
+        <v>UPDATE [dbo].[post] SET [type] = '1' WHERE post_id=30</v>
       </c>
     </row>
   </sheetData>
@@ -4086,7 +4207,7 @@
       </c>
       <c r="B2">
         <f ca="1">RANDBETWEEN(1,5)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C2" t="str">
         <f>"des "&amp;A2</f>
@@ -4109,7 +4230,7 @@
       </c>
       <c r="B3">
         <f t="shared" ref="B3:B18" ca="1" si="0">RANDBETWEEN(1,5)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C3" t="str">
         <f t="shared" ref="C3:C18" si="1">"des "&amp;A3</f>
@@ -4169,7 +4290,7 @@
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C6" t="str">
         <f t="shared" si="1"/>
@@ -4186,7 +4307,7 @@
       </c>
       <c r="B7">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C7" t="str">
         <f t="shared" si="1"/>
@@ -4203,7 +4324,7 @@
       </c>
       <c r="B8">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C8" t="str">
         <f t="shared" si="1"/>
@@ -4220,7 +4341,7 @@
       </c>
       <c r="B9">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C9" t="str">
         <f t="shared" si="1"/>
@@ -4237,7 +4358,7 @@
       </c>
       <c r="B10">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C10" t="str">
         <f t="shared" si="1"/>
@@ -4254,7 +4375,7 @@
       </c>
       <c r="B11">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C11" t="str">
         <f t="shared" si="1"/>
@@ -4271,7 +4392,7 @@
       </c>
       <c r="B12">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C12" t="str">
         <f t="shared" si="1"/>
@@ -4305,7 +4426,7 @@
       </c>
       <c r="B14">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C14" t="str">
         <f t="shared" si="1"/>
@@ -4339,7 +4460,7 @@
       </c>
       <c r="B16">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C16" t="str">
         <f t="shared" si="1"/>
@@ -4356,7 +4477,7 @@
       </c>
       <c r="B17">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C17" t="str">
         <f t="shared" si="1"/>
@@ -4373,7 +4494,7 @@
       </c>
       <c r="B18">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C18" t="str">
         <f t="shared" si="1"/>
@@ -4387,4 +4508,813 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O5" sqref="O5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="11.85546875" customWidth="1"/>
+    <col min="6" max="6" width="26" customWidth="1"/>
+    <col min="8" max="8" width="12.140625" customWidth="1"/>
+    <col min="9" max="9" width="20.5703125" customWidth="1"/>
+    <col min="12" max="12" width="20.85546875" customWidth="1"/>
+    <col min="16" max="16" width="34.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B1" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>139</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" t="s">
+        <v>140</v>
+      </c>
+      <c r="H2" t="s">
+        <v>141</v>
+      </c>
+      <c r="I2" t="s">
+        <v>142</v>
+      </c>
+      <c r="J2" t="s">
+        <v>143</v>
+      </c>
+      <c r="K2" t="s">
+        <v>3</v>
+      </c>
+      <c r="L2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="str">
+        <f>"khuong"&amp;A3</f>
+        <v>khuong1</v>
+      </c>
+      <c r="C3">
+        <v>123</v>
+      </c>
+      <c r="D3" t="str">
+        <f>"khuong "&amp;A3</f>
+        <v>khuong 1</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="F3" s="8" t="str">
+        <f>"yoshi@gmail.com"</f>
+        <v>yoshi@gmail.com</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="H3">
+        <f ca="1">RANDBETWEEN(1,5)</f>
+        <v>5</v>
+      </c>
+      <c r="I3">
+        <f ca="1">RANDBETWEEN(1,5)</f>
+        <v>5</v>
+      </c>
+      <c r="J3">
+        <f ca="1">SUM(H3,I3)</f>
+        <v>10</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3" s="3">
+        <f ca="1">NOW()</f>
+        <v>43825.10472210648</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="str">
+        <f t="shared" ref="B4:B18" si="0">"khuong"&amp;A4</f>
+        <v>khuong2</v>
+      </c>
+      <c r="C4">
+        <v>123</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" ref="D4:D18" si="1">"khuong "&amp;A4</f>
+        <v>khuong 2</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="F4" s="8" t="str">
+        <f t="shared" ref="F4:F18" si="2">"yoshi@gmail.com"</f>
+        <v>yoshi@gmail.com</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="H4">
+        <f t="shared" ref="H4:I18" ca="1" si="3">RANDBETWEEN(1,5)</f>
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <f t="shared" ref="J4:J18" ca="1" si="4">SUM(H4,I4)</f>
+        <v>2</v>
+      </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4" s="3">
+        <f t="shared" ref="L4:L18" ca="1" si="5">NOW()</f>
+        <v>43825.10472210648</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="str">
+        <f t="shared" si="0"/>
+        <v>khuong3</v>
+      </c>
+      <c r="C5">
+        <v>123</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" si="1"/>
+        <v>khuong 3</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="F5" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>yoshi@gmail.com</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="H5">
+        <f t="shared" ca="1" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="I5">
+        <f t="shared" ca="1" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="J5">
+        <f t="shared" ca="1" si="4"/>
+        <v>9</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="L5" s="3">
+        <f t="shared" ca="1" si="5"/>
+        <v>43825.10472210648</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="str">
+        <f t="shared" si="0"/>
+        <v>khuong4</v>
+      </c>
+      <c r="C6">
+        <v>123</v>
+      </c>
+      <c r="D6" t="str">
+        <f t="shared" si="1"/>
+        <v>khuong 4</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="F6" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>yoshi@gmail.com</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="H6">
+        <f t="shared" ca="1" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="I6">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <f t="shared" ca="1" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="L6" s="3">
+        <f t="shared" ca="1" si="5"/>
+        <v>43825.10472210648</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="str">
+        <f t="shared" si="0"/>
+        <v>khuong5</v>
+      </c>
+      <c r="C7">
+        <v>123</v>
+      </c>
+      <c r="D7" t="str">
+        <f t="shared" si="1"/>
+        <v>khuong 5</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="F7" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>yoshi@gmail.com</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="H7">
+        <f t="shared" ca="1" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="I7">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="J7">
+        <f t="shared" ca="1" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+      <c r="L7" s="3">
+        <f t="shared" ca="1" si="5"/>
+        <v>43825.10472210648</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="str">
+        <f t="shared" si="0"/>
+        <v>khuong6</v>
+      </c>
+      <c r="C8">
+        <v>123</v>
+      </c>
+      <c r="D8" t="str">
+        <f t="shared" si="1"/>
+        <v>khuong 6</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="F8" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>yoshi@gmail.com</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="H8">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="I8">
+        <f t="shared" ca="1" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="J8">
+        <f t="shared" ca="1" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="L8" s="3">
+        <f t="shared" ca="1" si="5"/>
+        <v>43825.10472210648</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="str">
+        <f t="shared" si="0"/>
+        <v>khuong7</v>
+      </c>
+      <c r="C9">
+        <v>123</v>
+      </c>
+      <c r="D9" t="str">
+        <f t="shared" si="1"/>
+        <v>khuong 7</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="F9" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>yoshi@gmail.com</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="H9">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="I9">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <f t="shared" ca="1" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="K9">
+        <v>1</v>
+      </c>
+      <c r="L9" s="3">
+        <f t="shared" ca="1" si="5"/>
+        <v>43825.10472210648</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="str">
+        <f t="shared" si="0"/>
+        <v>khuong8</v>
+      </c>
+      <c r="C10">
+        <v>123</v>
+      </c>
+      <c r="D10" t="str">
+        <f t="shared" si="1"/>
+        <v>khuong 8</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="F10" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>yoshi@gmail.com</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="H10">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="I10">
+        <f t="shared" ca="1" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="J10">
+        <f t="shared" ca="1" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="K10">
+        <v>1</v>
+      </c>
+      <c r="L10" s="3">
+        <f t="shared" ca="1" si="5"/>
+        <v>43825.10472210648</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="str">
+        <f t="shared" si="0"/>
+        <v>khuong9</v>
+      </c>
+      <c r="C11">
+        <v>123</v>
+      </c>
+      <c r="D11" t="str">
+        <f t="shared" si="1"/>
+        <v>khuong 9</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="F11" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>yoshi@gmail.com</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="H11">
+        <f t="shared" ca="1" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="I11">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="J11">
+        <f t="shared" ca="1" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
+      <c r="L11" s="3">
+        <f t="shared" ca="1" si="5"/>
+        <v>43825.10472210648</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" t="str">
+        <f t="shared" si="0"/>
+        <v>khuong10</v>
+      </c>
+      <c r="C12">
+        <v>123</v>
+      </c>
+      <c r="D12" t="str">
+        <f t="shared" si="1"/>
+        <v>khuong 10</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="F12" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>yoshi@gmail.com</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="H12">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="I12">
+        <f t="shared" ca="1" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="J12">
+        <f t="shared" ca="1" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="K12">
+        <v>1</v>
+      </c>
+      <c r="L12" s="3">
+        <f t="shared" ca="1" si="5"/>
+        <v>43825.10472210648</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" t="str">
+        <f t="shared" si="0"/>
+        <v>khuong11</v>
+      </c>
+      <c r="C13">
+        <v>123</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" si="1"/>
+        <v>khuong 11</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="F13" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>yoshi@gmail.com</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="H13">
+        <f t="shared" ca="1" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="I13">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="J13">
+        <f t="shared" ca="1" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="K13">
+        <v>1</v>
+      </c>
+      <c r="L13" s="3">
+        <f t="shared" ca="1" si="5"/>
+        <v>43825.10472210648</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" t="str">
+        <f t="shared" si="0"/>
+        <v>khuong12</v>
+      </c>
+      <c r="C14">
+        <v>123</v>
+      </c>
+      <c r="D14" t="str">
+        <f t="shared" si="1"/>
+        <v>khuong 12</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="F14" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>yoshi@gmail.com</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="H14">
+        <f t="shared" ca="1" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="I14">
+        <f t="shared" ca="1" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="J14">
+        <f t="shared" ca="1" si="4"/>
+        <v>8</v>
+      </c>
+      <c r="K14">
+        <v>1</v>
+      </c>
+      <c r="L14" s="3">
+        <f t="shared" ca="1" si="5"/>
+        <v>43825.10472210648</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" t="str">
+        <f t="shared" si="0"/>
+        <v>khuong13</v>
+      </c>
+      <c r="C15">
+        <v>123</v>
+      </c>
+      <c r="D15" t="str">
+        <f t="shared" si="1"/>
+        <v>khuong 13</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="F15" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>yoshi@gmail.com</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="H15">
+        <f t="shared" ca="1" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="I15">
+        <f t="shared" ca="1" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="J15">
+        <f t="shared" ca="1" si="4"/>
+        <v>8</v>
+      </c>
+      <c r="K15">
+        <v>1</v>
+      </c>
+      <c r="L15" s="3">
+        <f t="shared" ca="1" si="5"/>
+        <v>43825.10472210648</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" t="str">
+        <f t="shared" si="0"/>
+        <v>khuong14</v>
+      </c>
+      <c r="C16">
+        <v>123</v>
+      </c>
+      <c r="D16" t="str">
+        <f t="shared" si="1"/>
+        <v>khuong 14</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="F16" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>yoshi@gmail.com</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="H16">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="I16">
+        <f t="shared" ca="1" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="J16">
+        <f t="shared" ca="1" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="K16">
+        <v>1</v>
+      </c>
+      <c r="L16" s="3">
+        <f t="shared" ca="1" si="5"/>
+        <v>43825.10472210648</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17" t="str">
+        <f t="shared" si="0"/>
+        <v>khuong15</v>
+      </c>
+      <c r="C17">
+        <v>123</v>
+      </c>
+      <c r="D17" t="str">
+        <f t="shared" si="1"/>
+        <v>khuong 15</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="F17" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>yoshi@gmail.com</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="H17">
+        <f t="shared" ca="1" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="I17">
+        <f t="shared" ca="1" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="J17">
+        <f t="shared" ca="1" si="4"/>
+        <v>8</v>
+      </c>
+      <c r="K17">
+        <v>1</v>
+      </c>
+      <c r="L17" s="3">
+        <f t="shared" ca="1" si="5"/>
+        <v>43825.10472210648</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18" t="str">
+        <f t="shared" si="0"/>
+        <v>khuong16</v>
+      </c>
+      <c r="C18">
+        <v>123</v>
+      </c>
+      <c r="D18" t="str">
+        <f t="shared" si="1"/>
+        <v>khuong 16</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="F18" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>yoshi@gmail.com</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="H18">
+        <f t="shared" ca="1" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="I18">
+        <f t="shared" ca="1" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="J18">
+        <f t="shared" ca="1" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="K18">
+        <v>1</v>
+      </c>
+      <c r="L18" s="3">
+        <f t="shared" ca="1" si="5"/>
+        <v>43825.10472210648</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:P1"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="F3" r:id="rId1" display="yoshi240499@gmail.com"/>
+    <hyperlink ref="F4:F18" r:id="rId2" display="yoshi240499@gmail.com"/>
+    <hyperlink ref="G3" r:id="rId3" display="123@111"/>
+    <hyperlink ref="G4:G18" r:id="rId4" display="123@111"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
version 3.5 Update Order
</commit_message>
<xml_diff>
--- a/rau.xlsx
+++ b/rau.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6765" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6765" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="LoaiSP" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Post" sheetId="5" r:id="rId5"/>
     <sheet name="Relative_food" sheetId="6" r:id="rId6"/>
     <sheet name="Customer" sheetId="7" r:id="rId7"/>
+    <sheet name="Order" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="185">
   <si>
     <t>type_id</t>
   </si>
@@ -558,6 +559,33 @@
   </si>
   <si>
     <t>a138</t>
+  </si>
+  <si>
+    <t>SELECT [order_id] ,[cus_name] ,[cus_phone] ,[cus_add] ,[quan] ,[sum] ,[status] ,[username] ,[modified] ,[created] ,[cus_username] FROM [dbo].[order]</t>
+  </si>
+  <si>
+    <t>order_id</t>
+  </si>
+  <si>
+    <t>cus_name</t>
+  </si>
+  <si>
+    <t>cus_phone</t>
+  </si>
+  <si>
+    <t>cus_add</t>
+  </si>
+  <si>
+    <t>quan</t>
+  </si>
+  <si>
+    <t>khuong 1</t>
+  </si>
+  <si>
+    <t>0306171362</t>
+  </si>
+  <si>
+    <t>cus_username</t>
   </si>
 </sst>
 </file>
@@ -616,12 +644,12 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1615,19 +1643,19 @@
 IF(RANDBETWEEN(1,4)=2,"Stawberry",
 IF(RANDBETWEEN(1,4)=3,"Green Beans","Tomatoe"
 )))</f>
-        <v>Stawberry</v>
+        <v>Tomatoe</v>
       </c>
       <c r="C2" t="str">
         <f t="shared" ref="C2:C18" ca="1" si="1">"Description "&amp;B2</f>
-        <v>Description Stawberry</v>
+        <v>Description Tomatoe</v>
       </c>
       <c r="D2" t="str">
         <f ca="1">TEXT(RANDBETWEEN(1,1000),"0")</f>
-        <v>957</v>
+        <v>939</v>
       </c>
       <c r="E2" s="2" t="str">
         <f ca="1">TEXT(D2-D2*RAND()*0.1,"0")</f>
-        <v>953</v>
+        <v>848</v>
       </c>
       <c r="F2" t="str">
         <f t="shared" ref="F2:F18" si="2">"product-"&amp;A2&amp;".jpg"</f>
@@ -1642,23 +1670,23 @@
       </c>
       <c r="I2" s="2" t="str">
         <f ca="1">TEXT(RAND()+0.1-0.2,"0.0")</f>
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="J2">
         <f t="shared" ref="J2:K18" ca="1" si="4">RANDBETWEEN(1,10)</f>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="K2">
         <f t="shared" ca="1" si="4"/>
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="L2" s="2">
         <f ca="1">ABS(TEXT(RAND()+0.1-0.2,"0.0"))</f>
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
       <c r="M2">
         <f t="shared" ref="M2:M18" ca="1" si="5">RANDBETWEEN(1,4)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="N2">
         <v>1</v>
@@ -1673,7 +1701,7 @@
       </c>
       <c r="R2" t="str">
         <f ca="1">"INSERT INTO [dbo].[food] ([name] ,[description] ,[price] ,[price_promo] ,[thumb] ,[img] ,[unit] ,[percent_promo] ,[rating] ,[sold] ,[point] ,[type] ,[status] ,[username] ,[modified]) VALUES ('"&amp;B2&amp;"' ,'"&amp;C2&amp;"' ,"&amp;D2&amp;" ,"&amp;E2&amp;",' "&amp;F2&amp;"','"&amp;G2&amp;"' ,'"&amp;H2&amp;"' ,"&amp;I2&amp;" ,"&amp;J2&amp;","&amp;K2&amp;","&amp;L2&amp;" ,"&amp;M2&amp;","&amp;N2&amp;",'"&amp;O2&amp;"','"&amp;P2&amp;"')"</f>
-        <v>INSERT INTO [dbo].[food] ([name] ,[description] ,[price] ,[price_promo] ,[thumb] ,[img] ,[unit] ,[percent_promo] ,[rating] ,[sold] ,[point] ,[type] ,[status] ,[username] ,[modified]) VALUES ('Stawberry' ,'Description Stawberry' ,957 ,953,' product-1.jpg','product-1.jpg' ,'gam' ,0.5 ,8,10,0.7 ,1,1,'khuong','12/26/2019')</v>
+        <v>INSERT INTO [dbo].[food] ([name] ,[description] ,[price] ,[price_promo] ,[thumb] ,[img] ,[unit] ,[percent_promo] ,[rating] ,[sold] ,[point] ,[type] ,[status] ,[username] ,[modified]) VALUES ('Tomatoe' ,'Description Tomatoe' ,939 ,848,' product-1.jpg','product-1.jpg' ,'gam' ,0.1 ,6,2,0.3 ,4,1,'khuong','12/26/2019')</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
@@ -1690,11 +1718,11 @@
       </c>
       <c r="D3" t="str">
         <f t="shared" ref="D3:D18" ca="1" si="7">TEXT(RANDBETWEEN(1,1000),"0")</f>
-        <v>376</v>
+        <v>214</v>
       </c>
       <c r="E3" s="2" t="str">
         <f t="shared" ref="E3:E18" ca="1" si="8">TEXT(D3-D3*RAND()*0.1,"0")</f>
-        <v>348</v>
+        <v>210</v>
       </c>
       <c r="F3" t="str">
         <f t="shared" si="2"/>
@@ -1709,23 +1737,23 @@
       </c>
       <c r="I3" s="2" t="str">
         <f t="shared" ref="I3:I18" ca="1" si="9">TEXT(RAND()+0.1-0.2,"0.0")</f>
-        <v>0.7</v>
+        <v>0.4</v>
       </c>
       <c r="J3">
         <f t="shared" ca="1" si="4"/>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="K3">
         <f t="shared" ca="1" si="4"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L3" s="2">
         <f t="shared" ref="L3:L18" ca="1" si="10">ABS(TEXT(RAND()+0.1-0.2,"0.0"))</f>
-        <v>0.5</v>
+        <v>0.9</v>
       </c>
       <c r="M3">
         <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N3">
         <v>1</v>
@@ -1740,7 +1768,7 @@
       </c>
       <c r="R3" t="str">
         <f t="shared" ref="R3:R18" ca="1" si="12">"INSERT INTO [dbo].[food] ([name] ,[description] ,[price] ,[price_promo] ,[thumb] ,[img] ,[unit] ,[percent_promo] ,[rating] ,[sold] ,[point] ,[type] ,[status] ,[username] ,[modified]) VALUES ('"&amp;B3&amp;"' ,'"&amp;C3&amp;"' ,"&amp;D3&amp;" ,"&amp;E3&amp;",' "&amp;F3&amp;"','"&amp;G3&amp;"' ,'"&amp;H3&amp;"' ,"&amp;I3&amp;" ,"&amp;J3&amp;","&amp;K3&amp;","&amp;L3&amp;" ,"&amp;M3&amp;","&amp;N3&amp;",'"&amp;O3&amp;"','"&amp;P3&amp;"')"</f>
-        <v>INSERT INTO [dbo].[food] ([name] ,[description] ,[price] ,[price_promo] ,[thumb] ,[img] ,[unit] ,[percent_promo] ,[rating] ,[sold] ,[point] ,[type] ,[status] ,[username] ,[modified]) VALUES ('Tomatoe' ,'Description Tomatoe' ,376 ,348,' product-2.jpg','product-2.jpg' ,'gam' ,0.7 ,10,3,0.5 ,2,1,'khuong','12/26/2019')</v>
+        <v>INSERT INTO [dbo].[food] ([name] ,[description] ,[price] ,[price_promo] ,[thumb] ,[img] ,[unit] ,[percent_promo] ,[rating] ,[sold] ,[point] ,[type] ,[status] ,[username] ,[modified]) VALUES ('Tomatoe' ,'Description Tomatoe' ,214 ,210,' product-2.jpg','product-2.jpg' ,'gam' ,0.4 ,7,2,0.9 ,4,1,'khuong','12/26/2019')</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
@@ -1749,19 +1777,19 @@
       </c>
       <c r="B4" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Tomatoe</v>
+        <v>Bell Perpper</v>
       </c>
       <c r="C4" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Description Tomatoe</v>
+        <v>Description Bell Perpper</v>
       </c>
       <c r="D4" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>104</v>
+        <v>297</v>
       </c>
       <c r="E4" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>95</v>
+        <v>283</v>
       </c>
       <c r="F4" t="str">
         <f t="shared" si="2"/>
@@ -1776,23 +1804,23 @@
       </c>
       <c r="I4" s="2" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>0.3</v>
+        <v>0.6</v>
       </c>
       <c r="J4">
         <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K4">
         <f t="shared" ca="1" si="4"/>
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="L4" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>0.4</v>
+        <v>0.7</v>
       </c>
       <c r="M4">
         <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N4">
         <v>1</v>
@@ -1807,7 +1835,7 @@
       </c>
       <c r="R4" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>INSERT INTO [dbo].[food] ([name] ,[description] ,[price] ,[price_promo] ,[thumb] ,[img] ,[unit] ,[percent_promo] ,[rating] ,[sold] ,[point] ,[type] ,[status] ,[username] ,[modified]) VALUES ('Tomatoe' ,'Description Tomatoe' ,104 ,95,' product-3.jpg','product-3.jpg' ,'gam' ,0.3 ,2,4,0.4 ,2,1,'khuong','12/26/2019')</v>
+        <v>INSERT INTO [dbo].[food] ([name] ,[description] ,[price] ,[price_promo] ,[thumb] ,[img] ,[unit] ,[percent_promo] ,[rating] ,[sold] ,[point] ,[type] ,[status] ,[username] ,[modified]) VALUES ('Bell Perpper' ,'Description Bell Perpper' ,297 ,283,' product-3.jpg','product-3.jpg' ,'gam' ,0.6 ,1,10,0.7 ,4,1,'khuong','12/26/2019')</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
@@ -1824,11 +1852,11 @@
       </c>
       <c r="D5" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>918</v>
+        <v>989</v>
       </c>
       <c r="E5" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>843</v>
+        <v>979</v>
       </c>
       <c r="F5" t="str">
         <f t="shared" si="2"/>
@@ -1843,23 +1871,23 @@
       </c>
       <c r="I5" s="2" t="str">
         <f ca="1">TEXT(RAND()+0.1-0.2,"0.0")</f>
-        <v>0.6</v>
+        <v>0.3</v>
       </c>
       <c r="J5">
         <f t="shared" ca="1" si="4"/>
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="K5">
         <f t="shared" ca="1" si="4"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="L5" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>0.4</v>
+        <v>0.7</v>
       </c>
       <c r="M5">
         <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N5">
         <v>1</v>
@@ -1874,7 +1902,7 @@
       </c>
       <c r="R5" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>INSERT INTO [dbo].[food] ([name] ,[description] ,[price] ,[price_promo] ,[thumb] ,[img] ,[unit] ,[percent_promo] ,[rating] ,[sold] ,[point] ,[type] ,[status] ,[username] ,[modified]) VALUES ('Stawberry' ,'Description Stawberry' ,918 ,843,' product-4.jpg','product-4.jpg' ,'gam' ,0.6 ,9,3,0.4 ,2,1,'khuong','12/26/2019')</v>
+        <v>INSERT INTO [dbo].[food] ([name] ,[description] ,[price] ,[price_promo] ,[thumb] ,[img] ,[unit] ,[percent_promo] ,[rating] ,[sold] ,[point] ,[type] ,[status] ,[username] ,[modified]) VALUES ('Stawberry' ,'Description Stawberry' ,989 ,979,' product-4.jpg','product-4.jpg' ,'gam' ,0.3 ,2,5,0.7 ,1,1,'khuong','12/26/2019')</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
@@ -1883,19 +1911,19 @@
       </c>
       <c r="B6" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Bell Perpper</v>
+        <v>Tomatoe</v>
       </c>
       <c r="C6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Description Bell Perpper</v>
+        <v>Description Tomatoe</v>
       </c>
       <c r="D6" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>106</v>
+        <v>774</v>
       </c>
       <c r="E6" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>101</v>
+        <v>701</v>
       </c>
       <c r="F6" t="str">
         <f t="shared" si="2"/>
@@ -1910,23 +1938,23 @@
       </c>
       <c r="I6" s="2" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>0.2</v>
+        <v>0.0</v>
       </c>
       <c r="J6">
         <f t="shared" ca="1" si="4"/>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="K6">
         <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="L6" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="M6">
         <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N6">
         <v>1</v>
@@ -1941,7 +1969,7 @@
       </c>
       <c r="R6" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>INSERT INTO [dbo].[food] ([name] ,[description] ,[price] ,[price_promo] ,[thumb] ,[img] ,[unit] ,[percent_promo] ,[rating] ,[sold] ,[point] ,[type] ,[status] ,[username] ,[modified]) VALUES ('Bell Perpper' ,'Description Bell Perpper' ,106 ,101,' product-5.jpg','product-5.jpg' ,'gam' ,0.2 ,8,2,0.1 ,2,1,'khuong','12/26/2019')</v>
+        <v>INSERT INTO [dbo].[food] ([name] ,[description] ,[price] ,[price_promo] ,[thumb] ,[img] ,[unit] ,[percent_promo] ,[rating] ,[sold] ,[point] ,[type] ,[status] ,[username] ,[modified]) VALUES ('Tomatoe' ,'Description Tomatoe' ,774 ,701,' product-5.jpg','product-5.jpg' ,'gam' ,0.0 ,6,5,0.2 ,4,1,'khuong','12/26/2019')</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
@@ -1950,19 +1978,19 @@
       </c>
       <c r="B7" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Tomatoe</v>
+        <v>Bell Perpper</v>
       </c>
       <c r="C7" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Description Tomatoe</v>
+        <v>Description Bell Perpper</v>
       </c>
       <c r="D7" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>847</v>
+        <v>479</v>
       </c>
       <c r="E7" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>830</v>
+        <v>470</v>
       </c>
       <c r="F7" t="str">
         <f t="shared" si="2"/>
@@ -1977,23 +2005,23 @@
       </c>
       <c r="I7" s="2" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="J7">
         <f t="shared" ca="1" si="4"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="K7">
         <f t="shared" ca="1" si="4"/>
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="L7" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>0.3</v>
+        <v>0.8</v>
       </c>
       <c r="M7">
         <f t="shared" ca="1" si="5"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N7">
         <v>1</v>
@@ -2008,7 +2036,7 @@
       </c>
       <c r="R7" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>INSERT INTO [dbo].[food] ([name] ,[description] ,[price] ,[price_promo] ,[thumb] ,[img] ,[unit] ,[percent_promo] ,[rating] ,[sold] ,[point] ,[type] ,[status] ,[username] ,[modified]) VALUES ('Tomatoe' ,'Description Tomatoe' ,847 ,830,' product-6.jpg','product-6.jpg' ,'gam' ,0.4 ,6,10,0.3 ,4,1,'khuong','12/26/2019')</v>
+        <v>INSERT INTO [dbo].[food] ([name] ,[description] ,[price] ,[price_promo] ,[thumb] ,[img] ,[unit] ,[percent_promo] ,[rating] ,[sold] ,[point] ,[type] ,[status] ,[username] ,[modified]) VALUES ('Bell Perpper' ,'Description Bell Perpper' ,479 ,470,' product-6.jpg','product-6.jpg' ,'gam' ,0.5 ,4,2,0.8 ,3,1,'khuong','12/26/2019')</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
@@ -2017,19 +2045,19 @@
       </c>
       <c r="B8" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Bell Perpper</v>
+        <v>Tomatoe</v>
       </c>
       <c r="C8" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Description Bell Perpper</v>
+        <v>Description Tomatoe</v>
       </c>
       <c r="D8" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>899</v>
+        <v>281</v>
       </c>
       <c r="E8" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>816</v>
+        <v>258</v>
       </c>
       <c r="F8" t="str">
         <f t="shared" si="2"/>
@@ -2044,19 +2072,19 @@
       </c>
       <c r="I8" s="2" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>0.7</v>
+        <v>0.4</v>
       </c>
       <c r="J8">
         <f t="shared" ca="1" si="4"/>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="K8">
         <f t="shared" ca="1" si="4"/>
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="L8" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="M8">
         <f t="shared" ca="1" si="5"/>
@@ -2075,7 +2103,7 @@
       </c>
       <c r="R8" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>INSERT INTO [dbo].[food] ([name] ,[description] ,[price] ,[price_promo] ,[thumb] ,[img] ,[unit] ,[percent_promo] ,[rating] ,[sold] ,[point] ,[type] ,[status] ,[username] ,[modified]) VALUES ('Bell Perpper' ,'Description Bell Perpper' ,899 ,816,' product-7.jpg','product-7.jpg' ,'gam' ,0.7 ,3,10,0.5 ,2,1,'khuong','12/26/2019')</v>
+        <v>INSERT INTO [dbo].[food] ([name] ,[description] ,[price] ,[price_promo] ,[thumb] ,[img] ,[unit] ,[percent_promo] ,[rating] ,[sold] ,[point] ,[type] ,[status] ,[username] ,[modified]) VALUES ('Tomatoe' ,'Description Tomatoe' ,281 ,258,' product-7.jpg','product-7.jpg' ,'gam' ,0.4 ,9,7,0.2 ,2,1,'khuong','12/26/2019')</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
@@ -2092,11 +2120,11 @@
       </c>
       <c r="D9" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>906</v>
+        <v>665</v>
       </c>
       <c r="E9" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>847</v>
+        <v>657</v>
       </c>
       <c r="F9" t="str">
         <f t="shared" si="2"/>
@@ -2111,7 +2139,7 @@
       </c>
       <c r="I9" s="2" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="J9">
         <f t="shared" ca="1" si="4"/>
@@ -2119,15 +2147,15 @@
       </c>
       <c r="K9">
         <f t="shared" ca="1" si="4"/>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="L9" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="M9">
         <f t="shared" ca="1" si="5"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N9">
         <v>1</v>
@@ -2142,7 +2170,7 @@
       </c>
       <c r="R9" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>INSERT INTO [dbo].[food] ([name] ,[description] ,[price] ,[price_promo] ,[thumb] ,[img] ,[unit] ,[percent_promo] ,[rating] ,[sold] ,[point] ,[type] ,[status] ,[username] ,[modified]) VALUES ('Tomatoe' ,'Description Tomatoe' ,906 ,847,' product-8.jpg','product-8.jpg' ,'gam' ,0.2 ,10,3,0.8 ,3,1,'khuong','12/26/2019')</v>
+        <v>INSERT INTO [dbo].[food] ([name] ,[description] ,[price] ,[price_promo] ,[thumb] ,[img] ,[unit] ,[percent_promo] ,[rating] ,[sold] ,[point] ,[type] ,[status] ,[username] ,[modified]) VALUES ('Tomatoe' ,'Description Tomatoe' ,665 ,657,' product-8.jpg','product-8.jpg' ,'gam' ,0.5 ,10,9,0.7 ,4,1,'khuong','12/26/2019')</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
@@ -2151,19 +2179,19 @@
       </c>
       <c r="B10" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Bell Perpper</v>
+        <v>Tomatoe</v>
       </c>
       <c r="C10" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Description Bell Perpper</v>
+        <v>Description Tomatoe</v>
       </c>
       <c r="D10" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>85</v>
+        <v>366</v>
       </c>
       <c r="E10" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>81</v>
+        <v>363</v>
       </c>
       <c r="F10" t="str">
         <f t="shared" si="2"/>
@@ -2178,23 +2206,23 @@
       </c>
       <c r="I10" s="2" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>0.3</v>
+        <v>0.0</v>
       </c>
       <c r="J10">
         <f t="shared" ca="1" si="4"/>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="K10">
         <f t="shared" ca="1" si="4"/>
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="L10" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
       <c r="M10">
         <f t="shared" ca="1" si="5"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N10">
         <v>1</v>
@@ -2209,7 +2237,7 @@
       </c>
       <c r="R10" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>INSERT INTO [dbo].[food] ([name] ,[description] ,[price] ,[price_promo] ,[thumb] ,[img] ,[unit] ,[percent_promo] ,[rating] ,[sold] ,[point] ,[type] ,[status] ,[username] ,[modified]) VALUES ('Bell Perpper' ,'Description Bell Perpper' ,85 ,81,' product-9.jpg','product-9.jpg' ,'gam' ,0.3 ,6,10,0.3 ,3,1,'khuong','12/26/2019')</v>
+        <v>INSERT INTO [dbo].[food] ([name] ,[description] ,[price] ,[price_promo] ,[thumb] ,[img] ,[unit] ,[percent_promo] ,[rating] ,[sold] ,[point] ,[type] ,[status] ,[username] ,[modified]) VALUES ('Tomatoe' ,'Description Tomatoe' ,366 ,363,' product-9.jpg','product-9.jpg' ,'gam' ,0.0 ,1,6,0.1 ,4,1,'khuong','12/26/2019')</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
@@ -2218,19 +2246,19 @@
       </c>
       <c r="B11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Stawberry</v>
+        <v>Bell Perpper</v>
       </c>
       <c r="C11" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Description Stawberry</v>
+        <v>Description Bell Perpper</v>
       </c>
       <c r="D11" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>768</v>
+        <v>132</v>
       </c>
       <c r="E11" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>751</v>
+        <v>125</v>
       </c>
       <c r="F11" t="str">
         <f t="shared" si="2"/>
@@ -2245,23 +2273,23 @@
       </c>
       <c r="I11" s="2" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>0.0</v>
+        <v>0.3</v>
       </c>
       <c r="J11">
         <f t="shared" ca="1" si="4"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="K11">
         <f t="shared" ca="1" si="4"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="L11" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="M11">
         <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N11">
         <v>1</v>
@@ -2276,7 +2304,7 @@
       </c>
       <c r="R11" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>INSERT INTO [dbo].[food] ([name] ,[description] ,[price] ,[price_promo] ,[thumb] ,[img] ,[unit] ,[percent_promo] ,[rating] ,[sold] ,[point] ,[type] ,[status] ,[username] ,[modified]) VALUES ('Stawberry' ,'Description Stawberry' ,768 ,751,' product-10.jpg','product-10.jpg' ,'gam' ,0.0 ,5,8,0.1 ,2,1,'khuong','12/26/2019')</v>
+        <v>INSERT INTO [dbo].[food] ([name] ,[description] ,[price] ,[price_promo] ,[thumb] ,[img] ,[unit] ,[percent_promo] ,[rating] ,[sold] ,[point] ,[type] ,[status] ,[username] ,[modified]) VALUES ('Bell Perpper' ,'Description Bell Perpper' ,132 ,125,' product-10.jpg','product-10.jpg' ,'gam' ,0.3 ,3,10,0 ,3,1,'khuong','12/26/2019')</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
@@ -2285,19 +2313,19 @@
       </c>
       <c r="B12" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Green Beans</v>
+        <v>Bell Perpper</v>
       </c>
       <c r="C12" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Description Green Beans</v>
+        <v>Description Bell Perpper</v>
       </c>
       <c r="D12" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>39</v>
+        <v>880</v>
       </c>
       <c r="E12" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>39</v>
+        <v>818</v>
       </c>
       <c r="F12" t="str">
         <f t="shared" si="2"/>
@@ -2312,19 +2340,19 @@
       </c>
       <c r="I12" s="2" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="J12">
         <f t="shared" ca="1" si="4"/>
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="K12">
         <f t="shared" ca="1" si="4"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="L12" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>0.9</v>
+        <v>0.1</v>
       </c>
       <c r="M12">
         <f t="shared" ca="1" si="5"/>
@@ -2343,7 +2371,7 @@
       </c>
       <c r="R12" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>INSERT INTO [dbo].[food] ([name] ,[description] ,[price] ,[price_promo] ,[thumb] ,[img] ,[unit] ,[percent_promo] ,[rating] ,[sold] ,[point] ,[type] ,[status] ,[username] ,[modified]) VALUES ('Green Beans' ,'Description Green Beans' ,39 ,39,' product-11.jpg','product-11.jpg' ,'gam' ,0.6 ,3,5,0.9 ,4,1,'khuong','12/26/2019')</v>
+        <v>INSERT INTO [dbo].[food] ([name] ,[description] ,[price] ,[price_promo] ,[thumb] ,[img] ,[unit] ,[percent_promo] ,[rating] ,[sold] ,[point] ,[type] ,[status] ,[username] ,[modified]) VALUES ('Bell Perpper' ,'Description Bell Perpper' ,880 ,818,' product-11.jpg','product-11.jpg' ,'gam' ,0.4 ,10,7,0.1 ,4,1,'khuong','12/26/2019')</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
@@ -2352,19 +2380,19 @@
       </c>
       <c r="B13" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Tomatoe</v>
+        <v>Green Beans</v>
       </c>
       <c r="C13" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Description Tomatoe</v>
+        <v>Description Green Beans</v>
       </c>
       <c r="D13" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>171</v>
+        <v>619</v>
       </c>
       <c r="E13" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>166</v>
+        <v>575</v>
       </c>
       <c r="F13" t="str">
         <f t="shared" si="2"/>
@@ -2379,23 +2407,23 @@
       </c>
       <c r="I13" s="2" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>0.8</v>
+        <v>0.1</v>
       </c>
       <c r="J13">
         <f t="shared" ca="1" si="4"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="K13">
         <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="L13" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>0.9</v>
+        <v>0.3</v>
       </c>
       <c r="M13">
         <f t="shared" ca="1" si="5"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="N13">
         <v>1</v>
@@ -2410,7 +2438,7 @@
       </c>
       <c r="R13" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>INSERT INTO [dbo].[food] ([name] ,[description] ,[price] ,[price_promo] ,[thumb] ,[img] ,[unit] ,[percent_promo] ,[rating] ,[sold] ,[point] ,[type] ,[status] ,[username] ,[modified]) VALUES ('Tomatoe' ,'Description Tomatoe' ,171 ,166,' product-12.jpg','product-12.jpg' ,'gam' ,0.8 ,9,1,0.9 ,1,1,'khuong','12/26/2019')</v>
+        <v>INSERT INTO [dbo].[food] ([name] ,[description] ,[price] ,[price_promo] ,[thumb] ,[img] ,[unit] ,[percent_promo] ,[rating] ,[sold] ,[point] ,[type] ,[status] ,[username] ,[modified]) VALUES ('Green Beans' ,'Description Green Beans' ,619 ,575,' product-12.jpg','product-12.jpg' ,'gam' ,0.1 ,8,5,0.3 ,4,1,'khuong','12/26/2019')</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
@@ -2419,19 +2447,19 @@
       </c>
       <c r="B14" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Bell Perpper</v>
+        <v>Tomatoe</v>
       </c>
       <c r="C14" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Description Bell Perpper</v>
+        <v>Description Tomatoe</v>
       </c>
       <c r="D14" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>599</v>
+        <v>9</v>
       </c>
       <c r="E14" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>554</v>
+        <v>8</v>
       </c>
       <c r="F14" t="str">
         <f t="shared" si="2"/>
@@ -2446,23 +2474,23 @@
       </c>
       <c r="I14" s="2" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>0.0</v>
+        <v>0.5</v>
       </c>
       <c r="J14">
         <f t="shared" ca="1" si="4"/>
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="K14">
         <f t="shared" ca="1" si="4"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="L14" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="M14">
         <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N14">
         <v>1</v>
@@ -2477,7 +2505,7 @@
       </c>
       <c r="R14" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>INSERT INTO [dbo].[food] ([name] ,[description] ,[price] ,[price_promo] ,[thumb] ,[img] ,[unit] ,[percent_promo] ,[rating] ,[sold] ,[point] ,[type] ,[status] ,[username] ,[modified]) VALUES ('Bell Perpper' ,'Description Bell Perpper' ,599 ,554,' product-13.jpg','product-13.jpg' ,'gam' ,0.0 ,9,6,0.2 ,2,1,'khuong','12/26/2019')</v>
+        <v>INSERT INTO [dbo].[food] ([name] ,[description] ,[price] ,[price_promo] ,[thumb] ,[img] ,[unit] ,[percent_promo] ,[rating] ,[sold] ,[point] ,[type] ,[status] ,[username] ,[modified]) VALUES ('Tomatoe' ,'Description Tomatoe' ,9 ,8,' product-13.jpg','product-13.jpg' ,'gam' ,0.5 ,3,8,0.5 ,1,1,'khuong','12/26/2019')</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
@@ -2494,11 +2522,11 @@
       </c>
       <c r="D15" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>819</v>
+        <v>577</v>
       </c>
       <c r="E15" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>768</v>
+        <v>524</v>
       </c>
       <c r="F15" t="str">
         <f t="shared" si="2"/>
@@ -2513,19 +2541,19 @@
       </c>
       <c r="I15" s="2" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>0.7</v>
+        <v>0.0</v>
       </c>
       <c r="J15">
         <f t="shared" ca="1" si="4"/>
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="K15">
         <f t="shared" ca="1" si="4"/>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="L15" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
       <c r="M15">
         <f t="shared" ca="1" si="5"/>
@@ -2544,7 +2572,7 @@
       </c>
       <c r="R15" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>INSERT INTO [dbo].[food] ([name] ,[description] ,[price] ,[price_promo] ,[thumb] ,[img] ,[unit] ,[percent_promo] ,[rating] ,[sold] ,[point] ,[type] ,[status] ,[username] ,[modified]) VALUES ('Tomatoe' ,'Description Tomatoe' ,819 ,768,' product-14.jpg','product-14.jpg' ,'gam' ,0.7 ,10,4,0.4 ,3,1,'khuong','12/26/2019')</v>
+        <v>INSERT INTO [dbo].[food] ([name] ,[description] ,[price] ,[price_promo] ,[thumb] ,[img] ,[unit] ,[percent_promo] ,[rating] ,[sold] ,[point] ,[type] ,[status] ,[username] ,[modified]) VALUES ('Tomatoe' ,'Description Tomatoe' ,577 ,524,' product-14.jpg','product-14.jpg' ,'gam' ,0.0 ,4,7,0.3 ,3,1,'khuong','12/26/2019')</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
@@ -2553,19 +2581,19 @@
       </c>
       <c r="B16" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Tomatoe</v>
+        <v>Stawberry</v>
       </c>
       <c r="C16" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Description Tomatoe</v>
+        <v>Description Stawberry</v>
       </c>
       <c r="D16" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>829</v>
+        <v>809</v>
       </c>
       <c r="E16" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>817</v>
+        <v>760</v>
       </c>
       <c r="F16" t="str">
         <f t="shared" si="2"/>
@@ -2580,23 +2608,23 @@
       </c>
       <c r="I16" s="2" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="J16">
         <f t="shared" ca="1" si="4"/>
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="K16">
         <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="L16" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="M16">
         <f t="shared" ca="1" si="5"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N16">
         <v>1</v>
@@ -2611,7 +2639,7 @@
       </c>
       <c r="R16" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>INSERT INTO [dbo].[food] ([name] ,[description] ,[price] ,[price_promo] ,[thumb] ,[img] ,[unit] ,[percent_promo] ,[rating] ,[sold] ,[point] ,[type] ,[status] ,[username] ,[modified]) VALUES ('Tomatoe' ,'Description Tomatoe' ,829 ,817,' product-15.jpg','product-15.jpg' ,'gam' ,0.1 ,8,2,0.1 ,1,1,'khuong','12/26/2019')</v>
+        <v>INSERT INTO [dbo].[food] ([name] ,[description] ,[price] ,[price_promo] ,[thumb] ,[img] ,[unit] ,[percent_promo] ,[rating] ,[sold] ,[point] ,[type] ,[status] ,[username] ,[modified]) VALUES ('Stawberry' ,'Description Stawberry' ,809 ,760,' product-15.jpg','product-15.jpg' ,'gam' ,0.5 ,3,8,0 ,2,1,'khuong','12/26/2019')</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
@@ -2620,19 +2648,19 @@
       </c>
       <c r="B17" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Tomatoe</v>
+        <v>Bell Perpper</v>
       </c>
       <c r="C17" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Description Tomatoe</v>
+        <v>Description Bell Perpper</v>
       </c>
       <c r="D17" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>305</v>
+        <v>461</v>
       </c>
       <c r="E17" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>291</v>
+        <v>447</v>
       </c>
       <c r="F17" t="str">
         <f t="shared" si="2"/>
@@ -2647,23 +2675,23 @@
       </c>
       <c r="I17" s="2" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>0.7</v>
+        <v>0.0</v>
       </c>
       <c r="J17">
         <f t="shared" ca="1" si="4"/>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="K17">
         <f t="shared" ca="1" si="4"/>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="L17" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>0.1</v>
+        <v>0.9</v>
       </c>
       <c r="M17">
         <f t="shared" ca="1" si="5"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N17">
         <v>1</v>
@@ -2678,7 +2706,7 @@
       </c>
       <c r="R17" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>INSERT INTO [dbo].[food] ([name] ,[description] ,[price] ,[price_promo] ,[thumb] ,[img] ,[unit] ,[percent_promo] ,[rating] ,[sold] ,[point] ,[type] ,[status] ,[username] ,[modified]) VALUES ('Tomatoe' ,'Description Tomatoe' ,305 ,291,' product-16.jpg','product-16.jpg' ,'gam' ,0.7 ,9,10,0.1 ,3,1,'khuong','12/26/2019')</v>
+        <v>INSERT INTO [dbo].[food] ([name] ,[description] ,[price] ,[price_promo] ,[thumb] ,[img] ,[unit] ,[percent_promo] ,[rating] ,[sold] ,[point] ,[type] ,[status] ,[username] ,[modified]) VALUES ('Bell Perpper' ,'Description Bell Perpper' ,461 ,447,' product-16.jpg','product-16.jpg' ,'gam' ,0.0 ,7,5,0.9 ,4,1,'khuong','12/26/2019')</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
@@ -2687,19 +2715,19 @@
       </c>
       <c r="B18" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Green Beans</v>
+        <v>Bell Perpper</v>
       </c>
       <c r="C18" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Description Green Beans</v>
+        <v>Description Bell Perpper</v>
       </c>
       <c r="D18" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>194</v>
+        <v>26</v>
       </c>
       <c r="E18" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>186</v>
+        <v>25</v>
       </c>
       <c r="F18" t="str">
         <f t="shared" si="2"/>
@@ -2714,19 +2742,19 @@
       </c>
       <c r="I18" s="2" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>0.0</v>
+        <v>0.8</v>
       </c>
       <c r="J18">
         <f t="shared" ca="1" si="4"/>
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="K18">
         <f t="shared" ca="1" si="4"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="L18" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>0.1</v>
+        <v>0.8</v>
       </c>
       <c r="M18">
         <f t="shared" ca="1" si="5"/>
@@ -2745,7 +2773,7 @@
       </c>
       <c r="R18" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>INSERT INTO [dbo].[food] ([name] ,[description] ,[price] ,[price_promo] ,[thumb] ,[img] ,[unit] ,[percent_promo] ,[rating] ,[sold] ,[point] ,[type] ,[status] ,[username] ,[modified]) VALUES ('Green Beans' ,'Description Green Beans' ,194 ,186,' product-17.jpg','product-17.jpg' ,'gam' ,0.0 ,4,6,0.1 ,2,1,'khuong','12/26/2019')</v>
+        <v>INSERT INTO [dbo].[food] ([name] ,[description] ,[price] ,[price_promo] ,[thumb] ,[img] ,[unit] ,[percent_promo] ,[rating] ,[sold] ,[point] ,[type] ,[status] ,[username] ,[modified]) VALUES ('Bell Perpper' ,'Description Bell Perpper' ,26 ,25,' product-17.jpg','product-17.jpg' ,'gam' ,0.8 ,10,3,0.8 ,2,1,'khuong','12/26/2019')</v>
       </c>
     </row>
   </sheetData>
@@ -2824,7 +2852,7 @@
       </c>
       <c r="I2" s="3">
         <f ca="1">NOW()</f>
-        <v>43825.10472210648</v>
+        <v>43825.461475578704</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -2855,7 +2883,7 @@
       </c>
       <c r="I3" s="3">
         <f t="shared" ref="I3:I5" ca="1" si="1">NOW()</f>
-        <v>43825.10472210648</v>
+        <v>43825.461475578704</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -2886,7 +2914,7 @@
       </c>
       <c r="I4" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>43825.10472210648</v>
+        <v>43825.461475578704</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -2917,7 +2945,7 @@
       </c>
       <c r="I5" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>43825.10472210648</v>
+        <v>43825.461475578704</v>
       </c>
     </row>
   </sheetData>
@@ -3004,11 +3032,11 @@
       </c>
       <c r="I2" s="3">
         <f ca="1">NOW()</f>
-        <v>43825.10472210648</v>
+        <v>43825.461475578704</v>
       </c>
       <c r="J2" s="3">
         <f ca="1">NOW()</f>
-        <v>43825.10472210648</v>
+        <v>43825.461475578704</v>
       </c>
       <c r="L2" t="str">
         <f ca="1">"UPDATE [dbo].[post] SET [type] = '"&amp;E2&amp;"' WHERE post_id="&amp;A2</f>
@@ -3044,11 +3072,11 @@
       </c>
       <c r="I3" s="3">
         <f t="shared" ref="I3:J31" ca="1" si="2">NOW()</f>
-        <v>43825.10472210648</v>
+        <v>43825.461475578704</v>
       </c>
       <c r="J3" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.10472210648</v>
+        <v>43825.461475578704</v>
       </c>
       <c r="L3" t="str">
         <f t="shared" ref="L3:L31" ca="1" si="3">"UPDATE [dbo].[post] SET [type] = '"&amp;E3&amp;"' WHERE post_id="&amp;A3</f>
@@ -3070,7 +3098,7 @@
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F4" t="str">
         <f t="shared" si="0"/>
@@ -3084,15 +3112,15 @@
       </c>
       <c r="I4" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.10472210648</v>
+        <v>43825.461475578704</v>
       </c>
       <c r="J4" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.10472210648</v>
+        <v>43825.461475578704</v>
       </c>
       <c r="L4" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>UPDATE [dbo].[post] SET [type] = '1' WHERE post_id=3</v>
+        <v>UPDATE [dbo].[post] SET [type] = '3' WHERE post_id=3</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -3110,7 +3138,7 @@
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F5" t="str">
         <f t="shared" si="0"/>
@@ -3124,15 +3152,15 @@
       </c>
       <c r="I5" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.10472210648</v>
+        <v>43825.461475578704</v>
       </c>
       <c r="J5" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.10472210648</v>
+        <v>43825.461475578704</v>
       </c>
       <c r="L5" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>UPDATE [dbo].[post] SET [type] = '1' WHERE post_id=4</v>
+        <v>UPDATE [dbo].[post] SET [type] = '2' WHERE post_id=4</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -3150,7 +3178,7 @@
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F6" t="str">
         <f t="shared" si="0"/>
@@ -3164,15 +3192,15 @@
       </c>
       <c r="I6" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.10472210648</v>
+        <v>43825.461475578704</v>
       </c>
       <c r="J6" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.10472210648</v>
+        <v>43825.461475578704</v>
       </c>
       <c r="L6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>UPDATE [dbo].[post] SET [type] = '2' WHERE post_id=5</v>
+        <v>UPDATE [dbo].[post] SET [type] = '1' WHERE post_id=5</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -3204,11 +3232,11 @@
       </c>
       <c r="I7" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.10472210648</v>
+        <v>43825.461475578704</v>
       </c>
       <c r="J7" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.10472210648</v>
+        <v>43825.461475578704</v>
       </c>
       <c r="L7" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -3230,7 +3258,7 @@
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F8" t="str">
         <f t="shared" si="0"/>
@@ -3244,15 +3272,15 @@
       </c>
       <c r="I8" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.10472210648</v>
+        <v>43825.461475578704</v>
       </c>
       <c r="J8" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.10472210648</v>
+        <v>43825.461475578704</v>
       </c>
       <c r="L8" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>UPDATE [dbo].[post] SET [type] = '1' WHERE post_id=7</v>
+        <v>UPDATE [dbo].[post] SET [type] = '2' WHERE post_id=7</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -3284,11 +3312,11 @@
       </c>
       <c r="I9" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.10472210648</v>
+        <v>43825.461475578704</v>
       </c>
       <c r="J9" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.10472210648</v>
+        <v>43825.461475578704</v>
       </c>
       <c r="L9" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -3310,7 +3338,7 @@
       </c>
       <c r="E10">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F10" t="str">
         <f t="shared" si="0"/>
@@ -3324,15 +3352,15 @@
       </c>
       <c r="I10" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.10472210648</v>
+        <v>43825.461475578704</v>
       </c>
       <c r="J10" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.10472210648</v>
+        <v>43825.461475578704</v>
       </c>
       <c r="L10" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>UPDATE [dbo].[post] SET [type] = '2' WHERE post_id=9</v>
+        <v>UPDATE [dbo].[post] SET [type] = '1' WHERE post_id=9</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -3350,7 +3378,7 @@
       </c>
       <c r="E11">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F11" t="str">
         <f t="shared" si="0"/>
@@ -3364,15 +3392,15 @@
       </c>
       <c r="I11" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.10472210648</v>
+        <v>43825.461475578704</v>
       </c>
       <c r="J11" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.10472210648</v>
+        <v>43825.461475578704</v>
       </c>
       <c r="L11" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>UPDATE [dbo].[post] SET [type] = '3' WHERE post_id=10</v>
+        <v>UPDATE [dbo].[post] SET [type] = '1' WHERE post_id=10</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -3390,7 +3418,7 @@
       </c>
       <c r="E12">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F12" t="str">
         <f t="shared" si="0"/>
@@ -3404,15 +3432,15 @@
       </c>
       <c r="I12" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.10472210648</v>
+        <v>43825.461475578704</v>
       </c>
       <c r="J12" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.10472210648</v>
+        <v>43825.461475578704</v>
       </c>
       <c r="L12" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>UPDATE [dbo].[post] SET [type] = '1' WHERE post_id=11</v>
+        <v>UPDATE [dbo].[post] SET [type] = '4' WHERE post_id=11</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -3444,11 +3472,11 @@
       </c>
       <c r="I13" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.10472210648</v>
+        <v>43825.461475578704</v>
       </c>
       <c r="J13" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.10472210648</v>
+        <v>43825.461475578704</v>
       </c>
       <c r="L13" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -3484,11 +3512,11 @@
       </c>
       <c r="I14" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.10472210648</v>
+        <v>43825.461475578704</v>
       </c>
       <c r="J14" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.10472210648</v>
+        <v>43825.461475578704</v>
       </c>
       <c r="L14" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -3510,7 +3538,7 @@
       </c>
       <c r="E15">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F15" t="str">
         <f t="shared" si="0"/>
@@ -3524,15 +3552,15 @@
       </c>
       <c r="I15" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.10472210648</v>
+        <v>43825.461475578704</v>
       </c>
       <c r="J15" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.10472210648</v>
+        <v>43825.461475578704</v>
       </c>
       <c r="L15" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>UPDATE [dbo].[post] SET [type] = '3' WHERE post_id=14</v>
+        <v>UPDATE [dbo].[post] SET [type] = '2' WHERE post_id=14</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -3550,7 +3578,7 @@
       </c>
       <c r="E16">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F16" t="str">
         <f t="shared" si="0"/>
@@ -3564,15 +3592,15 @@
       </c>
       <c r="I16" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.10472210648</v>
+        <v>43825.461475578704</v>
       </c>
       <c r="J16" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.10472210648</v>
+        <v>43825.461475578704</v>
       </c>
       <c r="L16" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>UPDATE [dbo].[post] SET [type] = '2' WHERE post_id=15</v>
+        <v>UPDATE [dbo].[post] SET [type] = '3' WHERE post_id=15</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -3590,7 +3618,7 @@
       </c>
       <c r="E17">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F17" t="str">
         <f t="shared" si="0"/>
@@ -3604,15 +3632,15 @@
       </c>
       <c r="I17" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.10472210648</v>
+        <v>43825.461475578704</v>
       </c>
       <c r="J17" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.10472210648</v>
+        <v>43825.461475578704</v>
       </c>
       <c r="L17" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>UPDATE [dbo].[post] SET [type] = '4' WHERE post_id=16</v>
+        <v>UPDATE [dbo].[post] SET [type] = '2' WHERE post_id=16</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -3644,11 +3672,11 @@
       </c>
       <c r="I18" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.10472210648</v>
+        <v>43825.461475578704</v>
       </c>
       <c r="J18" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.10472210648</v>
+        <v>43825.461475578704</v>
       </c>
       <c r="L18" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -3684,11 +3712,11 @@
       </c>
       <c r="I19" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.10472210648</v>
+        <v>43825.461475578704</v>
       </c>
       <c r="J19" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.10472210648</v>
+        <v>43825.461475578704</v>
       </c>
       <c r="L19" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -3710,7 +3738,7 @@
       </c>
       <c r="E20">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F20" t="str">
         <f t="shared" si="0"/>
@@ -3724,15 +3752,15 @@
       </c>
       <c r="I20" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.10472210648</v>
+        <v>43825.461475578704</v>
       </c>
       <c r="J20" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.10472210648</v>
+        <v>43825.461475578704</v>
       </c>
       <c r="L20" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>UPDATE [dbo].[post] SET [type] = '2' WHERE post_id=19</v>
+        <v>UPDATE [dbo].[post] SET [type] = '4' WHERE post_id=19</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -3764,11 +3792,11 @@
       </c>
       <c r="I21" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.10472210648</v>
+        <v>43825.461475578704</v>
       </c>
       <c r="J21" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.10472210648</v>
+        <v>43825.461475578704</v>
       </c>
       <c r="L21" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -3790,7 +3818,7 @@
       </c>
       <c r="E22">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F22" t="str">
         <f t="shared" si="0"/>
@@ -3804,15 +3832,15 @@
       </c>
       <c r="I22" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.10472210648</v>
+        <v>43825.461475578704</v>
       </c>
       <c r="J22" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.10472210648</v>
+        <v>43825.461475578704</v>
       </c>
       <c r="L22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>UPDATE [dbo].[post] SET [type] = '1' WHERE post_id=21</v>
+        <v>UPDATE [dbo].[post] SET [type] = '3' WHERE post_id=21</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
@@ -3830,7 +3858,7 @@
       </c>
       <c r="E23">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F23" t="str">
         <f t="shared" si="0"/>
@@ -3844,15 +3872,15 @@
       </c>
       <c r="I23" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.10472210648</v>
+        <v>43825.461475578704</v>
       </c>
       <c r="J23" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.10472210648</v>
+        <v>43825.461475578704</v>
       </c>
       <c r="L23" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>UPDATE [dbo].[post] SET [type] = '3' WHERE post_id=22</v>
+        <v>UPDATE [dbo].[post] SET [type] = '4' WHERE post_id=22</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
@@ -3870,7 +3898,7 @@
       </c>
       <c r="E24">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F24" t="str">
         <f t="shared" si="0"/>
@@ -3884,15 +3912,15 @@
       </c>
       <c r="I24" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.10472210648</v>
+        <v>43825.461475578704</v>
       </c>
       <c r="J24" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.10472210648</v>
+        <v>43825.461475578704</v>
       </c>
       <c r="L24" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>UPDATE [dbo].[post] SET [type] = '4' WHERE post_id=23</v>
+        <v>UPDATE [dbo].[post] SET [type] = '2' WHERE post_id=23</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
@@ -3924,11 +3952,11 @@
       </c>
       <c r="I25" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.10472210648</v>
+        <v>43825.461475578704</v>
       </c>
       <c r="J25" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.10472210648</v>
+        <v>43825.461475578704</v>
       </c>
       <c r="L25" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -3964,11 +3992,11 @@
       </c>
       <c r="I26" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.10472210648</v>
+        <v>43825.461475578704</v>
       </c>
       <c r="J26" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.10472210648</v>
+        <v>43825.461475578704</v>
       </c>
       <c r="L26" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -3990,7 +4018,7 @@
       </c>
       <c r="E27">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F27" t="str">
         <f t="shared" si="0"/>
@@ -4004,15 +4032,15 @@
       </c>
       <c r="I27" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.10472210648</v>
+        <v>43825.461475578704</v>
       </c>
       <c r="J27" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.10472210648</v>
+        <v>43825.461475578704</v>
       </c>
       <c r="L27" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>UPDATE [dbo].[post] SET [type] = '3' WHERE post_id=26</v>
+        <v>UPDATE [dbo].[post] SET [type] = '2' WHERE post_id=26</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
@@ -4044,11 +4072,11 @@
       </c>
       <c r="I28" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.10472210648</v>
+        <v>43825.461475578704</v>
       </c>
       <c r="J28" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.10472210648</v>
+        <v>43825.461475578704</v>
       </c>
       <c r="L28" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -4070,7 +4098,7 @@
       </c>
       <c r="E29">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F29" t="str">
         <f t="shared" si="0"/>
@@ -4084,15 +4112,15 @@
       </c>
       <c r="I29" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.10472210648</v>
+        <v>43825.461475578704</v>
       </c>
       <c r="J29" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.10472210648</v>
+        <v>43825.461475578704</v>
       </c>
       <c r="L29" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>UPDATE [dbo].[post] SET [type] = '1' WHERE post_id=28</v>
+        <v>UPDATE [dbo].[post] SET [type] = '4' WHERE post_id=28</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
@@ -4110,7 +4138,7 @@
       </c>
       <c r="E30">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F30" t="str">
         <f t="shared" si="0"/>
@@ -4124,15 +4152,15 @@
       </c>
       <c r="I30" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.10472210648</v>
+        <v>43825.461475578704</v>
       </c>
       <c r="J30" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.10472210648</v>
+        <v>43825.461475578704</v>
       </c>
       <c r="L30" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>UPDATE [dbo].[post] SET [type] = '1' WHERE post_id=29</v>
+        <v>UPDATE [dbo].[post] SET [type] = '4' WHERE post_id=29</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
@@ -4164,11 +4192,11 @@
       </c>
       <c r="I31" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.10472210648</v>
+        <v>43825.461475578704</v>
       </c>
       <c r="J31" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.10472210648</v>
+        <v>43825.461475578704</v>
       </c>
       <c r="L31" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -4230,7 +4258,7 @@
       </c>
       <c r="B3">
         <f t="shared" ref="B3:B18" ca="1" si="0">RANDBETWEEN(1,5)</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C3" t="str">
         <f t="shared" ref="C3:C18" si="1">"des "&amp;A3</f>
@@ -4250,7 +4278,7 @@
       </c>
       <c r="B4">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C4" t="str">
         <f t="shared" si="1"/>
@@ -4290,7 +4318,7 @@
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C6" t="str">
         <f t="shared" si="1"/>
@@ -4307,7 +4335,7 @@
       </c>
       <c r="B7">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C7" t="str">
         <f t="shared" si="1"/>
@@ -4341,7 +4369,7 @@
       </c>
       <c r="B9">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C9" t="str">
         <f t="shared" si="1"/>
@@ -4358,7 +4386,7 @@
       </c>
       <c r="B10">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C10" t="str">
         <f t="shared" si="1"/>
@@ -4375,7 +4403,7 @@
       </c>
       <c r="B11">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C11" t="str">
         <f t="shared" si="1"/>
@@ -4392,7 +4420,7 @@
       </c>
       <c r="B12">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C12" t="str">
         <f t="shared" si="1"/>
@@ -4409,7 +4437,7 @@
       </c>
       <c r="B13">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C13" t="str">
         <f t="shared" si="1"/>
@@ -4426,7 +4454,7 @@
       </c>
       <c r="B14">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C14" t="str">
         <f t="shared" si="1"/>
@@ -4460,7 +4488,7 @@
       </c>
       <c r="B16">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C16" t="str">
         <f t="shared" si="1"/>
@@ -4477,7 +4505,7 @@
       </c>
       <c r="B17">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C17" t="str">
         <f t="shared" si="1"/>
@@ -4494,7 +4522,7 @@
       </c>
       <c r="B18">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C18" t="str">
         <f t="shared" si="1"/>
@@ -4514,7 +4542,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
@@ -4529,23 +4557,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -4600,34 +4628,34 @@
         <f>"khuong "&amp;A3</f>
         <v>khuong 1</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="F3" s="8" t="str">
+      <c r="F3" s="7" t="str">
         <f>"yoshi@gmail.com"</f>
         <v>yoshi@gmail.com</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G3" s="6" t="s">
         <v>160</v>
       </c>
       <c r="H3">
         <f ca="1">RANDBETWEEN(1,5)</f>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I3">
         <f ca="1">RANDBETWEEN(1,5)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J3">
         <f ca="1">SUM(H3,I3)</f>
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="K3">
         <v>1</v>
       </c>
       <c r="L3" s="3">
         <f ca="1">NOW()</f>
-        <v>43825.10472210648</v>
+        <v>43825.461475578704</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
@@ -4645,34 +4673,34 @@
         <f t="shared" ref="D4:D18" si="1">"khuong "&amp;A4</f>
         <v>khuong 2</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="F4" s="8" t="str">
+      <c r="F4" s="7" t="str">
         <f t="shared" ref="F4:F18" si="2">"yoshi@gmail.com"</f>
         <v>yoshi@gmail.com</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="G4" s="6" t="s">
         <v>161</v>
       </c>
       <c r="H4">
         <f t="shared" ref="H4:I18" ca="1" si="3">RANDBETWEEN(1,5)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I4">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J4">
         <f t="shared" ref="J4:J18" ca="1" si="4">SUM(H4,I4)</f>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="K4">
         <v>1</v>
       </c>
       <c r="L4" s="3">
         <f t="shared" ref="L4:L18" ca="1" si="5">NOW()</f>
-        <v>43825.10472210648</v>
+        <v>43825.461475578704</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
@@ -4690,34 +4718,34 @@
         <f t="shared" si="1"/>
         <v>khuong 3</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="F5" s="8" t="str">
+      <c r="F5" s="7" t="str">
         <f t="shared" si="2"/>
         <v>yoshi@gmail.com</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="G5" s="6" t="s">
         <v>162</v>
       </c>
       <c r="H5">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I5">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J5">
         <f t="shared" ca="1" si="4"/>
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="K5">
         <v>1</v>
       </c>
       <c r="L5" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>43825.10472210648</v>
+        <v>43825.461475578704</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
@@ -4735,34 +4763,34 @@
         <f t="shared" si="1"/>
         <v>khuong 4</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="F6" s="8" t="str">
+      <c r="F6" s="7" t="str">
         <f t="shared" si="2"/>
         <v>yoshi@gmail.com</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="G6" s="6" t="s">
         <v>163</v>
       </c>
       <c r="H6">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I6">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="J6">
         <f t="shared" ca="1" si="4"/>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="K6">
         <v>1</v>
       </c>
       <c r="L6" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>43825.10472210648</v>
+        <v>43825.461475578704</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
@@ -4780,34 +4808,34 @@
         <f t="shared" si="1"/>
         <v>khuong 5</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="F7" s="8" t="str">
+      <c r="F7" s="7" t="str">
         <f t="shared" si="2"/>
         <v>yoshi@gmail.com</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="G7" s="6" t="s">
         <v>164</v>
       </c>
       <c r="H7">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I7">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J7">
         <f t="shared" ca="1" si="4"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="K7">
         <v>1</v>
       </c>
       <c r="L7" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>43825.10472210648</v>
+        <v>43825.461475578704</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
@@ -4825,19 +4853,19 @@
         <f t="shared" si="1"/>
         <v>khuong 6</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="F8" s="8" t="str">
+      <c r="F8" s="7" t="str">
         <f t="shared" si="2"/>
         <v>yoshi@gmail.com</v>
       </c>
-      <c r="G8" s="7" t="s">
+      <c r="G8" s="6" t="s">
         <v>165</v>
       </c>
       <c r="H8">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I8">
         <f t="shared" ca="1" si="3"/>
@@ -4845,14 +4873,14 @@
       </c>
       <c r="J8">
         <f t="shared" ca="1" si="4"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="K8">
         <v>1</v>
       </c>
       <c r="L8" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>43825.10472210648</v>
+        <v>43825.461475578704</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
@@ -4870,34 +4898,34 @@
         <f t="shared" si="1"/>
         <v>khuong 7</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="F9" s="8" t="str">
+      <c r="F9" s="7" t="str">
         <f t="shared" si="2"/>
         <v>yoshi@gmail.com</v>
       </c>
-      <c r="G9" s="7" t="s">
+      <c r="G9" s="6" t="s">
         <v>166</v>
       </c>
       <c r="H9">
         <f t="shared" ca="1" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="I9">
+        <f t="shared" ca="1" si="3"/>
         <v>2</v>
-      </c>
-      <c r="I9">
-        <f t="shared" ca="1" si="3"/>
-        <v>1</v>
       </c>
       <c r="J9">
         <f t="shared" ca="1" si="4"/>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="K9">
         <v>1</v>
       </c>
       <c r="L9" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>43825.10472210648</v>
+        <v>43825.461475578704</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
@@ -4915,19 +4943,19 @@
         <f t="shared" si="1"/>
         <v>khuong 8</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="E10" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="F10" s="8" t="str">
+      <c r="F10" s="7" t="str">
         <f t="shared" si="2"/>
         <v>yoshi@gmail.com</v>
       </c>
-      <c r="G10" s="7" t="s">
+      <c r="G10" s="6" t="s">
         <v>167</v>
       </c>
       <c r="H10">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I10">
         <f t="shared" ca="1" si="3"/>
@@ -4935,14 +4963,14 @@
       </c>
       <c r="J10">
         <f t="shared" ca="1" si="4"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K10">
         <v>1</v>
       </c>
       <c r="L10" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>43825.10472210648</v>
+        <v>43825.461475578704</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
@@ -4960,19 +4988,19 @@
         <f t="shared" si="1"/>
         <v>khuong 9</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="E11" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="F11" s="8" t="str">
+      <c r="F11" s="7" t="str">
         <f t="shared" si="2"/>
         <v>yoshi@gmail.com</v>
       </c>
-      <c r="G11" s="7" t="s">
+      <c r="G11" s="6" t="s">
         <v>168</v>
       </c>
       <c r="H11">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I11">
         <f t="shared" ca="1" si="3"/>
@@ -4980,14 +5008,14 @@
       </c>
       <c r="J11">
         <f t="shared" ca="1" si="4"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="K11">
         <v>1</v>
       </c>
       <c r="L11" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>43825.10472210648</v>
+        <v>43825.461475578704</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
@@ -5005,34 +5033,34 @@
         <f t="shared" si="1"/>
         <v>khuong 10</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="E12" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="F12" s="8" t="str">
+      <c r="F12" s="7" t="str">
         <f t="shared" si="2"/>
         <v>yoshi@gmail.com</v>
       </c>
-      <c r="G12" s="7" t="s">
+      <c r="G12" s="6" t="s">
         <v>169</v>
       </c>
       <c r="H12">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I12">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J12">
         <f t="shared" ca="1" si="4"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="K12">
         <v>1</v>
       </c>
       <c r="L12" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>43825.10472210648</v>
+        <v>43825.461475578704</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
@@ -5050,14 +5078,14 @@
         <f t="shared" si="1"/>
         <v>khuong 11</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="E13" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="F13" s="8" t="str">
+      <c r="F13" s="7" t="str">
         <f t="shared" si="2"/>
         <v>yoshi@gmail.com</v>
       </c>
-      <c r="G13" s="7" t="s">
+      <c r="G13" s="6" t="s">
         <v>170</v>
       </c>
       <c r="H13">
@@ -5077,7 +5105,7 @@
       </c>
       <c r="L13" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>43825.10472210648</v>
+        <v>43825.461475578704</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
@@ -5095,19 +5123,19 @@
         <f t="shared" si="1"/>
         <v>khuong 12</v>
       </c>
-      <c r="E14" s="6" t="s">
+      <c r="E14" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="F14" s="8" t="str">
+      <c r="F14" s="7" t="str">
         <f t="shared" si="2"/>
         <v>yoshi@gmail.com</v>
       </c>
-      <c r="G14" s="7" t="s">
+      <c r="G14" s="6" t="s">
         <v>171</v>
       </c>
       <c r="H14">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I14">
         <f t="shared" ca="1" si="3"/>
@@ -5115,14 +5143,14 @@
       </c>
       <c r="J14">
         <f t="shared" ca="1" si="4"/>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="K14">
         <v>1</v>
       </c>
       <c r="L14" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>43825.10472210648</v>
+        <v>43825.461475578704</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
@@ -5140,34 +5168,34 @@
         <f t="shared" si="1"/>
         <v>khuong 13</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="E15" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="F15" s="8" t="str">
+      <c r="F15" s="7" t="str">
         <f t="shared" si="2"/>
         <v>yoshi@gmail.com</v>
       </c>
-      <c r="G15" s="7" t="s">
+      <c r="G15" s="6" t="s">
         <v>172</v>
       </c>
       <c r="H15">
         <f t="shared" ca="1" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="I15">
+        <f t="shared" ca="1" si="3"/>
         <v>5</v>
-      </c>
-      <c r="I15">
-        <f t="shared" ca="1" si="3"/>
-        <v>3</v>
       </c>
       <c r="J15">
         <f t="shared" ca="1" si="4"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K15">
         <v>1</v>
       </c>
       <c r="L15" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>43825.10472210648</v>
+        <v>43825.461475578704</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
@@ -5185,19 +5213,19 @@
         <f t="shared" si="1"/>
         <v>khuong 14</v>
       </c>
-      <c r="E16" s="6" t="s">
+      <c r="E16" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="F16" s="8" t="str">
+      <c r="F16" s="7" t="str">
         <f t="shared" si="2"/>
         <v>yoshi@gmail.com</v>
       </c>
-      <c r="G16" s="7" t="s">
+      <c r="G16" s="6" t="s">
         <v>173</v>
       </c>
       <c r="H16">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I16">
         <f t="shared" ca="1" si="3"/>
@@ -5205,14 +5233,14 @@
       </c>
       <c r="J16">
         <f t="shared" ca="1" si="4"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="K16">
         <v>1</v>
       </c>
       <c r="L16" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>43825.10472210648</v>
+        <v>43825.461475578704</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -5230,23 +5258,23 @@
         <f t="shared" si="1"/>
         <v>khuong 15</v>
       </c>
-      <c r="E17" s="6" t="s">
+      <c r="E17" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="F17" s="8" t="str">
+      <c r="F17" s="7" t="str">
         <f t="shared" si="2"/>
         <v>yoshi@gmail.com</v>
       </c>
-      <c r="G17" s="7" t="s">
+      <c r="G17" s="6" t="s">
         <v>174</v>
       </c>
       <c r="H17">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I17">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J17">
         <f t="shared" ca="1" si="4"/>
@@ -5257,7 +5285,7 @@
       </c>
       <c r="L17" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>43825.10472210648</v>
+        <v>43825.461475578704</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -5275,34 +5303,34 @@
         <f t="shared" si="1"/>
         <v>khuong 16</v>
       </c>
-      <c r="E18" s="6" t="s">
+      <c r="E18" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="F18" s="8" t="str">
+      <c r="F18" s="7" t="str">
         <f t="shared" si="2"/>
         <v>yoshi@gmail.com</v>
       </c>
-      <c r="G18" s="7" t="s">
+      <c r="G18" s="6" t="s">
         <v>175</v>
       </c>
       <c r="H18">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I18">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="J18">
         <f t="shared" ca="1" si="4"/>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="K18">
         <v>1</v>
       </c>
       <c r="L18" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>43825.10472210648</v>
+        <v>43825.461475578704</v>
       </c>
     </row>
   </sheetData>
@@ -5317,4 +5345,643 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" customWidth="1"/>
+    <col min="9" max="10" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>177</v>
+      </c>
+      <c r="B2" t="s">
+        <v>178</v>
+      </c>
+      <c r="C2" t="s">
+        <v>179</v>
+      </c>
+      <c r="D2" t="s">
+        <v>180</v>
+      </c>
+      <c r="E2" t="s">
+        <v>181</v>
+      </c>
+      <c r="F2" t="s">
+        <v>143</v>
+      </c>
+      <c r="G2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" t="s">
+        <v>35</v>
+      </c>
+      <c r="K2" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="str">
+        <f>"khuong "&amp;A3</f>
+        <v>khuong 1</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="D3">
+        <v>123</v>
+      </c>
+      <c r="E3">
+        <f ca="1">RANDBETWEEN(0,5)</f>
+        <v>5</v>
+      </c>
+      <c r="F3">
+        <f ca="1">RANDBETWEEN(1000,8000)</f>
+        <v>7960</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3" s="3">
+        <f ca="1">NOW()</f>
+        <v>43825.461475578704</v>
+      </c>
+      <c r="J3" s="3">
+        <f ca="1">NOW()</f>
+        <v>43825.461475578704</v>
+      </c>
+      <c r="K3" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="str">
+        <f t="shared" ref="B4:B16" si="0">"khuong "&amp;A4</f>
+        <v>khuong 2</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="D4">
+        <v>124</v>
+      </c>
+      <c r="E4">
+        <f t="shared" ref="E4:E16" ca="1" si="1">RANDBETWEEN(0,5)</f>
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <f t="shared" ref="F4:F16" ca="1" si="2">RANDBETWEEN(1000,8000)</f>
+        <v>6822</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I4" s="3">
+        <f t="shared" ref="I4:J16" ca="1" si="3">NOW()</f>
+        <v>43825.461475578704</v>
+      </c>
+      <c r="J4" s="3">
+        <f t="shared" ca="1" si="3"/>
+        <v>43825.461475578704</v>
+      </c>
+      <c r="K4" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="str">
+        <f t="shared" si="0"/>
+        <v>khuong 3</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="D5">
+        <v>125</v>
+      </c>
+      <c r="E5">
+        <f t="shared" ca="1" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="F5">
+        <f t="shared" ca="1" si="2"/>
+        <v>4730</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I5" s="3">
+        <f t="shared" ca="1" si="3"/>
+        <v>43825.461475578704</v>
+      </c>
+      <c r="J5" s="3">
+        <f t="shared" ca="1" si="3"/>
+        <v>43825.461475578704</v>
+      </c>
+      <c r="K5" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="str">
+        <f t="shared" si="0"/>
+        <v>khuong 4</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="D6">
+        <v>126</v>
+      </c>
+      <c r="E6">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <f t="shared" ca="1" si="2"/>
+        <v>2951</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6" t="s">
+        <v>6</v>
+      </c>
+      <c r="I6" s="3">
+        <f t="shared" ca="1" si="3"/>
+        <v>43825.461475578704</v>
+      </c>
+      <c r="J6" s="3">
+        <f t="shared" ca="1" si="3"/>
+        <v>43825.461475578704</v>
+      </c>
+      <c r="K6" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="str">
+        <f t="shared" si="0"/>
+        <v>khuong 5</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="D7">
+        <v>127</v>
+      </c>
+      <c r="E7">
+        <f t="shared" ca="1" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="F7">
+        <f t="shared" ca="1" si="2"/>
+        <v>3307</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7" t="s">
+        <v>6</v>
+      </c>
+      <c r="I7" s="3">
+        <f t="shared" ca="1" si="3"/>
+        <v>43825.461475578704</v>
+      </c>
+      <c r="J7" s="3">
+        <f t="shared" ca="1" si="3"/>
+        <v>43825.461475578704</v>
+      </c>
+      <c r="K7" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="str">
+        <f t="shared" si="0"/>
+        <v>khuong 6</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="D8">
+        <v>128</v>
+      </c>
+      <c r="E8">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <f t="shared" ca="1" si="2"/>
+        <v>3287</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8" t="s">
+        <v>6</v>
+      </c>
+      <c r="I8" s="3">
+        <f t="shared" ca="1" si="3"/>
+        <v>43825.461475578704</v>
+      </c>
+      <c r="J8" s="3">
+        <f t="shared" ca="1" si="3"/>
+        <v>43825.461475578704</v>
+      </c>
+      <c r="K8" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="str">
+        <f t="shared" si="0"/>
+        <v>khuong 7</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="D9">
+        <v>129</v>
+      </c>
+      <c r="E9">
+        <f t="shared" ca="1" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="F9">
+        <f t="shared" ca="1" si="2"/>
+        <v>6956</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9" t="s">
+        <v>6</v>
+      </c>
+      <c r="I9" s="3">
+        <f t="shared" ca="1" si="3"/>
+        <v>43825.461475578704</v>
+      </c>
+      <c r="J9" s="3">
+        <f t="shared" ca="1" si="3"/>
+        <v>43825.461475578704</v>
+      </c>
+      <c r="K9" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="str">
+        <f t="shared" si="0"/>
+        <v>khuong 8</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="D10">
+        <v>130</v>
+      </c>
+      <c r="E10">
+        <f t="shared" ca="1" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="F10">
+        <f t="shared" ca="1" si="2"/>
+        <v>1957</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10" t="s">
+        <v>6</v>
+      </c>
+      <c r="I10" s="3">
+        <f t="shared" ca="1" si="3"/>
+        <v>43825.461475578704</v>
+      </c>
+      <c r="J10" s="3">
+        <f t="shared" ca="1" si="3"/>
+        <v>43825.461475578704</v>
+      </c>
+      <c r="K10" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="str">
+        <f t="shared" si="0"/>
+        <v>khuong 9</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="D11">
+        <v>131</v>
+      </c>
+      <c r="E11">
+        <f t="shared" ca="1" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="F11">
+        <f t="shared" ca="1" si="2"/>
+        <v>6169</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11" t="s">
+        <v>6</v>
+      </c>
+      <c r="I11" s="3">
+        <f t="shared" ca="1" si="3"/>
+        <v>43825.461475578704</v>
+      </c>
+      <c r="J11" s="3">
+        <f t="shared" ca="1" si="3"/>
+        <v>43825.461475578704</v>
+      </c>
+      <c r="K11" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" t="str">
+        <f t="shared" si="0"/>
+        <v>khuong 10</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="D12">
+        <v>132</v>
+      </c>
+      <c r="E12">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <f t="shared" ca="1" si="2"/>
+        <v>7284</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12" t="s">
+        <v>6</v>
+      </c>
+      <c r="I12" s="3">
+        <f t="shared" ca="1" si="3"/>
+        <v>43825.461475578704</v>
+      </c>
+      <c r="J12" s="3">
+        <f t="shared" ca="1" si="3"/>
+        <v>43825.461475578704</v>
+      </c>
+      <c r="K12" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" t="str">
+        <f t="shared" si="0"/>
+        <v>khuong 11</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="D13">
+        <v>133</v>
+      </c>
+      <c r="E13">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <f t="shared" ca="1" si="2"/>
+        <v>5007</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13" t="s">
+        <v>6</v>
+      </c>
+      <c r="I13" s="3">
+        <f t="shared" ca="1" si="3"/>
+        <v>43825.461475578704</v>
+      </c>
+      <c r="J13" s="3">
+        <f t="shared" ca="1" si="3"/>
+        <v>43825.461475578704</v>
+      </c>
+      <c r="K13" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" t="str">
+        <f t="shared" si="0"/>
+        <v>khuong 12</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="D14">
+        <v>134</v>
+      </c>
+      <c r="E14">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <f t="shared" ca="1" si="2"/>
+        <v>6670</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14" t="s">
+        <v>6</v>
+      </c>
+      <c r="I14" s="3">
+        <f t="shared" ca="1" si="3"/>
+        <v>43825.461475578704</v>
+      </c>
+      <c r="J14" s="3">
+        <f t="shared" ca="1" si="3"/>
+        <v>43825.461475578704</v>
+      </c>
+      <c r="K14" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" t="str">
+        <f t="shared" si="0"/>
+        <v>khuong 13</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="D15">
+        <v>135</v>
+      </c>
+      <c r="E15">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <f t="shared" ca="1" si="2"/>
+        <v>4519</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15" t="s">
+        <v>6</v>
+      </c>
+      <c r="I15" s="3">
+        <f t="shared" ca="1" si="3"/>
+        <v>43825.461475578704</v>
+      </c>
+      <c r="J15" s="3">
+        <f t="shared" ca="1" si="3"/>
+        <v>43825.461475578704</v>
+      </c>
+      <c r="K15" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" t="str">
+        <f t="shared" si="0"/>
+        <v>khuong 14</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="D16">
+        <v>136</v>
+      </c>
+      <c r="E16">
+        <f t="shared" ca="1" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="F16">
+        <f t="shared" ca="1" si="2"/>
+        <v>3483</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16" t="s">
+        <v>6</v>
+      </c>
+      <c r="I16" s="3">
+        <f t="shared" ca="1" si="3"/>
+        <v>43825.461475578704</v>
+      </c>
+      <c r="J16" s="3">
+        <f t="shared" ca="1" si="3"/>
+        <v>43825.461475578704</v>
+      </c>
+      <c r="K16" t="s">
+        <v>182</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:P1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
version 3.5 Update Seting
</commit_message>
<xml_diff>
--- a/rau.xlsx
+++ b/rau.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6765" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6765" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="LoaiSP" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="Relative_food" sheetId="6" r:id="rId6"/>
     <sheet name="Customer" sheetId="7" r:id="rId7"/>
     <sheet name="Order" sheetId="8" r:id="rId8"/>
+    <sheet name="Order_Detail" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="188">
   <si>
     <t>type_id</t>
   </si>
@@ -586,6 +587,15 @@
   </si>
   <si>
     <t>cus_username</t>
+  </si>
+  <si>
+    <t>SELECT [order_id] ,[food_id] ,[quan] ,[unit] ,[price] ,[total] FROM [dbo].[order_detail]</t>
+  </si>
+  <si>
+    <t>food_id</t>
+  </si>
+  <si>
+    <t>total</t>
   </si>
 </sst>
 </file>
@@ -1643,19 +1653,19 @@
 IF(RANDBETWEEN(1,4)=2,"Stawberry",
 IF(RANDBETWEEN(1,4)=3,"Green Beans","Tomatoe"
 )))</f>
-        <v>Tomatoe</v>
+        <v>Bell Perpper</v>
       </c>
       <c r="C2" t="str">
         <f t="shared" ref="C2:C18" ca="1" si="1">"Description "&amp;B2</f>
-        <v>Description Tomatoe</v>
+        <v>Description Bell Perpper</v>
       </c>
       <c r="D2" t="str">
         <f ca="1">TEXT(RANDBETWEEN(1,1000),"0")</f>
-        <v>939</v>
+        <v>4</v>
       </c>
       <c r="E2" s="2" t="str">
         <f ca="1">TEXT(D2-D2*RAND()*0.1,"0")</f>
-        <v>848</v>
+        <v>4</v>
       </c>
       <c r="F2" t="str">
         <f t="shared" ref="F2:F18" si="2">"product-"&amp;A2&amp;".jpg"</f>
@@ -1678,15 +1688,15 @@
       </c>
       <c r="K2">
         <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L2" s="2">
         <f ca="1">ABS(TEXT(RAND()+0.1-0.2,"0.0"))</f>
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="M2">
         <f t="shared" ref="M2:M18" ca="1" si="5">RANDBETWEEN(1,4)</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="N2">
         <v>1</v>
@@ -1701,7 +1711,7 @@
       </c>
       <c r="R2" t="str">
         <f ca="1">"INSERT INTO [dbo].[food] ([name] ,[description] ,[price] ,[price_promo] ,[thumb] ,[img] ,[unit] ,[percent_promo] ,[rating] ,[sold] ,[point] ,[type] ,[status] ,[username] ,[modified]) VALUES ('"&amp;B2&amp;"' ,'"&amp;C2&amp;"' ,"&amp;D2&amp;" ,"&amp;E2&amp;",' "&amp;F2&amp;"','"&amp;G2&amp;"' ,'"&amp;H2&amp;"' ,"&amp;I2&amp;" ,"&amp;J2&amp;","&amp;K2&amp;","&amp;L2&amp;" ,"&amp;M2&amp;","&amp;N2&amp;",'"&amp;O2&amp;"','"&amp;P2&amp;"')"</f>
-        <v>INSERT INTO [dbo].[food] ([name] ,[description] ,[price] ,[price_promo] ,[thumb] ,[img] ,[unit] ,[percent_promo] ,[rating] ,[sold] ,[point] ,[type] ,[status] ,[username] ,[modified]) VALUES ('Tomatoe' ,'Description Tomatoe' ,939 ,848,' product-1.jpg','product-1.jpg' ,'gam' ,0.1 ,6,2,0.3 ,4,1,'khuong','12/26/2019')</v>
+        <v>INSERT INTO [dbo].[food] ([name] ,[description] ,[price] ,[price_promo] ,[thumb] ,[img] ,[unit] ,[percent_promo] ,[rating] ,[sold] ,[point] ,[type] ,[status] ,[username] ,[modified]) VALUES ('Bell Perpper' ,'Description Bell Perpper' ,4 ,4,' product-1.jpg','product-1.jpg' ,'gam' ,0.1 ,6,4,0.5 ,2,1,'khuong','12/26/2019')</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
@@ -1718,11 +1728,11 @@
       </c>
       <c r="D3" t="str">
         <f t="shared" ref="D3:D18" ca="1" si="7">TEXT(RANDBETWEEN(1,1000),"0")</f>
-        <v>214</v>
+        <v>765</v>
       </c>
       <c r="E3" s="2" t="str">
         <f t="shared" ref="E3:E18" ca="1" si="8">TEXT(D3-D3*RAND()*0.1,"0")</f>
-        <v>210</v>
+        <v>736</v>
       </c>
       <c r="F3" t="str">
         <f t="shared" si="2"/>
@@ -1737,7 +1747,7 @@
       </c>
       <c r="I3" s="2" t="str">
         <f t="shared" ref="I3:I18" ca="1" si="9">TEXT(RAND()+0.1-0.2,"0.0")</f>
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
       <c r="J3">
         <f t="shared" ca="1" si="4"/>
@@ -1745,15 +1755,15 @@
       </c>
       <c r="K3">
         <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="L3" s="2">
         <f t="shared" ref="L3:L18" ca="1" si="10">ABS(TEXT(RAND()+0.1-0.2,"0.0"))</f>
-        <v>0.9</v>
+        <v>0.1</v>
       </c>
       <c r="M3">
         <f t="shared" ca="1" si="5"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="N3">
         <v>1</v>
@@ -1768,7 +1778,7 @@
       </c>
       <c r="R3" t="str">
         <f t="shared" ref="R3:R18" ca="1" si="12">"INSERT INTO [dbo].[food] ([name] ,[description] ,[price] ,[price_promo] ,[thumb] ,[img] ,[unit] ,[percent_promo] ,[rating] ,[sold] ,[point] ,[type] ,[status] ,[username] ,[modified]) VALUES ('"&amp;B3&amp;"' ,'"&amp;C3&amp;"' ,"&amp;D3&amp;" ,"&amp;E3&amp;",' "&amp;F3&amp;"','"&amp;G3&amp;"' ,'"&amp;H3&amp;"' ,"&amp;I3&amp;" ,"&amp;J3&amp;","&amp;K3&amp;","&amp;L3&amp;" ,"&amp;M3&amp;","&amp;N3&amp;",'"&amp;O3&amp;"','"&amp;P3&amp;"')"</f>
-        <v>INSERT INTO [dbo].[food] ([name] ,[description] ,[price] ,[price_promo] ,[thumb] ,[img] ,[unit] ,[percent_promo] ,[rating] ,[sold] ,[point] ,[type] ,[status] ,[username] ,[modified]) VALUES ('Tomatoe' ,'Description Tomatoe' ,214 ,210,' product-2.jpg','product-2.jpg' ,'gam' ,0.4 ,7,2,0.9 ,4,1,'khuong','12/26/2019')</v>
+        <v>INSERT INTO [dbo].[food] ([name] ,[description] ,[price] ,[price_promo] ,[thumb] ,[img] ,[unit] ,[percent_promo] ,[rating] ,[sold] ,[point] ,[type] ,[status] ,[username] ,[modified]) VALUES ('Tomatoe' ,'Description Tomatoe' ,765 ,736,' product-2.jpg','product-2.jpg' ,'gam' ,0.3 ,7,7,0.1 ,2,1,'khuong','12/26/2019')</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
@@ -1777,19 +1787,19 @@
       </c>
       <c r="B4" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Bell Perpper</v>
+        <v>Stawberry</v>
       </c>
       <c r="C4" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Description Bell Perpper</v>
+        <v>Description Stawberry</v>
       </c>
       <c r="D4" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>297</v>
+        <v>647</v>
       </c>
       <c r="E4" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>283</v>
+        <v>640</v>
       </c>
       <c r="F4" t="str">
         <f t="shared" si="2"/>
@@ -1804,7 +1814,7 @@
       </c>
       <c r="I4" s="2" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
       <c r="J4">
         <f t="shared" ca="1" si="4"/>
@@ -1816,11 +1826,11 @@
       </c>
       <c r="L4" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>0.7</v>
+        <v>0.2</v>
       </c>
       <c r="M4">
         <f t="shared" ca="1" si="5"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="N4">
         <v>1</v>
@@ -1835,7 +1845,7 @@
       </c>
       <c r="R4" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>INSERT INTO [dbo].[food] ([name] ,[description] ,[price] ,[price_promo] ,[thumb] ,[img] ,[unit] ,[percent_promo] ,[rating] ,[sold] ,[point] ,[type] ,[status] ,[username] ,[modified]) VALUES ('Bell Perpper' ,'Description Bell Perpper' ,297 ,283,' product-3.jpg','product-3.jpg' ,'gam' ,0.6 ,1,10,0.7 ,4,1,'khuong','12/26/2019')</v>
+        <v>INSERT INTO [dbo].[food] ([name] ,[description] ,[price] ,[price_promo] ,[thumb] ,[img] ,[unit] ,[percent_promo] ,[rating] ,[sold] ,[point] ,[type] ,[status] ,[username] ,[modified]) VALUES ('Stawberry' ,'Description Stawberry' ,647 ,640,' product-3.jpg','product-3.jpg' ,'gam' ,0.8 ,1,10,0.2 ,2,1,'khuong','12/26/2019')</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
@@ -1852,11 +1862,11 @@
       </c>
       <c r="D5" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>989</v>
+        <v>725</v>
       </c>
       <c r="E5" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>979</v>
+        <v>713</v>
       </c>
       <c r="F5" t="str">
         <f t="shared" si="2"/>
@@ -1871,23 +1881,23 @@
       </c>
       <c r="I5" s="2" t="str">
         <f ca="1">TEXT(RAND()+0.1-0.2,"0.0")</f>
-        <v>0.3</v>
+        <v>0.6</v>
       </c>
       <c r="J5">
         <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="K5">
         <f t="shared" ca="1" si="4"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L5" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>0.7</v>
+        <v>0.4</v>
       </c>
       <c r="M5">
         <f t="shared" ca="1" si="5"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N5">
         <v>1</v>
@@ -1902,7 +1912,7 @@
       </c>
       <c r="R5" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>INSERT INTO [dbo].[food] ([name] ,[description] ,[price] ,[price_promo] ,[thumb] ,[img] ,[unit] ,[percent_promo] ,[rating] ,[sold] ,[point] ,[type] ,[status] ,[username] ,[modified]) VALUES ('Stawberry' ,'Description Stawberry' ,989 ,979,' product-4.jpg','product-4.jpg' ,'gam' ,0.3 ,2,5,0.7 ,1,1,'khuong','12/26/2019')</v>
+        <v>INSERT INTO [dbo].[food] ([name] ,[description] ,[price] ,[price_promo] ,[thumb] ,[img] ,[unit] ,[percent_promo] ,[rating] ,[sold] ,[point] ,[type] ,[status] ,[username] ,[modified]) VALUES ('Stawberry' ,'Description Stawberry' ,725 ,713,' product-4.jpg','product-4.jpg' ,'gam' ,0.6 ,5,4,0.4 ,2,1,'khuong','12/26/2019')</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
@@ -1911,19 +1921,19 @@
       </c>
       <c r="B6" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Tomatoe</v>
+        <v>Bell Perpper</v>
       </c>
       <c r="C6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Description Tomatoe</v>
+        <v>Description Bell Perpper</v>
       </c>
       <c r="D6" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>774</v>
+        <v>103</v>
       </c>
       <c r="E6" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>701</v>
+        <v>93</v>
       </c>
       <c r="F6" t="str">
         <f t="shared" si="2"/>
@@ -1938,23 +1948,23 @@
       </c>
       <c r="I6" s="2" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>0.0</v>
+        <v>0.1</v>
       </c>
       <c r="J6">
         <f t="shared" ca="1" si="4"/>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="K6">
         <f t="shared" ca="1" si="4"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="L6" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="M6">
         <f t="shared" ca="1" si="5"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="N6">
         <v>1</v>
@@ -1969,7 +1979,7 @@
       </c>
       <c r="R6" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>INSERT INTO [dbo].[food] ([name] ,[description] ,[price] ,[price_promo] ,[thumb] ,[img] ,[unit] ,[percent_promo] ,[rating] ,[sold] ,[point] ,[type] ,[status] ,[username] ,[modified]) VALUES ('Tomatoe' ,'Description Tomatoe' ,774 ,701,' product-5.jpg','product-5.jpg' ,'gam' ,0.0 ,6,5,0.2 ,4,1,'khuong','12/26/2019')</v>
+        <v>INSERT INTO [dbo].[food] ([name] ,[description] ,[price] ,[price_promo] ,[thumb] ,[img] ,[unit] ,[percent_promo] ,[rating] ,[sold] ,[point] ,[type] ,[status] ,[username] ,[modified]) VALUES ('Bell Perpper' ,'Description Bell Perpper' ,103 ,93,' product-5.jpg','product-5.jpg' ,'gam' ,0.1 ,2,2,0.1 ,1,1,'khuong','12/26/2019')</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
@@ -1978,19 +1988,19 @@
       </c>
       <c r="B7" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Bell Perpper</v>
+        <v>Stawberry</v>
       </c>
       <c r="C7" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Description Bell Perpper</v>
+        <v>Description Stawberry</v>
       </c>
       <c r="D7" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>479</v>
+        <v>36</v>
       </c>
       <c r="E7" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>470</v>
+        <v>35</v>
       </c>
       <c r="F7" t="str">
         <f t="shared" si="2"/>
@@ -2005,19 +2015,19 @@
       </c>
       <c r="I7" s="2" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
       <c r="J7">
         <f t="shared" ca="1" si="4"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K7">
         <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L7" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="M7">
         <f t="shared" ca="1" si="5"/>
@@ -2036,7 +2046,7 @@
       </c>
       <c r="R7" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>INSERT INTO [dbo].[food] ([name] ,[description] ,[price] ,[price_promo] ,[thumb] ,[img] ,[unit] ,[percent_promo] ,[rating] ,[sold] ,[point] ,[type] ,[status] ,[username] ,[modified]) VALUES ('Bell Perpper' ,'Description Bell Perpper' ,479 ,470,' product-6.jpg','product-6.jpg' ,'gam' ,0.5 ,4,2,0.8 ,3,1,'khuong','12/26/2019')</v>
+        <v>INSERT INTO [dbo].[food] ([name] ,[description] ,[price] ,[price_promo] ,[thumb] ,[img] ,[unit] ,[percent_promo] ,[rating] ,[sold] ,[point] ,[type] ,[status] ,[username] ,[modified]) VALUES ('Stawberry' ,'Description Stawberry' ,36 ,35,' product-6.jpg','product-6.jpg' ,'gam' ,0.7 ,5,1,0 ,3,1,'khuong','12/26/2019')</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
@@ -2053,11 +2063,11 @@
       </c>
       <c r="D8" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>281</v>
+        <v>842</v>
       </c>
       <c r="E8" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>258</v>
+        <v>784</v>
       </c>
       <c r="F8" t="str">
         <f t="shared" si="2"/>
@@ -2072,23 +2082,23 @@
       </c>
       <c r="I8" s="2" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
       <c r="J8">
         <f t="shared" ca="1" si="4"/>
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="K8">
         <f t="shared" ca="1" si="4"/>
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="L8" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>0.2</v>
+        <v>0.6</v>
       </c>
       <c r="M8">
         <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N8">
         <v>1</v>
@@ -2103,7 +2113,7 @@
       </c>
       <c r="R8" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>INSERT INTO [dbo].[food] ([name] ,[description] ,[price] ,[price_promo] ,[thumb] ,[img] ,[unit] ,[percent_promo] ,[rating] ,[sold] ,[point] ,[type] ,[status] ,[username] ,[modified]) VALUES ('Tomatoe' ,'Description Tomatoe' ,281 ,258,' product-7.jpg','product-7.jpg' ,'gam' ,0.4 ,9,7,0.2 ,2,1,'khuong','12/26/2019')</v>
+        <v>INSERT INTO [dbo].[food] ([name] ,[description] ,[price] ,[price_promo] ,[thumb] ,[img] ,[unit] ,[percent_promo] ,[rating] ,[sold] ,[point] ,[type] ,[status] ,[username] ,[modified]) VALUES ('Tomatoe' ,'Description Tomatoe' ,842 ,784,' product-7.jpg','product-7.jpg' ,'gam' ,0.6 ,5,1,0.6 ,1,1,'khuong','12/26/2019')</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
@@ -2120,11 +2130,11 @@
       </c>
       <c r="D9" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>665</v>
+        <v>378</v>
       </c>
       <c r="E9" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>657</v>
+        <v>356</v>
       </c>
       <c r="F9" t="str">
         <f t="shared" si="2"/>
@@ -2147,15 +2157,15 @@
       </c>
       <c r="K9">
         <f t="shared" ca="1" si="4"/>
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="L9" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>0.7</v>
+        <v>0.1</v>
       </c>
       <c r="M9">
         <f t="shared" ca="1" si="5"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N9">
         <v>1</v>
@@ -2170,7 +2180,7 @@
       </c>
       <c r="R9" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>INSERT INTO [dbo].[food] ([name] ,[description] ,[price] ,[price_promo] ,[thumb] ,[img] ,[unit] ,[percent_promo] ,[rating] ,[sold] ,[point] ,[type] ,[status] ,[username] ,[modified]) VALUES ('Tomatoe' ,'Description Tomatoe' ,665 ,657,' product-8.jpg','product-8.jpg' ,'gam' ,0.5 ,10,9,0.7 ,4,1,'khuong','12/26/2019')</v>
+        <v>INSERT INTO [dbo].[food] ([name] ,[description] ,[price] ,[price_promo] ,[thumb] ,[img] ,[unit] ,[percent_promo] ,[rating] ,[sold] ,[point] ,[type] ,[status] ,[username] ,[modified]) VALUES ('Tomatoe' ,'Description Tomatoe' ,378 ,356,' product-8.jpg','product-8.jpg' ,'gam' ,0.5 ,10,6,0.1 ,3,1,'khuong','12/26/2019')</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
@@ -2179,19 +2189,19 @@
       </c>
       <c r="B10" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Tomatoe</v>
+        <v>Bell Perpper</v>
       </c>
       <c r="C10" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Description Tomatoe</v>
+        <v>Description Bell Perpper</v>
       </c>
       <c r="D10" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>366</v>
+        <v>625</v>
       </c>
       <c r="E10" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>363</v>
+        <v>615</v>
       </c>
       <c r="F10" t="str">
         <f t="shared" si="2"/>
@@ -2206,23 +2216,23 @@
       </c>
       <c r="I10" s="2" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>0.0</v>
+        <v>0.5</v>
       </c>
       <c r="J10">
         <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K10">
         <f t="shared" ca="1" si="4"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="L10" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="M10">
         <f t="shared" ca="1" si="5"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N10">
         <v>1</v>
@@ -2237,7 +2247,7 @@
       </c>
       <c r="R10" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>INSERT INTO [dbo].[food] ([name] ,[description] ,[price] ,[price_promo] ,[thumb] ,[img] ,[unit] ,[percent_promo] ,[rating] ,[sold] ,[point] ,[type] ,[status] ,[username] ,[modified]) VALUES ('Tomatoe' ,'Description Tomatoe' ,366 ,363,' product-9.jpg','product-9.jpg' ,'gam' ,0.0 ,1,6,0.1 ,4,1,'khuong','12/26/2019')</v>
+        <v>INSERT INTO [dbo].[food] ([name] ,[description] ,[price] ,[price_promo] ,[thumb] ,[img] ,[unit] ,[percent_promo] ,[rating] ,[sold] ,[point] ,[type] ,[status] ,[username] ,[modified]) VALUES ('Bell Perpper' ,'Description Bell Perpper' ,625 ,615,' product-9.jpg','product-9.jpg' ,'gam' ,0.5 ,2,8,0.2 ,3,1,'khuong','12/26/2019')</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
@@ -2246,19 +2256,19 @@
       </c>
       <c r="B11" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Bell Perpper</v>
+        <v>Green Beans</v>
       </c>
       <c r="C11" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Description Bell Perpper</v>
+        <v>Description Green Beans</v>
       </c>
       <c r="D11" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>132</v>
+        <v>721</v>
       </c>
       <c r="E11" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>125</v>
+        <v>697</v>
       </c>
       <c r="F11" t="str">
         <f t="shared" si="2"/>
@@ -2273,19 +2283,19 @@
       </c>
       <c r="I11" s="2" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="J11">
         <f t="shared" ca="1" si="4"/>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="K11">
         <f t="shared" ca="1" si="4"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="L11" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="M11">
         <f t="shared" ca="1" si="5"/>
@@ -2304,7 +2314,7 @@
       </c>
       <c r="R11" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>INSERT INTO [dbo].[food] ([name] ,[description] ,[price] ,[price_promo] ,[thumb] ,[img] ,[unit] ,[percent_promo] ,[rating] ,[sold] ,[point] ,[type] ,[status] ,[username] ,[modified]) VALUES ('Bell Perpper' ,'Description Bell Perpper' ,132 ,125,' product-10.jpg','product-10.jpg' ,'gam' ,0.3 ,3,10,0 ,3,1,'khuong','12/26/2019')</v>
+        <v>INSERT INTO [dbo].[food] ([name] ,[description] ,[price] ,[price_promo] ,[thumb] ,[img] ,[unit] ,[percent_promo] ,[rating] ,[sold] ,[point] ,[type] ,[status] ,[username] ,[modified]) VALUES ('Green Beans' ,'Description Green Beans' ,721 ,697,' product-10.jpg','product-10.jpg' ,'gam' ,0.2 ,9,3,0.8 ,3,1,'khuong','12/26/2019')</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
@@ -2313,19 +2323,19 @@
       </c>
       <c r="B12" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Bell Perpper</v>
+        <v>Green Beans</v>
       </c>
       <c r="C12" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Description Bell Perpper</v>
+        <v>Description Green Beans</v>
       </c>
       <c r="D12" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>880</v>
+        <v>548</v>
       </c>
       <c r="E12" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>818</v>
+        <v>497</v>
       </c>
       <c r="F12" t="str">
         <f t="shared" si="2"/>
@@ -2340,7 +2350,7 @@
       </c>
       <c r="I12" s="2" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="J12">
         <f t="shared" ca="1" si="4"/>
@@ -2348,15 +2358,15 @@
       </c>
       <c r="K12">
         <f t="shared" ca="1" si="4"/>
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="L12" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="M12">
         <f t="shared" ca="1" si="5"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N12">
         <v>1</v>
@@ -2371,7 +2381,7 @@
       </c>
       <c r="R12" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>INSERT INTO [dbo].[food] ([name] ,[description] ,[price] ,[price_promo] ,[thumb] ,[img] ,[unit] ,[percent_promo] ,[rating] ,[sold] ,[point] ,[type] ,[status] ,[username] ,[modified]) VALUES ('Bell Perpper' ,'Description Bell Perpper' ,880 ,818,' product-11.jpg','product-11.jpg' ,'gam' ,0.4 ,10,7,0.1 ,4,1,'khuong','12/26/2019')</v>
+        <v>INSERT INTO [dbo].[food] ([name] ,[description] ,[price] ,[price_promo] ,[thumb] ,[img] ,[unit] ,[percent_promo] ,[rating] ,[sold] ,[point] ,[type] ,[status] ,[username] ,[modified]) VALUES ('Green Beans' ,'Description Green Beans' ,548 ,497,' product-11.jpg','product-11.jpg' ,'gam' ,0.5 ,10,10,0.5 ,3,1,'khuong','12/26/2019')</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
@@ -2380,19 +2390,19 @@
       </c>
       <c r="B13" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Green Beans</v>
+        <v>Tomatoe</v>
       </c>
       <c r="C13" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Description Green Beans</v>
+        <v>Description Tomatoe</v>
       </c>
       <c r="D13" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>619</v>
+        <v>137</v>
       </c>
       <c r="E13" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>575</v>
+        <v>124</v>
       </c>
       <c r="F13" t="str">
         <f t="shared" si="2"/>
@@ -2407,23 +2417,23 @@
       </c>
       <c r="I13" s="2" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="J13">
         <f t="shared" ca="1" si="4"/>
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="K13">
         <f t="shared" ca="1" si="4"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="L13" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="M13">
         <f t="shared" ca="1" si="5"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="N13">
         <v>1</v>
@@ -2438,7 +2448,7 @@
       </c>
       <c r="R13" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>INSERT INTO [dbo].[food] ([name] ,[description] ,[price] ,[price_promo] ,[thumb] ,[img] ,[unit] ,[percent_promo] ,[rating] ,[sold] ,[point] ,[type] ,[status] ,[username] ,[modified]) VALUES ('Green Beans' ,'Description Green Beans' ,619 ,575,' product-12.jpg','product-12.jpg' ,'gam' ,0.1 ,8,5,0.3 ,4,1,'khuong','12/26/2019')</v>
+        <v>INSERT INTO [dbo].[food] ([name] ,[description] ,[price] ,[price_promo] ,[thumb] ,[img] ,[unit] ,[percent_promo] ,[rating] ,[sold] ,[point] ,[type] ,[status] ,[username] ,[modified]) VALUES ('Tomatoe' ,'Description Tomatoe' ,137 ,124,' product-12.jpg','product-12.jpg' ,'gam' ,0.5 ,3,2,0.4 ,2,1,'khuong','12/26/2019')</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
@@ -2447,19 +2457,19 @@
       </c>
       <c r="B14" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Tomatoe</v>
+        <v>Green Beans</v>
       </c>
       <c r="C14" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Description Tomatoe</v>
+        <v>Description Green Beans</v>
       </c>
       <c r="D14" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>9</v>
+        <v>125</v>
       </c>
       <c r="E14" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>8</v>
+        <v>117</v>
       </c>
       <c r="F14" t="str">
         <f t="shared" si="2"/>
@@ -2478,15 +2488,15 @@
       </c>
       <c r="J14">
         <f t="shared" ca="1" si="4"/>
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="K14">
         <f t="shared" ca="1" si="4"/>
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="L14" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
       <c r="M14">
         <f t="shared" ca="1" si="5"/>
@@ -2505,7 +2515,7 @@
       </c>
       <c r="R14" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>INSERT INTO [dbo].[food] ([name] ,[description] ,[price] ,[price_promo] ,[thumb] ,[img] ,[unit] ,[percent_promo] ,[rating] ,[sold] ,[point] ,[type] ,[status] ,[username] ,[modified]) VALUES ('Tomatoe' ,'Description Tomatoe' ,9 ,8,' product-13.jpg','product-13.jpg' ,'gam' ,0.5 ,3,8,0.5 ,1,1,'khuong','12/26/2019')</v>
+        <v>INSERT INTO [dbo].[food] ([name] ,[description] ,[price] ,[price_promo] ,[thumb] ,[img] ,[unit] ,[percent_promo] ,[rating] ,[sold] ,[point] ,[type] ,[status] ,[username] ,[modified]) VALUES ('Green Beans' ,'Description Green Beans' ,125 ,117,' product-13.jpg','product-13.jpg' ,'gam' ,0.5 ,8,1,0.7 ,1,1,'khuong','12/26/2019')</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
@@ -2514,19 +2524,19 @@
       </c>
       <c r="B15" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Tomatoe</v>
+        <v>Green Beans</v>
       </c>
       <c r="C15" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Description Tomatoe</v>
+        <v>Description Green Beans</v>
       </c>
       <c r="D15" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>577</v>
+        <v>583</v>
       </c>
       <c r="E15" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>524</v>
+        <v>577</v>
       </c>
       <c r="F15" t="str">
         <f t="shared" si="2"/>
@@ -2541,11 +2551,11 @@
       </c>
       <c r="I15" s="2" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>0.0</v>
+        <v>0.8</v>
       </c>
       <c r="J15">
         <f t="shared" ca="1" si="4"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="K15">
         <f t="shared" ca="1" si="4"/>
@@ -2553,11 +2563,11 @@
       </c>
       <c r="L15" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="M15">
         <f t="shared" ca="1" si="5"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N15">
         <v>1</v>
@@ -2572,7 +2582,7 @@
       </c>
       <c r="R15" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>INSERT INTO [dbo].[food] ([name] ,[description] ,[price] ,[price_promo] ,[thumb] ,[img] ,[unit] ,[percent_promo] ,[rating] ,[sold] ,[point] ,[type] ,[status] ,[username] ,[modified]) VALUES ('Tomatoe' ,'Description Tomatoe' ,577 ,524,' product-14.jpg','product-14.jpg' ,'gam' ,0.0 ,4,7,0.3 ,3,1,'khuong','12/26/2019')</v>
+        <v>INSERT INTO [dbo].[food] ([name] ,[description] ,[price] ,[price_promo] ,[thumb] ,[img] ,[unit] ,[percent_promo] ,[rating] ,[sold] ,[point] ,[type] ,[status] ,[username] ,[modified]) VALUES ('Green Beans' ,'Description Green Beans' ,583 ,577,' product-14.jpg','product-14.jpg' ,'gam' ,0.8 ,8,7,0.2 ,2,1,'khuong','12/26/2019')</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
@@ -2581,19 +2591,19 @@
       </c>
       <c r="B16" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Stawberry</v>
+        <v>Green Beans</v>
       </c>
       <c r="C16" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Description Stawberry</v>
+        <v>Description Green Beans</v>
       </c>
       <c r="D16" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>809</v>
+        <v>221</v>
       </c>
       <c r="E16" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>760</v>
+        <v>200</v>
       </c>
       <c r="F16" t="str">
         <f t="shared" si="2"/>
@@ -2608,23 +2618,23 @@
       </c>
       <c r="I16" s="2" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
       <c r="J16">
         <f t="shared" ca="1" si="4"/>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="K16">
         <f t="shared" ca="1" si="4"/>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="L16" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="M16">
         <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N16">
         <v>1</v>
@@ -2639,7 +2649,7 @@
       </c>
       <c r="R16" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>INSERT INTO [dbo].[food] ([name] ,[description] ,[price] ,[price_promo] ,[thumb] ,[img] ,[unit] ,[percent_promo] ,[rating] ,[sold] ,[point] ,[type] ,[status] ,[username] ,[modified]) VALUES ('Stawberry' ,'Description Stawberry' ,809 ,760,' product-15.jpg','product-15.jpg' ,'gam' ,0.5 ,3,8,0 ,2,1,'khuong','12/26/2019')</v>
+        <v>INSERT INTO [dbo].[food] ([name] ,[description] ,[price] ,[price_promo] ,[thumb] ,[img] ,[unit] ,[percent_promo] ,[rating] ,[sold] ,[point] ,[type] ,[status] ,[username] ,[modified]) VALUES ('Green Beans' ,'Description Green Beans' ,221 ,200,' product-15.jpg','product-15.jpg' ,'gam' ,0.7 ,9,6,0.6 ,3,1,'khuong','12/26/2019')</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
@@ -2648,19 +2658,19 @@
       </c>
       <c r="B17" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Bell Perpper</v>
+        <v>Tomatoe</v>
       </c>
       <c r="C17" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Description Bell Perpper</v>
+        <v>Description Tomatoe</v>
       </c>
       <c r="D17" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>461</v>
+        <v>870</v>
       </c>
       <c r="E17" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>447</v>
+        <v>868</v>
       </c>
       <c r="F17" t="str">
         <f t="shared" si="2"/>
@@ -2675,19 +2685,19 @@
       </c>
       <c r="I17" s="2" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>0.0</v>
+        <v>0.3</v>
       </c>
       <c r="J17">
         <f t="shared" ca="1" si="4"/>
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="K17">
         <f t="shared" ca="1" si="4"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="L17" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>0.9</v>
+        <v>0</v>
       </c>
       <c r="M17">
         <f t="shared" ca="1" si="5"/>
@@ -2706,7 +2716,7 @@
       </c>
       <c r="R17" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>INSERT INTO [dbo].[food] ([name] ,[description] ,[price] ,[price_promo] ,[thumb] ,[img] ,[unit] ,[percent_promo] ,[rating] ,[sold] ,[point] ,[type] ,[status] ,[username] ,[modified]) VALUES ('Bell Perpper' ,'Description Bell Perpper' ,461 ,447,' product-16.jpg','product-16.jpg' ,'gam' ,0.0 ,7,5,0.9 ,4,1,'khuong','12/26/2019')</v>
+        <v>INSERT INTO [dbo].[food] ([name] ,[description] ,[price] ,[price_promo] ,[thumb] ,[img] ,[unit] ,[percent_promo] ,[rating] ,[sold] ,[point] ,[type] ,[status] ,[username] ,[modified]) VALUES ('Tomatoe' ,'Description Tomatoe' ,870 ,868,' product-16.jpg','product-16.jpg' ,'gam' ,0.3 ,3,2,0 ,4,1,'khuong','12/26/2019')</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
@@ -2715,19 +2725,19 @@
       </c>
       <c r="B18" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Bell Perpper</v>
+        <v>Tomatoe</v>
       </c>
       <c r="C18" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Description Bell Perpper</v>
+        <v>Description Tomatoe</v>
       </c>
       <c r="D18" t="str">
         <f t="shared" ca="1" si="7"/>
-        <v>26</v>
+        <v>58</v>
       </c>
       <c r="E18" s="2" t="str">
         <f t="shared" ca="1" si="8"/>
-        <v>25</v>
+        <v>56</v>
       </c>
       <c r="F18" t="str">
         <f t="shared" si="2"/>
@@ -2742,7 +2752,7 @@
       </c>
       <c r="I18" s="2" t="str">
         <f t="shared" ca="1" si="9"/>
-        <v>0.8</v>
+        <v>0.4</v>
       </c>
       <c r="J18">
         <f t="shared" ca="1" si="4"/>
@@ -2750,15 +2760,15 @@
       </c>
       <c r="K18">
         <f t="shared" ca="1" si="4"/>
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="L18" s="2">
         <f t="shared" ca="1" si="10"/>
-        <v>0.8</v>
+        <v>0.3</v>
       </c>
       <c r="M18">
         <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N18">
         <v>1</v>
@@ -2773,7 +2783,7 @@
       </c>
       <c r="R18" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>INSERT INTO [dbo].[food] ([name] ,[description] ,[price] ,[price_promo] ,[thumb] ,[img] ,[unit] ,[percent_promo] ,[rating] ,[sold] ,[point] ,[type] ,[status] ,[username] ,[modified]) VALUES ('Bell Perpper' ,'Description Bell Perpper' ,26 ,25,' product-17.jpg','product-17.jpg' ,'gam' ,0.8 ,10,3,0.8 ,2,1,'khuong','12/26/2019')</v>
+        <v>INSERT INTO [dbo].[food] ([name] ,[description] ,[price] ,[price_promo] ,[thumb] ,[img] ,[unit] ,[percent_promo] ,[rating] ,[sold] ,[point] ,[type] ,[status] ,[username] ,[modified]) VALUES ('Tomatoe' ,'Description Tomatoe' ,58 ,56,' product-17.jpg','product-17.jpg' ,'gam' ,0.4 ,10,8,0.3 ,3,1,'khuong','12/26/2019')</v>
       </c>
     </row>
   </sheetData>
@@ -2852,7 +2862,7 @@
       </c>
       <c r="I2" s="3">
         <f ca="1">NOW()</f>
-        <v>43825.461475578704</v>
+        <v>43825.908281249998</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -2883,7 +2893,7 @@
       </c>
       <c r="I3" s="3">
         <f t="shared" ref="I3:I5" ca="1" si="1">NOW()</f>
-        <v>43825.461475578704</v>
+        <v>43825.908281249998</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -2914,7 +2924,7 @@
       </c>
       <c r="I4" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>43825.461475578704</v>
+        <v>43825.908281249998</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -2945,7 +2955,7 @@
       </c>
       <c r="I5" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>43825.461475578704</v>
+        <v>43825.908281249998</v>
       </c>
     </row>
   </sheetData>
@@ -3018,7 +3028,7 @@
       </c>
       <c r="E2">
         <f ca="1">RANDBETWEEN(1,4)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F2" t="str">
         <f t="shared" ref="F2:F31" si="0">"image_1 ("&amp;A2&amp;").jpg"</f>
@@ -3032,15 +3042,15 @@
       </c>
       <c r="I2" s="3">
         <f ca="1">NOW()</f>
-        <v>43825.461475578704</v>
+        <v>43825.908281249998</v>
       </c>
       <c r="J2" s="3">
         <f ca="1">NOW()</f>
-        <v>43825.461475578704</v>
+        <v>43825.908281249998</v>
       </c>
       <c r="L2" t="str">
         <f ca="1">"UPDATE [dbo].[post] SET [type] = '"&amp;E2&amp;"' WHERE post_id="&amp;A2</f>
-        <v>UPDATE [dbo].[post] SET [type] = '1' WHERE post_id=1</v>
+        <v>UPDATE [dbo].[post] SET [type] = '4' WHERE post_id=1</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -3058,7 +3068,7 @@
       </c>
       <c r="E3">
         <f t="shared" ref="E3:E31" ca="1" si="1">RANDBETWEEN(1,4)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F3" t="str">
         <f t="shared" si="0"/>
@@ -3072,15 +3082,15 @@
       </c>
       <c r="I3" s="3">
         <f t="shared" ref="I3:J31" ca="1" si="2">NOW()</f>
-        <v>43825.461475578704</v>
+        <v>43825.908281249998</v>
       </c>
       <c r="J3" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.461475578704</v>
+        <v>43825.908281249998</v>
       </c>
       <c r="L3" t="str">
         <f t="shared" ref="L3:L31" ca="1" si="3">"UPDATE [dbo].[post] SET [type] = '"&amp;E3&amp;"' WHERE post_id="&amp;A3</f>
-        <v>UPDATE [dbo].[post] SET [type] = '3' WHERE post_id=2</v>
+        <v>UPDATE [dbo].[post] SET [type] = '2' WHERE post_id=2</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -3112,11 +3122,11 @@
       </c>
       <c r="I4" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.461475578704</v>
+        <v>43825.908281249998</v>
       </c>
       <c r="J4" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.461475578704</v>
+        <v>43825.908281249998</v>
       </c>
       <c r="L4" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -3138,7 +3148,7 @@
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F5" t="str">
         <f t="shared" si="0"/>
@@ -3152,15 +3162,15 @@
       </c>
       <c r="I5" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.461475578704</v>
+        <v>43825.908281249998</v>
       </c>
       <c r="J5" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.461475578704</v>
+        <v>43825.908281249998</v>
       </c>
       <c r="L5" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>UPDATE [dbo].[post] SET [type] = '2' WHERE post_id=4</v>
+        <v>UPDATE [dbo].[post] SET [type] = '1' WHERE post_id=4</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -3178,7 +3188,7 @@
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F6" t="str">
         <f t="shared" si="0"/>
@@ -3192,15 +3202,15 @@
       </c>
       <c r="I6" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.461475578704</v>
+        <v>43825.908281249998</v>
       </c>
       <c r="J6" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.461475578704</v>
+        <v>43825.908281249998</v>
       </c>
       <c r="L6" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>UPDATE [dbo].[post] SET [type] = '1' WHERE post_id=5</v>
+        <v>UPDATE [dbo].[post] SET [type] = '3' WHERE post_id=5</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -3232,11 +3242,11 @@
       </c>
       <c r="I7" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.461475578704</v>
+        <v>43825.908281249998</v>
       </c>
       <c r="J7" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.461475578704</v>
+        <v>43825.908281249998</v>
       </c>
       <c r="L7" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -3258,7 +3268,7 @@
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F8" t="str">
         <f t="shared" si="0"/>
@@ -3272,15 +3282,15 @@
       </c>
       <c r="I8" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.461475578704</v>
+        <v>43825.908281249998</v>
       </c>
       <c r="J8" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.461475578704</v>
+        <v>43825.908281249998</v>
       </c>
       <c r="L8" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>UPDATE [dbo].[post] SET [type] = '2' WHERE post_id=7</v>
+        <v>UPDATE [dbo].[post] SET [type] = '3' WHERE post_id=7</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -3298,7 +3308,7 @@
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F9" t="str">
         <f t="shared" si="0"/>
@@ -3312,15 +3322,15 @@
       </c>
       <c r="I9" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.461475578704</v>
+        <v>43825.908281249998</v>
       </c>
       <c r="J9" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.461475578704</v>
+        <v>43825.908281249998</v>
       </c>
       <c r="L9" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>UPDATE [dbo].[post] SET [type] = '2' WHERE post_id=8</v>
+        <v>UPDATE [dbo].[post] SET [type] = '1' WHERE post_id=8</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -3338,7 +3348,7 @@
       </c>
       <c r="E10">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F10" t="str">
         <f t="shared" si="0"/>
@@ -3352,15 +3362,15 @@
       </c>
       <c r="I10" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.461475578704</v>
+        <v>43825.908281249998</v>
       </c>
       <c r="J10" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.461475578704</v>
+        <v>43825.908281249998</v>
       </c>
       <c r="L10" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>UPDATE [dbo].[post] SET [type] = '1' WHERE post_id=9</v>
+        <v>UPDATE [dbo].[post] SET [type] = '4' WHERE post_id=9</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -3378,7 +3388,7 @@
       </c>
       <c r="E11">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F11" t="str">
         <f t="shared" si="0"/>
@@ -3392,15 +3402,15 @@
       </c>
       <c r="I11" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.461475578704</v>
+        <v>43825.908281249998</v>
       </c>
       <c r="J11" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.461475578704</v>
+        <v>43825.908281249998</v>
       </c>
       <c r="L11" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>UPDATE [dbo].[post] SET [type] = '1' WHERE post_id=10</v>
+        <v>UPDATE [dbo].[post] SET [type] = '3' WHERE post_id=10</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -3418,7 +3428,7 @@
       </c>
       <c r="E12">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F12" t="str">
         <f t="shared" si="0"/>
@@ -3432,15 +3442,15 @@
       </c>
       <c r="I12" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.461475578704</v>
+        <v>43825.908281249998</v>
       </c>
       <c r="J12" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.461475578704</v>
+        <v>43825.908281249998</v>
       </c>
       <c r="L12" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>UPDATE [dbo].[post] SET [type] = '4' WHERE post_id=11</v>
+        <v>UPDATE [dbo].[post] SET [type] = '1' WHERE post_id=11</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -3458,7 +3468,7 @@
       </c>
       <c r="E13">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F13" t="str">
         <f t="shared" si="0"/>
@@ -3472,15 +3482,15 @@
       </c>
       <c r="I13" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.461475578704</v>
+        <v>43825.908281249998</v>
       </c>
       <c r="J13" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.461475578704</v>
+        <v>43825.908281249998</v>
       </c>
       <c r="L13" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>UPDATE [dbo].[post] SET [type] = '2' WHERE post_id=12</v>
+        <v>UPDATE [dbo].[post] SET [type] = '1' WHERE post_id=12</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -3512,11 +3522,11 @@
       </c>
       <c r="I14" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.461475578704</v>
+        <v>43825.908281249998</v>
       </c>
       <c r="J14" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.461475578704</v>
+        <v>43825.908281249998</v>
       </c>
       <c r="L14" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -3538,7 +3548,7 @@
       </c>
       <c r="E15">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F15" t="str">
         <f t="shared" si="0"/>
@@ -3552,15 +3562,15 @@
       </c>
       <c r="I15" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.461475578704</v>
+        <v>43825.908281249998</v>
       </c>
       <c r="J15" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.461475578704</v>
+        <v>43825.908281249998</v>
       </c>
       <c r="L15" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>UPDATE [dbo].[post] SET [type] = '2' WHERE post_id=14</v>
+        <v>UPDATE [dbo].[post] SET [type] = '1' WHERE post_id=14</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -3578,7 +3588,7 @@
       </c>
       <c r="E16">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F16" t="str">
         <f t="shared" si="0"/>
@@ -3592,15 +3602,15 @@
       </c>
       <c r="I16" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.461475578704</v>
+        <v>43825.908281249998</v>
       </c>
       <c r="J16" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.461475578704</v>
+        <v>43825.908281249998</v>
       </c>
       <c r="L16" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>UPDATE [dbo].[post] SET [type] = '3' WHERE post_id=15</v>
+        <v>UPDATE [dbo].[post] SET [type] = '4' WHERE post_id=15</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -3618,7 +3628,7 @@
       </c>
       <c r="E17">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F17" t="str">
         <f t="shared" si="0"/>
@@ -3632,15 +3642,15 @@
       </c>
       <c r="I17" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.461475578704</v>
+        <v>43825.908281249998</v>
       </c>
       <c r="J17" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.461475578704</v>
+        <v>43825.908281249998</v>
       </c>
       <c r="L17" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>UPDATE [dbo].[post] SET [type] = '2' WHERE post_id=16</v>
+        <v>UPDATE [dbo].[post] SET [type] = '3' WHERE post_id=16</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -3658,7 +3668,7 @@
       </c>
       <c r="E18">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F18" t="str">
         <f t="shared" si="0"/>
@@ -3672,15 +3682,15 @@
       </c>
       <c r="I18" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.461475578704</v>
+        <v>43825.908281249998</v>
       </c>
       <c r="J18" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.461475578704</v>
+        <v>43825.908281249998</v>
       </c>
       <c r="L18" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>UPDATE [dbo].[post] SET [type] = '1' WHERE post_id=17</v>
+        <v>UPDATE [dbo].[post] SET [type] = '3' WHERE post_id=17</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
@@ -3698,7 +3708,7 @@
       </c>
       <c r="E19">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F19" t="str">
         <f t="shared" si="0"/>
@@ -3712,15 +3722,15 @@
       </c>
       <c r="I19" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.461475578704</v>
+        <v>43825.908281249998</v>
       </c>
       <c r="J19" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.461475578704</v>
+        <v>43825.908281249998</v>
       </c>
       <c r="L19" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>UPDATE [dbo].[post] SET [type] = '4' WHERE post_id=18</v>
+        <v>UPDATE [dbo].[post] SET [type] = '2' WHERE post_id=18</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -3752,11 +3762,11 @@
       </c>
       <c r="I20" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.461475578704</v>
+        <v>43825.908281249998</v>
       </c>
       <c r="J20" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.461475578704</v>
+        <v>43825.908281249998</v>
       </c>
       <c r="L20" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -3778,7 +3788,7 @@
       </c>
       <c r="E21">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F21" t="str">
         <f t="shared" si="0"/>
@@ -3792,15 +3802,15 @@
       </c>
       <c r="I21" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.461475578704</v>
+        <v>43825.908281249998</v>
       </c>
       <c r="J21" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.461475578704</v>
+        <v>43825.908281249998</v>
       </c>
       <c r="L21" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>UPDATE [dbo].[post] SET [type] = '1' WHERE post_id=20</v>
+        <v>UPDATE [dbo].[post] SET [type] = '2' WHERE post_id=20</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
@@ -3818,7 +3828,7 @@
       </c>
       <c r="E22">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F22" t="str">
         <f t="shared" si="0"/>
@@ -3832,15 +3842,15 @@
       </c>
       <c r="I22" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.461475578704</v>
+        <v>43825.908281249998</v>
       </c>
       <c r="J22" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.461475578704</v>
+        <v>43825.908281249998</v>
       </c>
       <c r="L22" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>UPDATE [dbo].[post] SET [type] = '3' WHERE post_id=21</v>
+        <v>UPDATE [dbo].[post] SET [type] = '4' WHERE post_id=21</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
@@ -3858,7 +3868,7 @@
       </c>
       <c r="E23">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F23" t="str">
         <f t="shared" si="0"/>
@@ -3872,15 +3882,15 @@
       </c>
       <c r="I23" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.461475578704</v>
+        <v>43825.908281249998</v>
       </c>
       <c r="J23" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.461475578704</v>
+        <v>43825.908281249998</v>
       </c>
       <c r="L23" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>UPDATE [dbo].[post] SET [type] = '4' WHERE post_id=22</v>
+        <v>UPDATE [dbo].[post] SET [type] = '3' WHERE post_id=22</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
@@ -3898,7 +3908,7 @@
       </c>
       <c r="E24">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F24" t="str">
         <f t="shared" si="0"/>
@@ -3912,15 +3922,15 @@
       </c>
       <c r="I24" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.461475578704</v>
+        <v>43825.908281249998</v>
       </c>
       <c r="J24" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.461475578704</v>
+        <v>43825.908281249998</v>
       </c>
       <c r="L24" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>UPDATE [dbo].[post] SET [type] = '2' WHERE post_id=23</v>
+        <v>UPDATE [dbo].[post] SET [type] = '4' WHERE post_id=23</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
@@ -3938,7 +3948,7 @@
       </c>
       <c r="E25">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F25" t="str">
         <f t="shared" si="0"/>
@@ -3952,15 +3962,15 @@
       </c>
       <c r="I25" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.461475578704</v>
+        <v>43825.908281249998</v>
       </c>
       <c r="J25" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.461475578704</v>
+        <v>43825.908281249998</v>
       </c>
       <c r="L25" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>UPDATE [dbo].[post] SET [type] = '4' WHERE post_id=24</v>
+        <v>UPDATE [dbo].[post] SET [type] = '3' WHERE post_id=24</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
@@ -3978,7 +3988,7 @@
       </c>
       <c r="E26">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F26" t="str">
         <f t="shared" si="0"/>
@@ -3992,15 +4002,15 @@
       </c>
       <c r="I26" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.461475578704</v>
+        <v>43825.908281249998</v>
       </c>
       <c r="J26" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.461475578704</v>
+        <v>43825.908281249998</v>
       </c>
       <c r="L26" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>UPDATE [dbo].[post] SET [type] = '2' WHERE post_id=25</v>
+        <v>UPDATE [dbo].[post] SET [type] = '1' WHERE post_id=25</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
@@ -4018,7 +4028,7 @@
       </c>
       <c r="E27">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F27" t="str">
         <f t="shared" si="0"/>
@@ -4032,15 +4042,15 @@
       </c>
       <c r="I27" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.461475578704</v>
+        <v>43825.908281249998</v>
       </c>
       <c r="J27" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.461475578704</v>
+        <v>43825.908281249998</v>
       </c>
       <c r="L27" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>UPDATE [dbo].[post] SET [type] = '2' WHERE post_id=26</v>
+        <v>UPDATE [dbo].[post] SET [type] = '4' WHERE post_id=26</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
@@ -4058,7 +4068,7 @@
       </c>
       <c r="E28">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F28" t="str">
         <f t="shared" si="0"/>
@@ -4072,15 +4082,15 @@
       </c>
       <c r="I28" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.461475578704</v>
+        <v>43825.908281249998</v>
       </c>
       <c r="J28" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.461475578704</v>
+        <v>43825.908281249998</v>
       </c>
       <c r="L28" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>UPDATE [dbo].[post] SET [type] = '3' WHERE post_id=27</v>
+        <v>UPDATE [dbo].[post] SET [type] = '1' WHERE post_id=27</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
@@ -4098,7 +4108,7 @@
       </c>
       <c r="E29">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F29" t="str">
         <f t="shared" si="0"/>
@@ -4112,15 +4122,15 @@
       </c>
       <c r="I29" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.461475578704</v>
+        <v>43825.908281249998</v>
       </c>
       <c r="J29" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.461475578704</v>
+        <v>43825.908281249998</v>
       </c>
       <c r="L29" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>UPDATE [dbo].[post] SET [type] = '4' WHERE post_id=28</v>
+        <v>UPDATE [dbo].[post] SET [type] = '1' WHERE post_id=28</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
@@ -4138,7 +4148,7 @@
       </c>
       <c r="E30">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F30" t="str">
         <f t="shared" si="0"/>
@@ -4152,15 +4162,15 @@
       </c>
       <c r="I30" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.461475578704</v>
+        <v>43825.908281249998</v>
       </c>
       <c r="J30" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.461475578704</v>
+        <v>43825.908281249998</v>
       </c>
       <c r="L30" t="str">
         <f t="shared" ca="1" si="3"/>
-        <v>UPDATE [dbo].[post] SET [type] = '4' WHERE post_id=29</v>
+        <v>UPDATE [dbo].[post] SET [type] = '2' WHERE post_id=29</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
@@ -4192,11 +4202,11 @@
       </c>
       <c r="I31" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.461475578704</v>
+        <v>43825.908281249998</v>
       </c>
       <c r="J31" s="3">
         <f t="shared" ca="1" si="2"/>
-        <v>43825.461475578704</v>
+        <v>43825.908281249998</v>
       </c>
       <c r="L31" t="str">
         <f t="shared" ca="1" si="3"/>
@@ -4235,7 +4245,7 @@
       </c>
       <c r="B2">
         <f ca="1">RANDBETWEEN(1,5)</f>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C2" t="str">
         <f>"des "&amp;A2</f>
@@ -4258,7 +4268,7 @@
       </c>
       <c r="B3">
         <f t="shared" ref="B3:B18" ca="1" si="0">RANDBETWEEN(1,5)</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C3" t="str">
         <f t="shared" ref="C3:C18" si="1">"des "&amp;A3</f>
@@ -4278,7 +4288,7 @@
       </c>
       <c r="B4">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C4" t="str">
         <f t="shared" si="1"/>
@@ -4298,7 +4308,7 @@
       </c>
       <c r="B5">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C5" t="str">
         <f t="shared" si="1"/>
@@ -4369,7 +4379,7 @@
       </c>
       <c r="B9">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C9" t="str">
         <f t="shared" si="1"/>
@@ -4403,7 +4413,7 @@
       </c>
       <c r="B11">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C11" t="str">
         <f t="shared" si="1"/>
@@ -4420,7 +4430,7 @@
       </c>
       <c r="B12">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C12" t="str">
         <f t="shared" si="1"/>
@@ -4437,7 +4447,7 @@
       </c>
       <c r="B13">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C13" t="str">
         <f t="shared" si="1"/>
@@ -4454,7 +4464,7 @@
       </c>
       <c r="B14">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C14" t="str">
         <f t="shared" si="1"/>
@@ -4488,7 +4498,7 @@
       </c>
       <c r="B16">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C16" t="str">
         <f t="shared" si="1"/>
@@ -4505,7 +4515,7 @@
       </c>
       <c r="B17">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C17" t="str">
         <f t="shared" si="1"/>
@@ -4522,7 +4532,7 @@
       </c>
       <c r="B18">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C18" t="str">
         <f t="shared" si="1"/>
@@ -4542,8 +4552,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4640,22 +4650,22 @@
       </c>
       <c r="H3">
         <f ca="1">RANDBETWEEN(1,5)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I3">
         <f ca="1">RANDBETWEEN(1,5)</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J3">
         <f ca="1">SUM(H3,I3)</f>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="K3">
         <v>1</v>
       </c>
       <c r="L3" s="3">
         <f ca="1">NOW()</f>
-        <v>43825.461475578704</v>
+        <v>43825.908281249998</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
@@ -4689,18 +4699,18 @@
       </c>
       <c r="I4">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J4">
         <f t="shared" ref="J4:J18" ca="1" si="4">SUM(H4,I4)</f>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="K4">
         <v>1</v>
       </c>
       <c r="L4" s="3">
         <f t="shared" ref="L4:L18" ca="1" si="5">NOW()</f>
-        <v>43825.461475578704</v>
+        <v>43825.908281249998</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
@@ -4734,18 +4744,18 @@
       </c>
       <c r="I5">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J5">
         <f t="shared" ca="1" si="4"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K5">
         <v>1</v>
       </c>
       <c r="L5" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>43825.461475578704</v>
+        <v>43825.908281249998</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
@@ -4775,7 +4785,7 @@
       </c>
       <c r="H6">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I6">
         <f t="shared" ca="1" si="3"/>
@@ -4783,14 +4793,14 @@
       </c>
       <c r="J6">
         <f t="shared" ca="1" si="4"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K6">
         <v>1</v>
       </c>
       <c r="L6" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>43825.461475578704</v>
+        <v>43825.908281249998</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
@@ -4820,22 +4830,22 @@
       </c>
       <c r="H7">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I7">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J7">
         <f t="shared" ca="1" si="4"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="K7">
         <v>1</v>
       </c>
       <c r="L7" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>43825.461475578704</v>
+        <v>43825.908281249998</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
@@ -4865,7 +4875,7 @@
       </c>
       <c r="H8">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I8">
         <f t="shared" ca="1" si="3"/>
@@ -4873,14 +4883,14 @@
       </c>
       <c r="J8">
         <f t="shared" ca="1" si="4"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="K8">
         <v>1</v>
       </c>
       <c r="L8" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>43825.461475578704</v>
+        <v>43825.908281249998</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
@@ -4910,22 +4920,22 @@
       </c>
       <c r="H9">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I9">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J9">
         <f t="shared" ca="1" si="4"/>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="K9">
         <v>1</v>
       </c>
       <c r="L9" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>43825.461475578704</v>
+        <v>43825.908281249998</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
@@ -4955,22 +4965,22 @@
       </c>
       <c r="H10">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I10">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J10">
         <f t="shared" ca="1" si="4"/>
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="K10">
         <v>1</v>
       </c>
       <c r="L10" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>43825.461475578704</v>
+        <v>43825.908281249998</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
@@ -5000,22 +5010,22 @@
       </c>
       <c r="H11">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I11">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J11">
         <f t="shared" ca="1" si="4"/>
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="K11">
         <v>1</v>
       </c>
       <c r="L11" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>43825.461475578704</v>
+        <v>43825.908281249998</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
@@ -5045,22 +5055,22 @@
       </c>
       <c r="H12">
         <f t="shared" ca="1" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="I12">
+        <f t="shared" ca="1" si="3"/>
         <v>5</v>
-      </c>
-      <c r="I12">
-        <f t="shared" ca="1" si="3"/>
-        <v>2</v>
       </c>
       <c r="J12">
         <f t="shared" ca="1" si="4"/>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="K12">
         <v>1</v>
       </c>
       <c r="L12" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>43825.461475578704</v>
+        <v>43825.908281249998</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
@@ -5090,22 +5100,22 @@
       </c>
       <c r="H13">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I13">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J13">
         <f t="shared" ca="1" si="4"/>
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="K13">
         <v>1</v>
       </c>
       <c r="L13" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>43825.461475578704</v>
+        <v>43825.908281249998</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
@@ -5135,22 +5145,22 @@
       </c>
       <c r="H14">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I14">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J14">
         <f t="shared" ca="1" si="4"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="K14">
         <v>1</v>
       </c>
       <c r="L14" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>43825.461475578704</v>
+        <v>43825.908281249998</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
@@ -5180,7 +5190,7 @@
       </c>
       <c r="H15">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I15">
         <f t="shared" ca="1" si="3"/>
@@ -5188,14 +5198,14 @@
       </c>
       <c r="J15">
         <f t="shared" ca="1" si="4"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="K15">
         <v>1</v>
       </c>
       <c r="L15" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>43825.461475578704</v>
+        <v>43825.908281249998</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
@@ -5225,22 +5235,22 @@
       </c>
       <c r="H16">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I16">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J16">
         <f t="shared" ca="1" si="4"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="K16">
         <v>1</v>
       </c>
       <c r="L16" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>43825.461475578704</v>
+        <v>43825.908281249998</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -5274,18 +5284,18 @@
       </c>
       <c r="I17">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J17">
         <f t="shared" ca="1" si="4"/>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="K17">
         <v>1</v>
       </c>
       <c r="L17" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>43825.461475578704</v>
+        <v>43825.908281249998</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -5330,7 +5340,7 @@
       </c>
       <c r="L18" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>43825.461475578704</v>
+        <v>43825.908281249998</v>
       </c>
     </row>
   </sheetData>
@@ -5351,7 +5361,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
@@ -5438,7 +5448,7 @@
       </c>
       <c r="F3">
         <f ca="1">RANDBETWEEN(1000,8000)</f>
-        <v>7960</v>
+        <v>3096</v>
       </c>
       <c r="G3">
         <v>1</v>
@@ -5448,11 +5458,11 @@
       </c>
       <c r="I3" s="3">
         <f ca="1">NOW()</f>
-        <v>43825.461475578704</v>
+        <v>43825.908281249998</v>
       </c>
       <c r="J3" s="3">
         <f ca="1">NOW()</f>
-        <v>43825.461475578704</v>
+        <v>43825.908281249998</v>
       </c>
       <c r="K3" t="s">
         <v>182</v>
@@ -5474,11 +5484,11 @@
       </c>
       <c r="E4">
         <f t="shared" ref="E4:E16" ca="1" si="1">RANDBETWEEN(0,5)</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F4">
         <f t="shared" ref="F4:F16" ca="1" si="2">RANDBETWEEN(1000,8000)</f>
-        <v>6822</v>
+        <v>6173</v>
       </c>
       <c r="G4">
         <v>1</v>
@@ -5488,11 +5498,11 @@
       </c>
       <c r="I4" s="3">
         <f t="shared" ref="I4:J16" ca="1" si="3">NOW()</f>
-        <v>43825.461475578704</v>
+        <v>43825.908281249998</v>
       </c>
       <c r="J4" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>43825.461475578704</v>
+        <v>43825.908281249998</v>
       </c>
       <c r="K4" t="s">
         <v>182</v>
@@ -5514,11 +5524,11 @@
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F5">
         <f t="shared" ca="1" si="2"/>
-        <v>4730</v>
+        <v>3679</v>
       </c>
       <c r="G5">
         <v>1</v>
@@ -5528,11 +5538,11 @@
       </c>
       <c r="I5" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>43825.461475578704</v>
+        <v>43825.908281249998</v>
       </c>
       <c r="J5" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>43825.461475578704</v>
+        <v>43825.908281249998</v>
       </c>
       <c r="K5" t="s">
         <v>182</v>
@@ -5558,7 +5568,7 @@
       </c>
       <c r="F6">
         <f t="shared" ca="1" si="2"/>
-        <v>2951</v>
+        <v>5693</v>
       </c>
       <c r="G6">
         <v>1</v>
@@ -5568,11 +5578,11 @@
       </c>
       <c r="I6" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>43825.461475578704</v>
+        <v>43825.908281249998</v>
       </c>
       <c r="J6" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>43825.461475578704</v>
+        <v>43825.908281249998</v>
       </c>
       <c r="K6" t="s">
         <v>182</v>
@@ -5594,11 +5604,11 @@
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F7">
         <f t="shared" ca="1" si="2"/>
-        <v>3307</v>
+        <v>7910</v>
       </c>
       <c r="G7">
         <v>1</v>
@@ -5608,11 +5618,11 @@
       </c>
       <c r="I7" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>43825.461475578704</v>
+        <v>43825.908281249998</v>
       </c>
       <c r="J7" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>43825.461475578704</v>
+        <v>43825.908281249998</v>
       </c>
       <c r="K7" t="s">
         <v>182</v>
@@ -5638,7 +5648,7 @@
       </c>
       <c r="F8">
         <f t="shared" ca="1" si="2"/>
-        <v>3287</v>
+        <v>2729</v>
       </c>
       <c r="G8">
         <v>1</v>
@@ -5648,11 +5658,11 @@
       </c>
       <c r="I8" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>43825.461475578704</v>
+        <v>43825.908281249998</v>
       </c>
       <c r="J8" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>43825.461475578704</v>
+        <v>43825.908281249998</v>
       </c>
       <c r="K8" t="s">
         <v>182</v>
@@ -5674,11 +5684,11 @@
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F9">
         <f t="shared" ca="1" si="2"/>
-        <v>6956</v>
+        <v>2694</v>
       </c>
       <c r="G9">
         <v>1</v>
@@ -5688,11 +5698,11 @@
       </c>
       <c r="I9" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>43825.461475578704</v>
+        <v>43825.908281249998</v>
       </c>
       <c r="J9" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>43825.461475578704</v>
+        <v>43825.908281249998</v>
       </c>
       <c r="K9" t="s">
         <v>182</v>
@@ -5714,11 +5724,11 @@
       </c>
       <c r="E10">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F10">
         <f t="shared" ca="1" si="2"/>
-        <v>1957</v>
+        <v>7269</v>
       </c>
       <c r="G10">
         <v>1</v>
@@ -5728,11 +5738,11 @@
       </c>
       <c r="I10" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>43825.461475578704</v>
+        <v>43825.908281249998</v>
       </c>
       <c r="J10" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>43825.461475578704</v>
+        <v>43825.908281249998</v>
       </c>
       <c r="K10" t="s">
         <v>182</v>
@@ -5754,11 +5764,11 @@
       </c>
       <c r="E11">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F11">
         <f t="shared" ca="1" si="2"/>
-        <v>6169</v>
+        <v>6727</v>
       </c>
       <c r="G11">
         <v>1</v>
@@ -5768,11 +5778,11 @@
       </c>
       <c r="I11" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>43825.461475578704</v>
+        <v>43825.908281249998</v>
       </c>
       <c r="J11" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>43825.461475578704</v>
+        <v>43825.908281249998</v>
       </c>
       <c r="K11" t="s">
         <v>182</v>
@@ -5794,11 +5804,11 @@
       </c>
       <c r="E12">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F12">
         <f t="shared" ca="1" si="2"/>
-        <v>7284</v>
+        <v>5240</v>
       </c>
       <c r="G12">
         <v>1</v>
@@ -5808,11 +5818,11 @@
       </c>
       <c r="I12" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>43825.461475578704</v>
+        <v>43825.908281249998</v>
       </c>
       <c r="J12" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>43825.461475578704</v>
+        <v>43825.908281249998</v>
       </c>
       <c r="K12" t="s">
         <v>182</v>
@@ -5834,11 +5844,11 @@
       </c>
       <c r="E13">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F13">
         <f t="shared" ca="1" si="2"/>
-        <v>5007</v>
+        <v>6862</v>
       </c>
       <c r="G13">
         <v>1</v>
@@ -5848,11 +5858,11 @@
       </c>
       <c r="I13" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>43825.461475578704</v>
+        <v>43825.908281249998</v>
       </c>
       <c r="J13" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>43825.461475578704</v>
+        <v>43825.908281249998</v>
       </c>
       <c r="K13" t="s">
         <v>182</v>
@@ -5874,11 +5884,11 @@
       </c>
       <c r="E14">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F14">
         <f t="shared" ca="1" si="2"/>
-        <v>6670</v>
+        <v>1282</v>
       </c>
       <c r="G14">
         <v>1</v>
@@ -5888,11 +5898,11 @@
       </c>
       <c r="I14" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>43825.461475578704</v>
+        <v>43825.908281249998</v>
       </c>
       <c r="J14" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>43825.461475578704</v>
+        <v>43825.908281249998</v>
       </c>
       <c r="K14" t="s">
         <v>182</v>
@@ -5914,11 +5924,11 @@
       </c>
       <c r="E15">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F15">
         <f t="shared" ca="1" si="2"/>
-        <v>4519</v>
+        <v>5428</v>
       </c>
       <c r="G15">
         <v>1</v>
@@ -5928,11 +5938,11 @@
       </c>
       <c r="I15" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>43825.461475578704</v>
+        <v>43825.908281249998</v>
       </c>
       <c r="J15" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>43825.461475578704</v>
+        <v>43825.908281249998</v>
       </c>
       <c r="K15" t="s">
         <v>182</v>
@@ -5954,11 +5964,11 @@
       </c>
       <c r="E16">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F16">
         <f t="shared" ca="1" si="2"/>
-        <v>3483</v>
+        <v>5680</v>
       </c>
       <c r="G16">
         <v>1</v>
@@ -5968,11 +5978,11 @@
       </c>
       <c r="I16" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>43825.461475578704</v>
+        <v>43825.908281249998</v>
       </c>
       <c r="J16" s="3">
         <f t="shared" ca="1" si="3"/>
-        <v>43825.461475578704</v>
+        <v>43825.908281249998</v>
       </c>
       <c r="K16" t="s">
         <v>182</v>
@@ -5984,4 +5994,179 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M5" sqref="M5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>177</v>
+      </c>
+      <c r="B2" t="s">
+        <v>186</v>
+      </c>
+      <c r="C2" t="s">
+        <v>181</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <f ca="1">RANDBETWEEN(1,3)</f>
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <f ca="1">RANDBETWEEN(1,3)</f>
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <f ca="1">RANDBETWEEN(1,10)</f>
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3">
+        <v>1000</v>
+      </c>
+      <c r="F3">
+        <f ca="1">E3*C3</f>
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <f t="shared" ref="A4:B7" ca="1" si="0">RANDBETWEEN(1,3)</f>
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <f t="shared" ref="C4:C7" ca="1" si="1">RANDBETWEEN(1,10)</f>
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4">
+        <v>1000</v>
+      </c>
+      <c r="F4">
+        <f t="shared" ref="F4:F7" ca="1" si="2">E4*C4</f>
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <f t="shared" ca="1" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="D5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5">
+        <v>1000</v>
+      </c>
+      <c r="F5">
+        <f t="shared" ca="1" si="2"/>
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <f t="shared" ca="1" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="D6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6">
+        <v>1000</v>
+      </c>
+      <c r="F6">
+        <f t="shared" ca="1" si="2"/>
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="C7">
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7">
+        <v>1000</v>
+      </c>
+      <c r="F7">
+        <f t="shared" ca="1" si="2"/>
+        <v>2000</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:M1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>